<commit_message>
Made several updates to BOM, Project Log, and Schematics
</commit_message>
<xml_diff>
--- a/Notes/Chameleon BOM.xlsx
+++ b/Notes/Chameleon BOM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="150" windowWidth="24240" windowHeight="12075"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="82">
   <si>
     <t>Mfg Part #</t>
   </si>
@@ -64,6 +64,207 @@
   </si>
   <si>
     <t>Bill of Materials - Chameleon Drink Coasters</t>
+  </si>
+  <si>
+    <t>NCP1402SN50T1G</t>
+  </si>
+  <si>
+    <t>IC Boost Regulator 5V 0.2A</t>
+  </si>
+  <si>
+    <t>6-TSOP (0.059", 1.50mm Width) 5 leads</t>
+  </si>
+  <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>Also available at Newark, Farnell, Avnet, Verical, etc</t>
+  </si>
+  <si>
+    <t>SRN3015-330M</t>
+  </si>
+  <si>
+    <t>Inductor 33uH</t>
+  </si>
+  <si>
+    <t>3mm x 3mm</t>
+  </si>
+  <si>
+    <t>BAT750TA</t>
+  </si>
+  <si>
+    <t>SOT-23-3</t>
+  </si>
+  <si>
+    <t>Used with Boost Regulator</t>
+  </si>
+  <si>
+    <t>Used with Boost Regulator. Typical Forward Voltage = 290mV @ 250mA</t>
+  </si>
+  <si>
+    <t>Diode Schottky 40V 750mA</t>
+  </si>
+  <si>
+    <t>3.5mm x 2.8mm</t>
+  </si>
+  <si>
+    <t>Output Capacitor used with Boost Regulator</t>
+  </si>
+  <si>
+    <t>Capacitor Tantalum 47uF 10V 20%</t>
+  </si>
+  <si>
+    <t>TCJB476M010R0070</t>
+  </si>
+  <si>
+    <t>Input Capacitor used with Boost Regulator</t>
+  </si>
+  <si>
+    <t>3.2mm x 1.6mm</t>
+  </si>
+  <si>
+    <t>C3216Y5V1A106Z/0.85</t>
+  </si>
+  <si>
+    <t>Capacitor Ceramic 10uF 10V Y5V</t>
+  </si>
+  <si>
+    <t>PCA9685PW,112</t>
+  </si>
+  <si>
+    <t>Future</t>
+  </si>
+  <si>
+    <t>Also available at Digikey and Verical</t>
+  </si>
+  <si>
+    <t>TSSOP-28</t>
+  </si>
+  <si>
+    <t>IC LED Driver RGBA</t>
+  </si>
+  <si>
+    <t>Battery (Li-Poly 500mAh)</t>
+  </si>
+  <si>
+    <t>Nominal Voltage: 3.7V</t>
+  </si>
+  <si>
+    <t>Shenzhen Puchuangyuan Technology Co. Ltd</t>
+  </si>
+  <si>
+    <t>JHY-303450</t>
+  </si>
+  <si>
+    <t>50.5mm x 34.5 mm x 3.2mm</t>
+  </si>
+  <si>
+    <t>Crystal 20 MHZ 8pF</t>
+  </si>
+  <si>
+    <t>NX3225SA-20.000000MHZ</t>
+  </si>
+  <si>
+    <t>1210</t>
+  </si>
+  <si>
+    <t>DigiKey</t>
+  </si>
+  <si>
+    <t>AVR Timing</t>
+  </si>
+  <si>
+    <t>CC0805DRNPO9BN8R0</t>
+  </si>
+  <si>
+    <t>0805</t>
+  </si>
+  <si>
+    <t>Capacitor Ceramic 8pF 50V</t>
+  </si>
+  <si>
+    <t>Used for Crystal loading</t>
+  </si>
+  <si>
+    <t>PLCC-6 RGB LED</t>
+  </si>
+  <si>
+    <t>5mm x 5mm</t>
+  </si>
+  <si>
+    <t>LED Lighting</t>
+  </si>
+  <si>
+    <t>Resistor 1.0kΩ 1/4W 5%</t>
+  </si>
+  <si>
+    <t>RC1206JR-071KL</t>
+  </si>
+  <si>
+    <t>Used for QMatrix X&amp;Y line resistors</t>
+  </si>
+  <si>
+    <t>Resistor 470K OHM 1/4W 5%</t>
+  </si>
+  <si>
+    <t>RC1206JR-07470KL</t>
+  </si>
+  <si>
+    <t>1206</t>
+  </si>
+  <si>
+    <t>Used for QMatrix RY line resistors</t>
+  </si>
+  <si>
+    <t>Capacitor Ceramic 4.7nF 50V 10%</t>
+  </si>
+  <si>
+    <t>CC1206KRX7R9BB472</t>
+  </si>
+  <si>
+    <t>Used for QMatrix RY line capacitors</t>
+  </si>
+  <si>
+    <t>Switch Tactile SPST-NO 0.05A 15V</t>
+  </si>
+  <si>
+    <t>TL3315NF160Q</t>
+  </si>
+  <si>
+    <t>4.5mm x 4.5mm</t>
+  </si>
+  <si>
+    <t>AVR Reset</t>
+  </si>
+  <si>
+    <t>Inductor 33uH 10%</t>
+  </si>
+  <si>
+    <t>LB3218T330K</t>
+  </si>
+  <si>
+    <t>1207</t>
+  </si>
+  <si>
+    <t>AVR Analog Reference Filtering</t>
+  </si>
+  <si>
+    <t>LED Red Diffused</t>
+  </si>
+  <si>
+    <t>LH N974-KN-1</t>
+  </si>
+  <si>
+    <t>Power Indicator</t>
+  </si>
+  <si>
+    <t>Capacitor Ceramic 0.1uF 50V 10%</t>
+  </si>
+  <si>
+    <t>GRM319R71H104KA01D</t>
+  </si>
+  <si>
+    <t>Used for Power Input/Output filtering and Decoupling</t>
   </si>
 </sst>
 </file>
@@ -215,7 +416,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -289,12 +490,39 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="15">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Lucida Sans Unicode"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -458,25 +686,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="9"/>
-        <color theme="1"/>
-        <name val="Lucida Sans Unicode"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
         <color theme="1" tint="0.14996795556505021"/>
         <name val="Lucida Sans Unicode"/>
         <scheme val="none"/>
@@ -578,19 +787,19 @@
   <tableColumns count="11">
     <tableColumn id="1" name="Description" dataDxfId="10"/>
     <tableColumn id="2" name="Mfg Part #" dataDxfId="9"/>
-    <tableColumn id="3" name="Package" dataDxfId="8"/>
-    <tableColumn id="5" name="Default Supplier" dataDxfId="7"/>
-    <tableColumn id="10" name="Supplier On Hand" dataDxfId="6"/>
-    <tableColumn id="4" name="Qty per board" dataDxfId="5"/>
-    <tableColumn id="6" name="Total Qty Needed" dataDxfId="4">
+    <tableColumn id="3" name="Package" dataDxfId="0"/>
+    <tableColumn id="5" name="Default Supplier" dataDxfId="8"/>
+    <tableColumn id="10" name="Supplier On Hand" dataDxfId="7"/>
+    <tableColumn id="4" name="Qty per board" dataDxfId="6"/>
+    <tableColumn id="6" name="Total Qty Needed" dataDxfId="5">
       <calculatedColumnFormula>SUM(Table4[[#This Row],[Qty per board]]*Goal)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Price per part at Qty" dataDxfId="3"/>
-    <tableColumn id="7" name="Total Price" dataDxfId="2">
+    <tableColumn id="11" name="Price per part at Qty" dataDxfId="4"/>
+    <tableColumn id="7" name="Total Price" dataDxfId="3">
       <calculatedColumnFormula>SUM(H6*G6)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Notes" dataDxfId="1"/>
-    <tableColumn id="9" name="Part References" dataDxfId="0"/>
+    <tableColumn id="8" name="Notes" dataDxfId="2"/>
+    <tableColumn id="9" name="Part References" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="Projects and Stuff" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -886,7 +1095,7 @@
   <dimension ref="A1:K200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -921,7 +1130,7 @@
         <v>4</v>
       </c>
       <c r="K1" s="9">
-        <v>500</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.25">
@@ -958,7 +1167,7 @@
       </c>
       <c r="B4" s="14">
         <f>SUM(I6:I200)</f>
-        <v>0</v>
+        <v>4254.63</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -1005,316 +1214,560 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="15"/>
+    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="17">
+        <v>1335</v>
+      </c>
+      <c r="F6" s="15">
+        <v>1</v>
+      </c>
       <c r="G6" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="H6" s="18"/>
+        <v>1000</v>
+      </c>
+      <c r="H6" s="18">
+        <v>0.33</v>
+      </c>
       <c r="I6" s="24">
         <f>SUM(H6*G6)</f>
-        <v>0</v>
-      </c>
-      <c r="J6" s="19"/>
+        <v>330</v>
+      </c>
+      <c r="J6" s="19" t="s">
+        <v>19</v>
+      </c>
       <c r="K6" s="19"/>
     </row>
     <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="15"/>
+      <c r="A7" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="17">
+        <v>3796</v>
+      </c>
+      <c r="F7" s="15">
+        <v>1</v>
+      </c>
       <c r="G7" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="H7" s="18"/>
+        <v>1000</v>
+      </c>
+      <c r="H7" s="18">
+        <v>0.16</v>
+      </c>
       <c r="I7" s="24">
         <f>SUM(H7*G7)</f>
-        <v>0</v>
-      </c>
-      <c r="J7" s="19"/>
+        <v>160</v>
+      </c>
+      <c r="J7" s="19" t="s">
+        <v>25</v>
+      </c>
       <c r="K7" s="19"/>
     </row>
-    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="15"/>
+    <row r="8" spans="1:11" ht="27" x14ac:dyDescent="0.25">
+      <c r="A8" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="17">
+        <v>22159</v>
+      </c>
+      <c r="F8" s="15">
+        <v>1</v>
+      </c>
       <c r="G8" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="H8" s="18"/>
+        <v>1000</v>
+      </c>
+      <c r="H8" s="18">
+        <v>9.4759999999999997E-2</v>
+      </c>
       <c r="I8" s="24">
         <f>SUM(H8*G8)</f>
-        <v>0</v>
-      </c>
-      <c r="J8" s="19"/>
+        <v>94.759999999999991</v>
+      </c>
+      <c r="J8" s="19" t="s">
+        <v>26</v>
+      </c>
       <c r="K8" s="19"/>
     </row>
     <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="15"/>
+      <c r="A9" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="17">
+        <v>39210</v>
+      </c>
+      <c r="F9" s="15">
+        <v>1</v>
+      </c>
       <c r="G9" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="18"/>
+        <v>1000</v>
+      </c>
+      <c r="H9" s="18">
+        <v>0.45100000000000001</v>
+      </c>
       <c r="I9" s="24">
         <f t="shared" ref="I9:I69" si="0">SUM(H9*G9)</f>
-        <v>0</v>
-      </c>
-      <c r="J9" s="19"/>
+        <v>451</v>
+      </c>
+      <c r="J9" s="19" t="s">
+        <v>29</v>
+      </c>
       <c r="K9" s="19"/>
     </row>
     <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="15"/>
+      <c r="A10" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="17">
+        <v>116496</v>
+      </c>
+      <c r="F10" s="15">
+        <v>1</v>
+      </c>
       <c r="G10" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="H10" s="18"/>
+        <v>1000</v>
+      </c>
+      <c r="H10" s="18">
+        <v>3.8249999999999999E-2</v>
+      </c>
       <c r="I10" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J10" s="19"/>
+        <v>38.25</v>
+      </c>
+      <c r="J10" s="19" t="s">
+        <v>32</v>
+      </c>
       <c r="K10" s="19"/>
     </row>
     <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="15"/>
+      <c r="A11" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="17">
+        <v>1375</v>
+      </c>
+      <c r="F11" s="15">
+        <v>1</v>
+      </c>
       <c r="G11" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="H11" s="18"/>
+        <v>1000</v>
+      </c>
+      <c r="H11" s="18">
+        <v>0.95</v>
+      </c>
       <c r="I11" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J11" s="19"/>
+        <v>950</v>
+      </c>
+      <c r="J11" s="19" t="s">
+        <v>38</v>
+      </c>
       <c r="K11" s="19"/>
     </row>
-    <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="19"/>
+    <row r="12" spans="1:11" ht="54" x14ac:dyDescent="0.25">
+      <c r="A12" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>43</v>
+      </c>
       <c r="E12" s="17"/>
-      <c r="F12" s="15"/>
+      <c r="F12" s="15">
+        <v>1</v>
+      </c>
       <c r="G12" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="H12" s="18"/>
+        <v>1000</v>
+      </c>
+      <c r="H12" s="18">
+        <v>1.66</v>
+      </c>
       <c r="I12" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="19"/>
+        <v>1660</v>
+      </c>
+      <c r="J12" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="K12" s="19"/>
     </row>
     <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="15"/>
+      <c r="A13" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="17">
+        <v>9900</v>
+      </c>
+      <c r="F13" s="15">
+        <v>1</v>
+      </c>
       <c r="G13" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="H13" s="18"/>
+        <v>1000</v>
+      </c>
+      <c r="H13" s="18">
+        <v>0.53761999999999999</v>
+      </c>
       <c r="I13" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J13" s="19"/>
+        <v>537.62</v>
+      </c>
+      <c r="J13" s="19" t="s">
+        <v>50</v>
+      </c>
       <c r="K13" s="19"/>
     </row>
     <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="15"/>
+      <c r="A14" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="17">
+        <v>7417</v>
+      </c>
+      <c r="F14" s="15">
+        <v>2</v>
+      </c>
       <c r="G14" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="H14" s="18"/>
+        <v>2000</v>
+      </c>
+      <c r="H14" s="18">
+        <v>1.6500000000000001E-2</v>
+      </c>
       <c r="I14" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J14" s="19"/>
+        <v>33</v>
+      </c>
+      <c r="J14" s="19" t="s">
+        <v>54</v>
+      </c>
       <c r="K14" s="19"/>
     </row>
     <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="23"/>
+      <c r="A15" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="20"/>
+      <c r="C15" s="23" t="s">
+        <v>56</v>
+      </c>
       <c r="D15" s="19"/>
       <c r="E15" s="17"/>
-      <c r="F15" s="15"/>
+      <c r="F15" s="15">
+        <v>5</v>
+      </c>
       <c r="G15" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="H15" s="18"/>
       <c r="I15" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J15" s="19"/>
+      <c r="J15" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="K15" s="19"/>
     </row>
     <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="15"/>
+      <c r="A16" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="23">
+        <v>1206</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="17">
+        <v>195000</v>
+      </c>
+      <c r="F16" s="15">
+        <v>1</v>
+      </c>
       <c r="G16" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="H16" s="18"/>
       <c r="I16" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J16" s="19"/>
+      <c r="J16" s="19" t="s">
+        <v>60</v>
+      </c>
       <c r="K16" s="19"/>
     </row>
     <row r="17" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="15"/>
+      <c r="A17" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="17">
+        <v>53903</v>
+      </c>
+      <c r="F17" s="15">
+        <v>1</v>
+      </c>
       <c r="G17" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="H17" s="18"/>
       <c r="I17" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J17" s="19"/>
+      <c r="J17" s="19" t="s">
+        <v>64</v>
+      </c>
       <c r="K17" s="19"/>
     </row>
     <row r="18" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="15"/>
+      <c r="A18" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="23">
+        <v>1206</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="17">
+        <v>56717</v>
+      </c>
+      <c r="F18" s="15">
+        <v>1</v>
+      </c>
       <c r="G18" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="H18" s="18"/>
       <c r="I18" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J18" s="19"/>
+      <c r="J18" s="19" t="s">
+        <v>67</v>
+      </c>
       <c r="K18" s="19"/>
     </row>
     <row r="19" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="15"/>
+      <c r="A19" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="17">
+        <v>88036</v>
+      </c>
+      <c r="F19" s="15">
+        <v>1</v>
+      </c>
       <c r="G19" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="H19" s="18"/>
       <c r="I19" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J19" s="19"/>
+      <c r="J19" s="19" t="s">
+        <v>71</v>
+      </c>
       <c r="K19" s="19"/>
     </row>
     <row r="20" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="15"/>
+      <c r="A20" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" s="17">
+        <v>2440</v>
+      </c>
+      <c r="F20" s="15">
+        <v>1</v>
+      </c>
       <c r="G20" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="H20" s="18"/>
       <c r="I20" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J20" s="19"/>
+      <c r="J20" s="19" t="s">
+        <v>75</v>
+      </c>
       <c r="K20" s="19"/>
     </row>
     <row r="21" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="21"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="15"/>
+      <c r="A21" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="17">
+        <v>586403</v>
+      </c>
+      <c r="F21" s="15">
+        <v>1</v>
+      </c>
       <c r="G21" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="H21" s="18"/>
       <c r="I21" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J21" s="19"/>
+      <c r="J21" s="19" t="s">
+        <v>78</v>
+      </c>
       <c r="K21" s="19"/>
     </row>
-    <row r="22" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="21"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="17"/>
+    <row r="22" spans="1:11" ht="27" x14ac:dyDescent="0.25">
+      <c r="A22" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" s="23">
+        <v>1206</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="17">
+        <v>310439</v>
+      </c>
       <c r="F22" s="15"/>
       <c r="G22" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
@@ -1325,13 +1778,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J22" s="19"/>
+      <c r="J22" s="19" t="s">
+        <v>81</v>
+      </c>
       <c r="K22" s="19"/>
     </row>
     <row r="23" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="21"/>
       <c r="B23" s="20"/>
-      <c r="C23" s="23"/>
+      <c r="C23" s="29"/>
       <c r="D23" s="19"/>
       <c r="E23" s="17"/>
       <c r="F23" s="15"/>
@@ -1350,7 +1805,7 @@
     <row r="24" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="21"/>
       <c r="B24" s="20"/>
-      <c r="C24" s="23"/>
+      <c r="C24" s="29"/>
       <c r="D24" s="19"/>
       <c r="E24" s="17"/>
       <c r="F24" s="15"/>
@@ -1369,7 +1824,7 @@
     <row r="25" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="21"/>
       <c r="B25" s="20"/>
-      <c r="C25" s="23"/>
+      <c r="C25" s="29"/>
       <c r="D25" s="19"/>
       <c r="E25" s="17"/>
       <c r="F25" s="15"/>
@@ -1388,7 +1843,7 @@
     <row r="26" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="21"/>
       <c r="B26" s="20"/>
-      <c r="C26" s="23"/>
+      <c r="C26" s="29"/>
       <c r="D26" s="19"/>
       <c r="E26" s="17"/>
       <c r="F26" s="15"/>
@@ -1407,7 +1862,7 @@
     <row r="27" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="21"/>
       <c r="B27" s="20"/>
-      <c r="C27" s="23"/>
+      <c r="C27" s="29"/>
       <c r="D27" s="19"/>
       <c r="E27" s="17"/>
       <c r="F27" s="15"/>
@@ -1426,7 +1881,7 @@
     <row r="28" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="21"/>
       <c r="B28" s="20"/>
-      <c r="C28" s="23"/>
+      <c r="C28" s="29"/>
       <c r="D28" s="19"/>
       <c r="E28" s="17"/>
       <c r="F28" s="15"/>
@@ -1445,7 +1900,7 @@
     <row r="29" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="21"/>
       <c r="B29" s="20"/>
-      <c r="C29" s="23"/>
+      <c r="C29" s="29"/>
       <c r="D29" s="19"/>
       <c r="E29" s="17"/>
       <c r="F29" s="15"/>
@@ -1464,7 +1919,7 @@
     <row r="30" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="21"/>
       <c r="B30" s="20"/>
-      <c r="C30" s="23"/>
+      <c r="C30" s="29"/>
       <c r="D30" s="19"/>
       <c r="E30" s="17"/>
       <c r="F30" s="15"/>
@@ -1483,7 +1938,7 @@
     <row r="31" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="21"/>
       <c r="B31" s="20"/>
-      <c r="C31" s="23"/>
+      <c r="C31" s="29"/>
       <c r="D31" s="19"/>
       <c r="E31" s="17"/>
       <c r="F31" s="15"/>
@@ -1502,7 +1957,7 @@
     <row r="32" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="21"/>
       <c r="B32" s="20"/>
-      <c r="C32" s="23"/>
+      <c r="C32" s="29"/>
       <c r="D32" s="19"/>
       <c r="E32" s="17"/>
       <c r="F32" s="15"/>
@@ -1521,7 +1976,7 @@
     <row r="33" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="21"/>
       <c r="B33" s="20"/>
-      <c r="C33" s="23"/>
+      <c r="C33" s="29"/>
       <c r="D33" s="19"/>
       <c r="E33" s="17"/>
       <c r="F33" s="15"/>
@@ -1540,7 +1995,7 @@
     <row r="34" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="21"/>
       <c r="B34" s="20"/>
-      <c r="C34" s="23"/>
+      <c r="C34" s="29"/>
       <c r="D34" s="19"/>
       <c r="E34" s="17"/>
       <c r="F34" s="15"/>
@@ -1559,7 +2014,7 @@
     <row r="35" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="21"/>
       <c r="B35" s="20"/>
-      <c r="C35" s="23"/>
+      <c r="C35" s="29"/>
       <c r="D35" s="19"/>
       <c r="E35" s="17"/>
       <c r="F35" s="15"/>
@@ -1578,7 +2033,7 @@
     <row r="36" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="21"/>
       <c r="B36" s="20"/>
-      <c r="C36" s="23"/>
+      <c r="C36" s="29"/>
       <c r="D36" s="19"/>
       <c r="E36" s="17"/>
       <c r="F36" s="15"/>
@@ -1597,7 +2052,7 @@
     <row r="37" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="21"/>
       <c r="B37" s="20"/>
-      <c r="C37" s="23"/>
+      <c r="C37" s="29"/>
       <c r="D37" s="19"/>
       <c r="E37" s="17"/>
       <c r="F37" s="15"/>
@@ -1616,7 +2071,7 @@
     <row r="38" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="21"/>
       <c r="B38" s="20"/>
-      <c r="C38" s="23"/>
+      <c r="C38" s="29"/>
       <c r="D38" s="19"/>
       <c r="E38" s="17"/>
       <c r="F38" s="15"/>
@@ -1635,7 +2090,7 @@
     <row r="39" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="21"/>
       <c r="B39" s="20"/>
-      <c r="C39" s="23"/>
+      <c r="C39" s="29"/>
       <c r="D39" s="19"/>
       <c r="E39" s="17"/>
       <c r="F39" s="15"/>
@@ -1654,7 +2109,7 @@
     <row r="40" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="21"/>
       <c r="B40" s="20"/>
-      <c r="C40" s="23"/>
+      <c r="C40" s="29"/>
       <c r="D40" s="19"/>
       <c r="E40" s="17"/>
       <c r="F40" s="15"/>
@@ -1673,7 +2128,7 @@
     <row r="41" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="21"/>
       <c r="B41" s="20"/>
-      <c r="C41" s="23"/>
+      <c r="C41" s="29"/>
       <c r="D41" s="19"/>
       <c r="E41" s="17"/>
       <c r="F41" s="15"/>
@@ -1692,7 +2147,7 @@
     <row r="42" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="21"/>
       <c r="B42" s="20"/>
-      <c r="C42" s="23"/>
+      <c r="C42" s="29"/>
       <c r="D42" s="19"/>
       <c r="E42" s="17"/>
       <c r="F42" s="15"/>
@@ -1711,7 +2166,7 @@
     <row r="43" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="21"/>
       <c r="B43" s="20"/>
-      <c r="C43" s="23"/>
+      <c r="C43" s="29"/>
       <c r="D43" s="19"/>
       <c r="E43" s="17"/>
       <c r="F43" s="15"/>
@@ -1730,7 +2185,7 @@
     <row r="44" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="21"/>
       <c r="B44" s="20"/>
-      <c r="C44" s="23"/>
+      <c r="C44" s="29"/>
       <c r="D44" s="19"/>
       <c r="E44" s="17"/>
       <c r="F44" s="15"/>
@@ -1749,7 +2204,7 @@
     <row r="45" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="21"/>
       <c r="B45" s="20"/>
-      <c r="C45" s="23"/>
+      <c r="C45" s="29"/>
       <c r="D45" s="19"/>
       <c r="E45" s="17"/>
       <c r="F45" s="15"/>
@@ -1768,7 +2223,7 @@
     <row r="46" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="21"/>
       <c r="B46" s="20"/>
-      <c r="C46" s="23"/>
+      <c r="C46" s="29"/>
       <c r="D46" s="19"/>
       <c r="E46" s="17"/>
       <c r="F46" s="15"/>
@@ -1787,7 +2242,7 @@
     <row r="47" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="21"/>
       <c r="B47" s="20"/>
-      <c r="C47" s="23"/>
+      <c r="C47" s="29"/>
       <c r="D47" s="19"/>
       <c r="E47" s="17"/>
       <c r="F47" s="15"/>
@@ -1806,7 +2261,7 @@
     <row r="48" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="21"/>
       <c r="B48" s="20"/>
-      <c r="C48" s="23"/>
+      <c r="C48" s="29"/>
       <c r="D48" s="19"/>
       <c r="E48" s="17"/>
       <c r="F48" s="15"/>
@@ -1825,7 +2280,7 @@
     <row r="49" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="21"/>
       <c r="B49" s="20"/>
-      <c r="C49" s="23"/>
+      <c r="C49" s="29"/>
       <c r="D49" s="19"/>
       <c r="E49" s="17"/>
       <c r="F49" s="15"/>
@@ -1844,7 +2299,7 @@
     <row r="50" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="21"/>
       <c r="B50" s="20"/>
-      <c r="C50" s="23"/>
+      <c r="C50" s="29"/>
       <c r="D50" s="19"/>
       <c r="E50" s="17"/>
       <c r="F50" s="15"/>
@@ -1863,7 +2318,7 @@
     <row r="51" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="21"/>
       <c r="B51" s="20"/>
-      <c r="C51" s="23"/>
+      <c r="C51" s="29"/>
       <c r="D51" s="19"/>
       <c r="E51" s="17"/>
       <c r="F51" s="15"/>
@@ -1882,7 +2337,7 @@
     <row r="52" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="21"/>
       <c r="B52" s="20"/>
-      <c r="C52" s="23"/>
+      <c r="C52" s="29"/>
       <c r="D52" s="19"/>
       <c r="E52" s="17"/>
       <c r="F52" s="15"/>
@@ -1901,7 +2356,7 @@
     <row r="53" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="21"/>
       <c r="B53" s="20"/>
-      <c r="C53" s="23"/>
+      <c r="C53" s="29"/>
       <c r="D53" s="19"/>
       <c r="E53" s="17"/>
       <c r="F53" s="15"/>
@@ -1920,7 +2375,7 @@
     <row r="54" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="21"/>
       <c r="B54" s="20"/>
-      <c r="C54" s="23"/>
+      <c r="C54" s="29"/>
       <c r="D54" s="19"/>
       <c r="E54" s="17"/>
       <c r="F54" s="15"/>
@@ -1939,7 +2394,7 @@
     <row r="55" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="21"/>
       <c r="B55" s="20"/>
-      <c r="C55" s="23"/>
+      <c r="C55" s="29"/>
       <c r="D55" s="19"/>
       <c r="E55" s="17"/>
       <c r="F55" s="15"/>
@@ -1958,7 +2413,7 @@
     <row r="56" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="21"/>
       <c r="B56" s="20"/>
-      <c r="C56" s="23"/>
+      <c r="C56" s="29"/>
       <c r="D56" s="19"/>
       <c r="E56" s="17"/>
       <c r="F56" s="15"/>
@@ -1977,7 +2432,7 @@
     <row r="57" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="21"/>
       <c r="B57" s="20"/>
-      <c r="C57" s="23"/>
+      <c r="C57" s="29"/>
       <c r="D57" s="19"/>
       <c r="E57" s="17"/>
       <c r="F57" s="15"/>
@@ -1996,7 +2451,7 @@
     <row r="58" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="21"/>
       <c r="B58" s="20"/>
-      <c r="C58" s="23"/>
+      <c r="C58" s="29"/>
       <c r="D58" s="19"/>
       <c r="E58" s="17"/>
       <c r="F58" s="15"/>
@@ -2015,7 +2470,7 @@
     <row r="59" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="21"/>
       <c r="B59" s="20"/>
-      <c r="C59" s="23"/>
+      <c r="C59" s="29"/>
       <c r="D59" s="19"/>
       <c r="E59" s="17"/>
       <c r="F59" s="15"/>
@@ -2034,7 +2489,7 @@
     <row r="60" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="21"/>
       <c r="B60" s="20"/>
-      <c r="C60" s="23"/>
+      <c r="C60" s="29"/>
       <c r="D60" s="19"/>
       <c r="E60" s="17"/>
       <c r="F60" s="15"/>
@@ -2053,7 +2508,7 @@
     <row r="61" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="21"/>
       <c r="B61" s="20"/>
-      <c r="C61" s="23"/>
+      <c r="C61" s="29"/>
       <c r="D61" s="19"/>
       <c r="E61" s="17"/>
       <c r="F61" s="15"/>
@@ -2072,7 +2527,7 @@
     <row r="62" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="21"/>
       <c r="B62" s="20"/>
-      <c r="C62" s="23"/>
+      <c r="C62" s="29"/>
       <c r="D62" s="19"/>
       <c r="E62" s="17"/>
       <c r="F62" s="15"/>
@@ -2091,7 +2546,7 @@
     <row r="63" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="21"/>
       <c r="B63" s="20"/>
-      <c r="C63" s="23"/>
+      <c r="C63" s="29"/>
       <c r="D63" s="19"/>
       <c r="E63" s="17"/>
       <c r="F63" s="15"/>
@@ -2110,7 +2565,7 @@
     <row r="64" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="21"/>
       <c r="B64" s="20"/>
-      <c r="C64" s="23"/>
+      <c r="C64" s="29"/>
       <c r="D64" s="19"/>
       <c r="E64" s="17"/>
       <c r="F64" s="15"/>
@@ -2129,7 +2584,7 @@
     <row r="65" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="21"/>
       <c r="B65" s="20"/>
-      <c r="C65" s="23"/>
+      <c r="C65" s="29"/>
       <c r="D65" s="19"/>
       <c r="E65" s="17"/>
       <c r="F65" s="15"/>
@@ -2148,7 +2603,7 @@
     <row r="66" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="21"/>
       <c r="B66" s="20"/>
-      <c r="C66" s="23"/>
+      <c r="C66" s="29"/>
       <c r="D66" s="19"/>
       <c r="E66" s="17"/>
       <c r="F66" s="15"/>
@@ -2167,7 +2622,7 @@
     <row r="67" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="21"/>
       <c r="B67" s="20"/>
-      <c r="C67" s="23"/>
+      <c r="C67" s="29"/>
       <c r="D67" s="19"/>
       <c r="E67" s="17"/>
       <c r="F67" s="15"/>
@@ -2186,7 +2641,7 @@
     <row r="68" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="21"/>
       <c r="B68" s="20"/>
-      <c r="C68" s="23"/>
+      <c r="C68" s="29"/>
       <c r="D68" s="19"/>
       <c r="E68" s="17"/>
       <c r="F68" s="15"/>
@@ -2205,7 +2660,7 @@
     <row r="69" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="21"/>
       <c r="B69" s="20"/>
-      <c r="C69" s="23"/>
+      <c r="C69" s="29"/>
       <c r="D69" s="19"/>
       <c r="E69" s="17"/>
       <c r="F69" s="15"/>
@@ -2224,7 +2679,7 @@
     <row r="70" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="21"/>
       <c r="B70" s="20"/>
-      <c r="C70" s="23"/>
+      <c r="C70" s="29"/>
       <c r="D70" s="19"/>
       <c r="E70" s="17"/>
       <c r="F70" s="15"/>
@@ -2243,7 +2698,7 @@
     <row r="71" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="21"/>
       <c r="B71" s="20"/>
-      <c r="C71" s="23"/>
+      <c r="C71" s="29"/>
       <c r="D71" s="19"/>
       <c r="E71" s="17"/>
       <c r="F71" s="15"/>
@@ -2262,7 +2717,7 @@
     <row r="72" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="21"/>
       <c r="B72" s="20"/>
-      <c r="C72" s="23"/>
+      <c r="C72" s="29"/>
       <c r="D72" s="19"/>
       <c r="E72" s="17"/>
       <c r="F72" s="15"/>
@@ -2281,7 +2736,7 @@
     <row r="73" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="21"/>
       <c r="B73" s="20"/>
-      <c r="C73" s="23"/>
+      <c r="C73" s="29"/>
       <c r="D73" s="19"/>
       <c r="E73" s="17"/>
       <c r="F73" s="15"/>
@@ -2300,7 +2755,7 @@
     <row r="74" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="21"/>
       <c r="B74" s="20"/>
-      <c r="C74" s="23"/>
+      <c r="C74" s="29"/>
       <c r="D74" s="19"/>
       <c r="E74" s="17"/>
       <c r="F74" s="15"/>
@@ -2319,7 +2774,7 @@
     <row r="75" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="21"/>
       <c r="B75" s="20"/>
-      <c r="C75" s="23"/>
+      <c r="C75" s="29"/>
       <c r="D75" s="19"/>
       <c r="E75" s="17"/>
       <c r="F75" s="15"/>
@@ -2338,7 +2793,7 @@
     <row r="76" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="21"/>
       <c r="B76" s="20"/>
-      <c r="C76" s="23"/>
+      <c r="C76" s="29"/>
       <c r="D76" s="19"/>
       <c r="E76" s="17"/>
       <c r="F76" s="15"/>
@@ -2357,7 +2812,7 @@
     <row r="77" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="21"/>
       <c r="B77" s="20"/>
-      <c r="C77" s="23"/>
+      <c r="C77" s="29"/>
       <c r="D77" s="19"/>
       <c r="E77" s="17"/>
       <c r="F77" s="15"/>
@@ -2376,7 +2831,7 @@
     <row r="78" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="21"/>
       <c r="B78" s="20"/>
-      <c r="C78" s="23"/>
+      <c r="C78" s="29"/>
       <c r="D78" s="19"/>
       <c r="E78" s="17"/>
       <c r="F78" s="15"/>
@@ -2395,7 +2850,7 @@
     <row r="79" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="21"/>
       <c r="B79" s="20"/>
-      <c r="C79" s="23"/>
+      <c r="C79" s="29"/>
       <c r="D79" s="19"/>
       <c r="E79" s="17"/>
       <c r="F79" s="15"/>
@@ -2414,7 +2869,7 @@
     <row r="80" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="21"/>
       <c r="B80" s="20"/>
-      <c r="C80" s="23"/>
+      <c r="C80" s="29"/>
       <c r="D80" s="19"/>
       <c r="E80" s="17"/>
       <c r="F80" s="15"/>
@@ -2433,7 +2888,7 @@
     <row r="81" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="21"/>
       <c r="B81" s="20"/>
-      <c r="C81" s="23"/>
+      <c r="C81" s="29"/>
       <c r="D81" s="19"/>
       <c r="E81" s="17"/>
       <c r="F81" s="15"/>
@@ -2452,7 +2907,7 @@
     <row r="82" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="21"/>
       <c r="B82" s="20"/>
-      <c r="C82" s="23"/>
+      <c r="C82" s="29"/>
       <c r="D82" s="19"/>
       <c r="E82" s="17"/>
       <c r="F82" s="15"/>
@@ -2471,7 +2926,7 @@
     <row r="83" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="21"/>
       <c r="B83" s="20"/>
-      <c r="C83" s="23"/>
+      <c r="C83" s="29"/>
       <c r="D83" s="19"/>
       <c r="E83" s="17"/>
       <c r="F83" s="15"/>
@@ -2490,7 +2945,7 @@
     <row r="84" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="21"/>
       <c r="B84" s="20"/>
-      <c r="C84" s="23"/>
+      <c r="C84" s="29"/>
       <c r="D84" s="19"/>
       <c r="E84" s="17"/>
       <c r="F84" s="15"/>
@@ -2509,7 +2964,7 @@
     <row r="85" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="21"/>
       <c r="B85" s="20"/>
-      <c r="C85" s="23"/>
+      <c r="C85" s="29"/>
       <c r="D85" s="19"/>
       <c r="E85" s="17"/>
       <c r="F85" s="15"/>
@@ -2528,7 +2983,7 @@
     <row r="86" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="21"/>
       <c r="B86" s="20"/>
-      <c r="C86" s="23"/>
+      <c r="C86" s="29"/>
       <c r="D86" s="19"/>
       <c r="E86" s="17"/>
       <c r="F86" s="15"/>
@@ -2547,7 +3002,7 @@
     <row r="87" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="21"/>
       <c r="B87" s="20"/>
-      <c r="C87" s="23"/>
+      <c r="C87" s="29"/>
       <c r="D87" s="19"/>
       <c r="E87" s="17"/>
       <c r="F87" s="15"/>
@@ -2566,7 +3021,7 @@
     <row r="88" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="21"/>
       <c r="B88" s="20"/>
-      <c r="C88" s="23"/>
+      <c r="C88" s="29"/>
       <c r="D88" s="19"/>
       <c r="E88" s="17"/>
       <c r="F88" s="15"/>
@@ -2585,7 +3040,7 @@
     <row r="89" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="21"/>
       <c r="B89" s="20"/>
-      <c r="C89" s="23"/>
+      <c r="C89" s="29"/>
       <c r="D89" s="19"/>
       <c r="E89" s="17"/>
       <c r="F89" s="15"/>
@@ -2604,7 +3059,7 @@
     <row r="90" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="21"/>
       <c r="B90" s="20"/>
-      <c r="C90" s="23"/>
+      <c r="C90" s="29"/>
       <c r="D90" s="19"/>
       <c r="E90" s="17"/>
       <c r="F90" s="15"/>
@@ -2623,7 +3078,7 @@
     <row r="91" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="21"/>
       <c r="B91" s="20"/>
-      <c r="C91" s="23"/>
+      <c r="C91" s="29"/>
       <c r="D91" s="19"/>
       <c r="E91" s="17"/>
       <c r="F91" s="15"/>
@@ -2642,7 +3097,7 @@
     <row r="92" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="21"/>
       <c r="B92" s="20"/>
-      <c r="C92" s="23"/>
+      <c r="C92" s="29"/>
       <c r="D92" s="19"/>
       <c r="E92" s="17"/>
       <c r="F92" s="15"/>
@@ -2661,7 +3116,7 @@
     <row r="93" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="21"/>
       <c r="B93" s="20"/>
-      <c r="C93" s="23"/>
+      <c r="C93" s="29"/>
       <c r="D93" s="19"/>
       <c r="E93" s="17"/>
       <c r="F93" s="15"/>
@@ -2680,7 +3135,7 @@
     <row r="94" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="21"/>
       <c r="B94" s="20"/>
-      <c r="C94" s="23"/>
+      <c r="C94" s="29"/>
       <c r="D94" s="19"/>
       <c r="E94" s="17"/>
       <c r="F94" s="15"/>
@@ -2699,7 +3154,7 @@
     <row r="95" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="21"/>
       <c r="B95" s="20"/>
-      <c r="C95" s="23"/>
+      <c r="C95" s="29"/>
       <c r="D95" s="19"/>
       <c r="E95" s="17"/>
       <c r="F95" s="15"/>
@@ -2718,7 +3173,7 @@
     <row r="96" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="21"/>
       <c r="B96" s="20"/>
-      <c r="C96" s="23"/>
+      <c r="C96" s="29"/>
       <c r="D96" s="19"/>
       <c r="E96" s="17"/>
       <c r="F96" s="15"/>
@@ -2737,7 +3192,7 @@
     <row r="97" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="21"/>
       <c r="B97" s="20"/>
-      <c r="C97" s="23"/>
+      <c r="C97" s="29"/>
       <c r="D97" s="19"/>
       <c r="E97" s="17"/>
       <c r="F97" s="15"/>
@@ -2756,7 +3211,7 @@
     <row r="98" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="21"/>
       <c r="B98" s="20"/>
-      <c r="C98" s="23"/>
+      <c r="C98" s="29"/>
       <c r="D98" s="19"/>
       <c r="E98" s="17"/>
       <c r="F98" s="15"/>
@@ -2775,7 +3230,7 @@
     <row r="99" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="21"/>
       <c r="B99" s="20"/>
-      <c r="C99" s="23"/>
+      <c r="C99" s="29"/>
       <c r="D99" s="19"/>
       <c r="E99" s="17"/>
       <c r="F99" s="15"/>
@@ -2794,7 +3249,7 @@
     <row r="100" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="21"/>
       <c r="B100" s="20"/>
-      <c r="C100" s="23"/>
+      <c r="C100" s="29"/>
       <c r="D100" s="19"/>
       <c r="E100" s="17"/>
       <c r="F100" s="15"/>
@@ -2813,7 +3268,7 @@
     <row r="101" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" s="21"/>
       <c r="B101" s="20"/>
-      <c r="C101" s="23"/>
+      <c r="C101" s="29"/>
       <c r="D101" s="19"/>
       <c r="E101" s="17"/>
       <c r="F101" s="15"/>
@@ -2832,7 +3287,7 @@
     <row r="102" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" s="21"/>
       <c r="B102" s="20"/>
-      <c r="C102" s="23"/>
+      <c r="C102" s="29"/>
       <c r="D102" s="19"/>
       <c r="E102" s="17"/>
       <c r="F102" s="15"/>
@@ -2851,7 +3306,7 @@
     <row r="103" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A103" s="21"/>
       <c r="B103" s="20"/>
-      <c r="C103" s="23"/>
+      <c r="C103" s="29"/>
       <c r="D103" s="19"/>
       <c r="E103" s="17"/>
       <c r="F103" s="15"/>
@@ -2870,7 +3325,7 @@
     <row r="104" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A104" s="21"/>
       <c r="B104" s="20"/>
-      <c r="C104" s="23"/>
+      <c r="C104" s="29"/>
       <c r="D104" s="19"/>
       <c r="E104" s="17"/>
       <c r="F104" s="15"/>
@@ -2889,7 +3344,7 @@
     <row r="105" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A105" s="21"/>
       <c r="B105" s="20"/>
-      <c r="C105" s="23"/>
+      <c r="C105" s="29"/>
       <c r="D105" s="19"/>
       <c r="E105" s="17"/>
       <c r="F105" s="15"/>
@@ -2908,7 +3363,7 @@
     <row r="106" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A106" s="21"/>
       <c r="B106" s="20"/>
-      <c r="C106" s="23"/>
+      <c r="C106" s="29"/>
       <c r="D106" s="19"/>
       <c r="E106" s="17"/>
       <c r="F106" s="15"/>
@@ -2927,7 +3382,7 @@
     <row r="107" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A107" s="21"/>
       <c r="B107" s="20"/>
-      <c r="C107" s="23"/>
+      <c r="C107" s="29"/>
       <c r="D107" s="19"/>
       <c r="E107" s="17"/>
       <c r="F107" s="15"/>
@@ -2946,7 +3401,7 @@
     <row r="108" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A108" s="21"/>
       <c r="B108" s="20"/>
-      <c r="C108" s="23"/>
+      <c r="C108" s="29"/>
       <c r="D108" s="19"/>
       <c r="E108" s="17"/>
       <c r="F108" s="15"/>
@@ -2965,7 +3420,7 @@
     <row r="109" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A109" s="21"/>
       <c r="B109" s="20"/>
-      <c r="C109" s="23"/>
+      <c r="C109" s="29"/>
       <c r="D109" s="19"/>
       <c r="E109" s="17"/>
       <c r="F109" s="15"/>
@@ -2984,7 +3439,7 @@
     <row r="110" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A110" s="21"/>
       <c r="B110" s="20"/>
-      <c r="C110" s="23"/>
+      <c r="C110" s="29"/>
       <c r="D110" s="19"/>
       <c r="E110" s="17"/>
       <c r="F110" s="15"/>
@@ -3003,7 +3458,7 @@
     <row r="111" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A111" s="21"/>
       <c r="B111" s="20"/>
-      <c r="C111" s="23"/>
+      <c r="C111" s="29"/>
       <c r="D111" s="19"/>
       <c r="E111" s="17"/>
       <c r="F111" s="15"/>
@@ -3022,7 +3477,7 @@
     <row r="112" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A112" s="21"/>
       <c r="B112" s="20"/>
-      <c r="C112" s="23"/>
+      <c r="C112" s="29"/>
       <c r="D112" s="19"/>
       <c r="E112" s="17"/>
       <c r="F112" s="15"/>
@@ -3041,7 +3496,7 @@
     <row r="113" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A113" s="21"/>
       <c r="B113" s="20"/>
-      <c r="C113" s="23"/>
+      <c r="C113" s="29"/>
       <c r="D113" s="19"/>
       <c r="E113" s="17"/>
       <c r="F113" s="15"/>
@@ -3060,7 +3515,7 @@
     <row r="114" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A114" s="21"/>
       <c r="B114" s="20"/>
-      <c r="C114" s="23"/>
+      <c r="C114" s="29"/>
       <c r="D114" s="19"/>
       <c r="E114" s="17"/>
       <c r="F114" s="15"/>
@@ -3079,7 +3534,7 @@
     <row r="115" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A115" s="21"/>
       <c r="B115" s="20"/>
-      <c r="C115" s="23"/>
+      <c r="C115" s="29"/>
       <c r="D115" s="19"/>
       <c r="E115" s="17"/>
       <c r="F115" s="15"/>
@@ -3098,7 +3553,7 @@
     <row r="116" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A116" s="21"/>
       <c r="B116" s="20"/>
-      <c r="C116" s="23"/>
+      <c r="C116" s="29"/>
       <c r="D116" s="19"/>
       <c r="E116" s="17"/>
       <c r="F116" s="15"/>
@@ -3117,7 +3572,7 @@
     <row r="117" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A117" s="21"/>
       <c r="B117" s="20"/>
-      <c r="C117" s="23"/>
+      <c r="C117" s="29"/>
       <c r="D117" s="19"/>
       <c r="E117" s="17"/>
       <c r="F117" s="15"/>
@@ -3136,7 +3591,7 @@
     <row r="118" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A118" s="21"/>
       <c r="B118" s="20"/>
-      <c r="C118" s="23"/>
+      <c r="C118" s="29"/>
       <c r="D118" s="19"/>
       <c r="E118" s="17"/>
       <c r="F118" s="15"/>
@@ -3155,7 +3610,7 @@
     <row r="119" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A119" s="21"/>
       <c r="B119" s="20"/>
-      <c r="C119" s="23"/>
+      <c r="C119" s="29"/>
       <c r="D119" s="19"/>
       <c r="E119" s="17"/>
       <c r="F119" s="15"/>
@@ -3174,7 +3629,7 @@
     <row r="120" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A120" s="21"/>
       <c r="B120" s="20"/>
-      <c r="C120" s="23"/>
+      <c r="C120" s="29"/>
       <c r="D120" s="19"/>
       <c r="E120" s="17"/>
       <c r="F120" s="15"/>
@@ -3193,7 +3648,7 @@
     <row r="121" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A121" s="21"/>
       <c r="B121" s="20"/>
-      <c r="C121" s="23"/>
+      <c r="C121" s="29"/>
       <c r="D121" s="19"/>
       <c r="E121" s="17"/>
       <c r="F121" s="15"/>
@@ -3212,7 +3667,7 @@
     <row r="122" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A122" s="21"/>
       <c r="B122" s="20"/>
-      <c r="C122" s="23"/>
+      <c r="C122" s="29"/>
       <c r="D122" s="19"/>
       <c r="E122" s="17"/>
       <c r="F122" s="15"/>
@@ -3231,7 +3686,7 @@
     <row r="123" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A123" s="21"/>
       <c r="B123" s="20"/>
-      <c r="C123" s="23"/>
+      <c r="C123" s="29"/>
       <c r="D123" s="19"/>
       <c r="E123" s="17"/>
       <c r="F123" s="15"/>
@@ -3250,7 +3705,7 @@
     <row r="124" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A124" s="21"/>
       <c r="B124" s="20"/>
-      <c r="C124" s="23"/>
+      <c r="C124" s="29"/>
       <c r="D124" s="19"/>
       <c r="E124" s="17"/>
       <c r="F124" s="15"/>
@@ -3269,7 +3724,7 @@
     <row r="125" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A125" s="21"/>
       <c r="B125" s="20"/>
-      <c r="C125" s="23"/>
+      <c r="C125" s="29"/>
       <c r="D125" s="19"/>
       <c r="E125" s="17"/>
       <c r="F125" s="15"/>
@@ -3288,7 +3743,7 @@
     <row r="126" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A126" s="21"/>
       <c r="B126" s="20"/>
-      <c r="C126" s="23"/>
+      <c r="C126" s="29"/>
       <c r="D126" s="19"/>
       <c r="E126" s="17"/>
       <c r="F126" s="15"/>
@@ -3307,7 +3762,7 @@
     <row r="127" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A127" s="21"/>
       <c r="B127" s="20"/>
-      <c r="C127" s="23"/>
+      <c r="C127" s="29"/>
       <c r="D127" s="19"/>
       <c r="E127" s="17"/>
       <c r="F127" s="15"/>
@@ -3326,7 +3781,7 @@
     <row r="128" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A128" s="21"/>
       <c r="B128" s="20"/>
-      <c r="C128" s="23"/>
+      <c r="C128" s="29"/>
       <c r="D128" s="19"/>
       <c r="E128" s="17"/>
       <c r="F128" s="15"/>
@@ -3345,7 +3800,7 @@
     <row r="129" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A129" s="21"/>
       <c r="B129" s="20"/>
-      <c r="C129" s="23"/>
+      <c r="C129" s="29"/>
       <c r="D129" s="19"/>
       <c r="E129" s="17"/>
       <c r="F129" s="15"/>
@@ -3364,7 +3819,7 @@
     <row r="130" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A130" s="21"/>
       <c r="B130" s="20"/>
-      <c r="C130" s="23"/>
+      <c r="C130" s="29"/>
       <c r="D130" s="19"/>
       <c r="E130" s="17"/>
       <c r="F130" s="15"/>
@@ -3383,7 +3838,7 @@
     <row r="131" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A131" s="21"/>
       <c r="B131" s="20"/>
-      <c r="C131" s="23"/>
+      <c r="C131" s="29"/>
       <c r="D131" s="19"/>
       <c r="E131" s="17"/>
       <c r="F131" s="15"/>
@@ -3402,7 +3857,7 @@
     <row r="132" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A132" s="21"/>
       <c r="B132" s="20"/>
-      <c r="C132" s="23"/>
+      <c r="C132" s="29"/>
       <c r="D132" s="19"/>
       <c r="E132" s="17"/>
       <c r="F132" s="15"/>
@@ -3421,7 +3876,7 @@
     <row r="133" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A133" s="21"/>
       <c r="B133" s="20"/>
-      <c r="C133" s="23"/>
+      <c r="C133" s="29"/>
       <c r="D133" s="19"/>
       <c r="E133" s="17"/>
       <c r="F133" s="15"/>
@@ -3440,7 +3895,7 @@
     <row r="134" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A134" s="21"/>
       <c r="B134" s="20"/>
-      <c r="C134" s="23"/>
+      <c r="C134" s="29"/>
       <c r="D134" s="19"/>
       <c r="E134" s="17"/>
       <c r="F134" s="15"/>
@@ -3459,7 +3914,7 @@
     <row r="135" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A135" s="21"/>
       <c r="B135" s="20"/>
-      <c r="C135" s="23"/>
+      <c r="C135" s="29"/>
       <c r="D135" s="19"/>
       <c r="E135" s="17"/>
       <c r="F135" s="15"/>
@@ -3478,7 +3933,7 @@
     <row r="136" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A136" s="21"/>
       <c r="B136" s="20"/>
-      <c r="C136" s="23"/>
+      <c r="C136" s="29"/>
       <c r="D136" s="19"/>
       <c r="E136" s="17"/>
       <c r="F136" s="15"/>
@@ -3497,7 +3952,7 @@
     <row r="137" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A137" s="21"/>
       <c r="B137" s="20"/>
-      <c r="C137" s="23"/>
+      <c r="C137" s="29"/>
       <c r="D137" s="19"/>
       <c r="E137" s="17"/>
       <c r="F137" s="15"/>
@@ -3516,7 +3971,7 @@
     <row r="138" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A138" s="21"/>
       <c r="B138" s="20"/>
-      <c r="C138" s="23"/>
+      <c r="C138" s="29"/>
       <c r="D138" s="19"/>
       <c r="E138" s="17"/>
       <c r="F138" s="15"/>
@@ -3535,7 +3990,7 @@
     <row r="139" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A139" s="21"/>
       <c r="B139" s="20"/>
-      <c r="C139" s="23"/>
+      <c r="C139" s="29"/>
       <c r="D139" s="19"/>
       <c r="E139" s="17"/>
       <c r="F139" s="15"/>
@@ -3554,7 +4009,7 @@
     <row r="140" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A140" s="21"/>
       <c r="B140" s="20"/>
-      <c r="C140" s="23"/>
+      <c r="C140" s="29"/>
       <c r="D140" s="19"/>
       <c r="E140" s="17"/>
       <c r="F140" s="15"/>
@@ -3573,7 +4028,7 @@
     <row r="141" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A141" s="21"/>
       <c r="B141" s="20"/>
-      <c r="C141" s="23"/>
+      <c r="C141" s="29"/>
       <c r="D141" s="19"/>
       <c r="E141" s="17"/>
       <c r="F141" s="15"/>
@@ -3592,7 +4047,7 @@
     <row r="142" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A142" s="21"/>
       <c r="B142" s="20"/>
-      <c r="C142" s="23"/>
+      <c r="C142" s="29"/>
       <c r="D142" s="19"/>
       <c r="E142" s="17"/>
       <c r="F142" s="15"/>
@@ -3611,7 +4066,7 @@
     <row r="143" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A143" s="21"/>
       <c r="B143" s="20"/>
-      <c r="C143" s="23"/>
+      <c r="C143" s="29"/>
       <c r="D143" s="19"/>
       <c r="E143" s="17"/>
       <c r="F143" s="15"/>
@@ -3630,7 +4085,7 @@
     <row r="144" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A144" s="21"/>
       <c r="B144" s="20"/>
-      <c r="C144" s="23"/>
+      <c r="C144" s="29"/>
       <c r="D144" s="19"/>
       <c r="E144" s="17"/>
       <c r="F144" s="15"/>
@@ -3649,7 +4104,7 @@
     <row r="145" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A145" s="21"/>
       <c r="B145" s="20"/>
-      <c r="C145" s="23"/>
+      <c r="C145" s="29"/>
       <c r="D145" s="19"/>
       <c r="E145" s="17"/>
       <c r="F145" s="15"/>
@@ -3668,7 +4123,7 @@
     <row r="146" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A146" s="21"/>
       <c r="B146" s="20"/>
-      <c r="C146" s="23"/>
+      <c r="C146" s="29"/>
       <c r="D146" s="19"/>
       <c r="E146" s="17"/>
       <c r="F146" s="15"/>
@@ -3687,7 +4142,7 @@
     <row r="147" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A147" s="21"/>
       <c r="B147" s="20"/>
-      <c r="C147" s="23"/>
+      <c r="C147" s="29"/>
       <c r="D147" s="19"/>
       <c r="E147" s="17"/>
       <c r="F147" s="15"/>
@@ -3706,7 +4161,7 @@
     <row r="148" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A148" s="21"/>
       <c r="B148" s="20"/>
-      <c r="C148" s="23"/>
+      <c r="C148" s="29"/>
       <c r="D148" s="19"/>
       <c r="E148" s="17"/>
       <c r="F148" s="15"/>
@@ -3725,7 +4180,7 @@
     <row r="149" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A149" s="21"/>
       <c r="B149" s="20"/>
-      <c r="C149" s="23"/>
+      <c r="C149" s="29"/>
       <c r="D149" s="19"/>
       <c r="E149" s="17"/>
       <c r="F149" s="15"/>
@@ -3744,7 +4199,7 @@
     <row r="150" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A150" s="21"/>
       <c r="B150" s="20"/>
-      <c r="C150" s="23"/>
+      <c r="C150" s="29"/>
       <c r="D150" s="19"/>
       <c r="E150" s="17"/>
       <c r="F150" s="15"/>
@@ -3763,7 +4218,7 @@
     <row r="151" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A151" s="21"/>
       <c r="B151" s="20"/>
-      <c r="C151" s="23"/>
+      <c r="C151" s="29"/>
       <c r="D151" s="19"/>
       <c r="E151" s="17"/>
       <c r="F151" s="15"/>
@@ -3782,7 +4237,7 @@
     <row r="152" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A152" s="21"/>
       <c r="B152" s="20"/>
-      <c r="C152" s="23"/>
+      <c r="C152" s="29"/>
       <c r="D152" s="19"/>
       <c r="E152" s="17"/>
       <c r="F152" s="15"/>
@@ -3801,7 +4256,7 @@
     <row r="153" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A153" s="21"/>
       <c r="B153" s="20"/>
-      <c r="C153" s="23"/>
+      <c r="C153" s="29"/>
       <c r="D153" s="19"/>
       <c r="E153" s="17"/>
       <c r="F153" s="15"/>
@@ -3820,7 +4275,7 @@
     <row r="154" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A154" s="21"/>
       <c r="B154" s="20"/>
-      <c r="C154" s="23"/>
+      <c r="C154" s="29"/>
       <c r="D154" s="19"/>
       <c r="E154" s="17"/>
       <c r="F154" s="15"/>
@@ -3839,7 +4294,7 @@
     <row r="155" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A155" s="21"/>
       <c r="B155" s="20"/>
-      <c r="C155" s="23"/>
+      <c r="C155" s="29"/>
       <c r="D155" s="19"/>
       <c r="E155" s="17"/>
       <c r="F155" s="15"/>
@@ -3858,7 +4313,7 @@
     <row r="156" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A156" s="21"/>
       <c r="B156" s="20"/>
-      <c r="C156" s="23"/>
+      <c r="C156" s="29"/>
       <c r="D156" s="19"/>
       <c r="E156" s="17"/>
       <c r="F156" s="15"/>
@@ -3877,7 +4332,7 @@
     <row r="157" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A157" s="21"/>
       <c r="B157" s="20"/>
-      <c r="C157" s="23"/>
+      <c r="C157" s="29"/>
       <c r="D157" s="19"/>
       <c r="E157" s="17"/>
       <c r="F157" s="15"/>
@@ -3896,7 +4351,7 @@
     <row r="158" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A158" s="21"/>
       <c r="B158" s="20"/>
-      <c r="C158" s="23"/>
+      <c r="C158" s="29"/>
       <c r="D158" s="19"/>
       <c r="E158" s="17"/>
       <c r="F158" s="15"/>
@@ -3915,7 +4370,7 @@
     <row r="159" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A159" s="21"/>
       <c r="B159" s="20"/>
-      <c r="C159" s="23"/>
+      <c r="C159" s="29"/>
       <c r="D159" s="19"/>
       <c r="E159" s="17"/>
       <c r="F159" s="15"/>
@@ -3934,7 +4389,7 @@
     <row r="160" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A160" s="21"/>
       <c r="B160" s="20"/>
-      <c r="C160" s="23"/>
+      <c r="C160" s="29"/>
       <c r="D160" s="19"/>
       <c r="E160" s="17"/>
       <c r="F160" s="15"/>
@@ -3953,7 +4408,7 @@
     <row r="161" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A161" s="21"/>
       <c r="B161" s="20"/>
-      <c r="C161" s="23"/>
+      <c r="C161" s="29"/>
       <c r="D161" s="19"/>
       <c r="E161" s="17"/>
       <c r="F161" s="15"/>
@@ -3972,7 +4427,7 @@
     <row r="162" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A162" s="21"/>
       <c r="B162" s="20"/>
-      <c r="C162" s="23"/>
+      <c r="C162" s="29"/>
       <c r="D162" s="19"/>
       <c r="E162" s="17"/>
       <c r="F162" s="15"/>
@@ -3991,7 +4446,7 @@
     <row r="163" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A163" s="21"/>
       <c r="B163" s="20"/>
-      <c r="C163" s="23"/>
+      <c r="C163" s="29"/>
       <c r="D163" s="19"/>
       <c r="E163" s="17"/>
       <c r="F163" s="15"/>
@@ -4010,7 +4465,7 @@
     <row r="164" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A164" s="21"/>
       <c r="B164" s="20"/>
-      <c r="C164" s="23"/>
+      <c r="C164" s="29"/>
       <c r="D164" s="19"/>
       <c r="E164" s="17"/>
       <c r="F164" s="15"/>
@@ -4029,7 +4484,7 @@
     <row r="165" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A165" s="21"/>
       <c r="B165" s="20"/>
-      <c r="C165" s="23"/>
+      <c r="C165" s="29"/>
       <c r="D165" s="19"/>
       <c r="E165" s="17"/>
       <c r="F165" s="15"/>
@@ -4048,7 +4503,7 @@
     <row r="166" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A166" s="21"/>
       <c r="B166" s="20"/>
-      <c r="C166" s="23"/>
+      <c r="C166" s="29"/>
       <c r="D166" s="19"/>
       <c r="E166" s="17"/>
       <c r="F166" s="15"/>
@@ -4067,7 +4522,7 @@
     <row r="167" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A167" s="21"/>
       <c r="B167" s="20"/>
-      <c r="C167" s="23"/>
+      <c r="C167" s="29"/>
       <c r="D167" s="19"/>
       <c r="E167" s="17"/>
       <c r="F167" s="15"/>
@@ -4086,7 +4541,7 @@
     <row r="168" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A168" s="21"/>
       <c r="B168" s="20"/>
-      <c r="C168" s="23"/>
+      <c r="C168" s="29"/>
       <c r="D168" s="19"/>
       <c r="E168" s="17"/>
       <c r="F168" s="15"/>
@@ -4105,7 +4560,7 @@
     <row r="169" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A169" s="21"/>
       <c r="B169" s="20"/>
-      <c r="C169" s="23"/>
+      <c r="C169" s="29"/>
       <c r="D169" s="19"/>
       <c r="E169" s="17"/>
       <c r="F169" s="15"/>
@@ -4124,7 +4579,7 @@
     <row r="170" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A170" s="21"/>
       <c r="B170" s="20"/>
-      <c r="C170" s="23"/>
+      <c r="C170" s="29"/>
       <c r="D170" s="19"/>
       <c r="E170" s="17"/>
       <c r="F170" s="15"/>
@@ -4143,7 +4598,7 @@
     <row r="171" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A171" s="21"/>
       <c r="B171" s="20"/>
-      <c r="C171" s="23"/>
+      <c r="C171" s="29"/>
       <c r="D171" s="19"/>
       <c r="E171" s="17"/>
       <c r="F171" s="15"/>
@@ -4162,7 +4617,7 @@
     <row r="172" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A172" s="21"/>
       <c r="B172" s="20"/>
-      <c r="C172" s="23"/>
+      <c r="C172" s="29"/>
       <c r="D172" s="19"/>
       <c r="E172" s="17"/>
       <c r="F172" s="15"/>
@@ -4181,7 +4636,7 @@
     <row r="173" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A173" s="21"/>
       <c r="B173" s="20"/>
-      <c r="C173" s="23"/>
+      <c r="C173" s="29"/>
       <c r="D173" s="19"/>
       <c r="E173" s="17"/>
       <c r="F173" s="15"/>
@@ -4200,7 +4655,7 @@
     <row r="174" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A174" s="21"/>
       <c r="B174" s="20"/>
-      <c r="C174" s="23"/>
+      <c r="C174" s="29"/>
       <c r="D174" s="19"/>
       <c r="E174" s="17"/>
       <c r="F174" s="15"/>
@@ -4219,7 +4674,7 @@
     <row r="175" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A175" s="21"/>
       <c r="B175" s="20"/>
-      <c r="C175" s="23"/>
+      <c r="C175" s="29"/>
       <c r="D175" s="19"/>
       <c r="E175" s="17"/>
       <c r="F175" s="15"/>
@@ -4238,7 +4693,7 @@
     <row r="176" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A176" s="21"/>
       <c r="B176" s="20"/>
-      <c r="C176" s="23"/>
+      <c r="C176" s="29"/>
       <c r="D176" s="19"/>
       <c r="E176" s="17"/>
       <c r="F176" s="15"/>
@@ -4257,7 +4712,7 @@
     <row r="177" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A177" s="21"/>
       <c r="B177" s="20"/>
-      <c r="C177" s="23"/>
+      <c r="C177" s="29"/>
       <c r="D177" s="19"/>
       <c r="E177" s="17"/>
       <c r="F177" s="15"/>
@@ -4276,7 +4731,7 @@
     <row r="178" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A178" s="21"/>
       <c r="B178" s="20"/>
-      <c r="C178" s="23"/>
+      <c r="C178" s="29"/>
       <c r="D178" s="19"/>
       <c r="E178" s="17"/>
       <c r="F178" s="15"/>
@@ -4295,7 +4750,7 @@
     <row r="179" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A179" s="21"/>
       <c r="B179" s="20"/>
-      <c r="C179" s="23"/>
+      <c r="C179" s="29"/>
       <c r="D179" s="19"/>
       <c r="E179" s="17"/>
       <c r="F179" s="15"/>
@@ -4314,7 +4769,7 @@
     <row r="180" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A180" s="21"/>
       <c r="B180" s="20"/>
-      <c r="C180" s="23"/>
+      <c r="C180" s="29"/>
       <c r="D180" s="19"/>
       <c r="E180" s="17"/>
       <c r="F180" s="15"/>
@@ -4333,7 +4788,7 @@
     <row r="181" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A181" s="21"/>
       <c r="B181" s="20"/>
-      <c r="C181" s="23"/>
+      <c r="C181" s="29"/>
       <c r="D181" s="19"/>
       <c r="E181" s="17"/>
       <c r="F181" s="15"/>
@@ -4352,7 +4807,7 @@
     <row r="182" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A182" s="21"/>
       <c r="B182" s="20"/>
-      <c r="C182" s="23"/>
+      <c r="C182" s="29"/>
       <c r="D182" s="19"/>
       <c r="E182" s="17"/>
       <c r="F182" s="15"/>
@@ -4371,7 +4826,7 @@
     <row r="183" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A183" s="21"/>
       <c r="B183" s="20"/>
-      <c r="C183" s="23"/>
+      <c r="C183" s="29"/>
       <c r="D183" s="19"/>
       <c r="E183" s="17"/>
       <c r="F183" s="15"/>
@@ -4390,7 +4845,7 @@
     <row r="184" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A184" s="21"/>
       <c r="B184" s="20"/>
-      <c r="C184" s="23"/>
+      <c r="C184" s="29"/>
       <c r="D184" s="19"/>
       <c r="E184" s="17"/>
       <c r="F184" s="15"/>
@@ -4409,7 +4864,7 @@
     <row r="185" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A185" s="21"/>
       <c r="B185" s="20"/>
-      <c r="C185" s="23"/>
+      <c r="C185" s="29"/>
       <c r="D185" s="19"/>
       <c r="E185" s="17"/>
       <c r="F185" s="15"/>
@@ -4428,7 +4883,7 @@
     <row r="186" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A186" s="21"/>
       <c r="B186" s="20"/>
-      <c r="C186" s="23"/>
+      <c r="C186" s="29"/>
       <c r="D186" s="19"/>
       <c r="E186" s="17"/>
       <c r="F186" s="15"/>
@@ -4447,7 +4902,7 @@
     <row r="187" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A187" s="21"/>
       <c r="B187" s="20"/>
-      <c r="C187" s="23"/>
+      <c r="C187" s="29"/>
       <c r="D187" s="19"/>
       <c r="E187" s="17"/>
       <c r="F187" s="15"/>
@@ -4466,7 +4921,7 @@
     <row r="188" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A188" s="21"/>
       <c r="B188" s="20"/>
-      <c r="C188" s="23"/>
+      <c r="C188" s="29"/>
       <c r="D188" s="19"/>
       <c r="E188" s="17"/>
       <c r="F188" s="15"/>
@@ -4485,7 +4940,7 @@
     <row r="189" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A189" s="21"/>
       <c r="B189" s="20"/>
-      <c r="C189" s="23"/>
+      <c r="C189" s="29"/>
       <c r="D189" s="19"/>
       <c r="E189" s="17"/>
       <c r="F189" s="15"/>
@@ -4504,7 +4959,7 @@
     <row r="190" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A190" s="21"/>
       <c r="B190" s="20"/>
-      <c r="C190" s="23"/>
+      <c r="C190" s="29"/>
       <c r="D190" s="19"/>
       <c r="E190" s="17"/>
       <c r="F190" s="15"/>
@@ -4523,7 +4978,7 @@
     <row r="191" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A191" s="21"/>
       <c r="B191" s="20"/>
-      <c r="C191" s="23"/>
+      <c r="C191" s="29"/>
       <c r="D191" s="19"/>
       <c r="E191" s="17"/>
       <c r="F191" s="15"/>
@@ -4542,7 +4997,7 @@
     <row r="192" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A192" s="21"/>
       <c r="B192" s="20"/>
-      <c r="C192" s="23"/>
+      <c r="C192" s="29"/>
       <c r="D192" s="19"/>
       <c r="E192" s="17"/>
       <c r="F192" s="15"/>
@@ -4561,7 +5016,7 @@
     <row r="193" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A193" s="21"/>
       <c r="B193" s="20"/>
-      <c r="C193" s="23"/>
+      <c r="C193" s="29"/>
       <c r="D193" s="19"/>
       <c r="E193" s="17"/>
       <c r="F193" s="15"/>
@@ -4580,7 +5035,7 @@
     <row r="194" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A194" s="21"/>
       <c r="B194" s="20"/>
-      <c r="C194" s="23"/>
+      <c r="C194" s="29"/>
       <c r="D194" s="19"/>
       <c r="E194" s="17"/>
       <c r="F194" s="15"/>
@@ -4599,7 +5054,7 @@
     <row r="195" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A195" s="21"/>
       <c r="B195" s="20"/>
-      <c r="C195" s="23"/>
+      <c r="C195" s="29"/>
       <c r="D195" s="19"/>
       <c r="E195" s="17"/>
       <c r="F195" s="15"/>
@@ -4618,7 +5073,7 @@
     <row r="196" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A196" s="21"/>
       <c r="B196" s="20"/>
-      <c r="C196" s="23"/>
+      <c r="C196" s="29"/>
       <c r="D196" s="19"/>
       <c r="E196" s="17"/>
       <c r="F196" s="15"/>
@@ -4637,7 +5092,7 @@
     <row r="197" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A197" s="21"/>
       <c r="B197" s="20"/>
-      <c r="C197" s="23"/>
+      <c r="C197" s="29"/>
       <c r="D197" s="19"/>
       <c r="E197" s="17"/>
       <c r="F197" s="15"/>
@@ -4656,7 +5111,7 @@
     <row r="198" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A198" s="21"/>
       <c r="B198" s="20"/>
-      <c r="C198" s="23"/>
+      <c r="C198" s="29"/>
       <c r="D198" s="19"/>
       <c r="E198" s="17"/>
       <c r="F198" s="15"/>
@@ -4675,7 +5130,7 @@
     <row r="199" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A199" s="21"/>
       <c r="B199" s="20"/>
-      <c r="C199" s="23"/>
+      <c r="C199" s="29"/>
       <c r="D199" s="19"/>
       <c r="E199" s="17"/>
       <c r="F199" s="15"/>
@@ -4694,7 +5149,7 @@
     <row r="200" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A200" s="21"/>
       <c r="B200" s="20"/>
-      <c r="C200" s="23"/>
+      <c r="C200" s="29"/>
       <c r="D200" s="19"/>
       <c r="E200" s="17"/>
       <c r="F200" s="15"/>
@@ -4717,11 +5172,26 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2:I2" r:id="rId1" display=" Projects and Stuff LLC - http://ww.projectsandstuff.com"/>
+    <hyperlink ref="B6" r:id="rId2"/>
+    <hyperlink ref="B8" r:id="rId3"/>
+    <hyperlink ref="B7" r:id="rId4"/>
+    <hyperlink ref="B9" r:id="rId5"/>
+    <hyperlink ref="B10" r:id="rId6"/>
+    <hyperlink ref="B11" r:id="rId7"/>
+    <hyperlink ref="B13" r:id="rId8"/>
+    <hyperlink ref="B14" r:id="rId9"/>
+    <hyperlink ref="B16" r:id="rId10"/>
+    <hyperlink ref="B17" r:id="rId11"/>
+    <hyperlink ref="B18" r:id="rId12"/>
+    <hyperlink ref="B19" r:id="rId13"/>
+    <hyperlink ref="B20" r:id="rId14"/>
+    <hyperlink ref="B21" r:id="rId15"/>
+    <hyperlink ref="B22" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId17"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId18"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Updated Schematics with USB connector, and updated BOM and Project Log
</commit_message>
<xml_diff>
--- a/Notes/Chameleon BOM.xlsx
+++ b/Notes/Chameleon BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="91">
   <si>
     <t>Mfg Part #</t>
   </si>
@@ -81,42 +81,21 @@
     <t>Also available at Newark, Farnell, Avnet, Verical, etc</t>
   </si>
   <si>
-    <t>SRN3015-330M</t>
-  </si>
-  <si>
-    <t>Inductor 33uH</t>
-  </si>
-  <si>
-    <t>3mm x 3mm</t>
-  </si>
-  <si>
     <t>BAT750TA</t>
   </si>
   <si>
     <t>SOT-23-3</t>
   </si>
   <si>
-    <t>Used with Boost Regulator</t>
-  </si>
-  <si>
     <t>Used with Boost Regulator. Typical Forward Voltage = 290mV @ 250mA</t>
   </si>
   <si>
     <t>Diode Schottky 40V 750mA</t>
   </si>
   <si>
-    <t>3.5mm x 2.8mm</t>
-  </si>
-  <si>
     <t>Output Capacitor used with Boost Regulator</t>
   </si>
   <si>
-    <t>Capacitor Tantalum 47uF 10V 20%</t>
-  </si>
-  <si>
-    <t>TCJB476M010R0070</t>
-  </si>
-  <si>
     <t>Input Capacitor used with Boost Regulator</t>
   </si>
   <si>
@@ -162,12 +141,6 @@
     <t>Crystal 20 MHZ 8pF</t>
   </si>
   <si>
-    <t>NX3225SA-20.000000MHZ</t>
-  </si>
-  <si>
-    <t>1210</t>
-  </si>
-  <si>
     <t>DigiKey</t>
   </si>
   <si>
@@ -246,9 +219,6 @@
     <t>1207</t>
   </si>
   <si>
-    <t>AVR Analog Reference Filtering</t>
-  </si>
-  <si>
     <t>LED Red Diffused</t>
   </si>
   <si>
@@ -265,6 +235,63 @@
   </si>
   <si>
     <t>Used for Power Input/Output filtering and Decoupling</t>
+  </si>
+  <si>
+    <t>3.1 mm x 1.6 mm</t>
+  </si>
+  <si>
+    <t>RC1206JR-07220RL</t>
+  </si>
+  <si>
+    <t>Current Limiting for Ble &amp; Green LEDs (Any resistor around 150 Ohms and with the same package will do)</t>
+  </si>
+  <si>
+    <t>Current Limiting for Red LEDs (Any resistor around 220 Ohms and with the same package will do)</t>
+  </si>
+  <si>
+    <t>RMCF1206JT150R</t>
+  </si>
+  <si>
+    <t>Resistor 220Ω 1/4W 5%</t>
+  </si>
+  <si>
+    <t>Resistor 150Ω 1/4W 5%</t>
+  </si>
+  <si>
+    <t>Resistor 10kΩ 1/4W 5%</t>
+  </si>
+  <si>
+    <t>RC1206JR-0710KL</t>
+  </si>
+  <si>
+    <t>Pull-up resistors</t>
+  </si>
+  <si>
+    <t>USB - Micro B</t>
+  </si>
+  <si>
+    <t>Connector Receptical USB Micro B</t>
+  </si>
+  <si>
+    <t>ZX62-B-5PA(11)</t>
+  </si>
+  <si>
+    <t>USB Connector for charging</t>
+  </si>
+  <si>
+    <t>5.0 mm x 3.2 mm</t>
+  </si>
+  <si>
+    <t>NX5032GA-20.000000MHZ-LN-CD-1</t>
+  </si>
+  <si>
+    <t>JMK316BJ476ML-T</t>
+  </si>
+  <si>
+    <t>Capacitor Ceramic 47uF 6.3V 20%</t>
+  </si>
+  <si>
+    <t>Used with AVR Analog Reference Filtering and Boost Regulator</t>
   </si>
 </sst>
 </file>
@@ -416,7 +443,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -484,16 +511,20 @@
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -503,26 +534,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="15">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Lucida Sans Unicode"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -686,6 +697,26 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="9"/>
+        <color theme="1"/>
+        <name val="Lucida Sans Unicode"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
         <color theme="1" tint="0.14996795556505021"/>
         <name val="Lucida Sans Unicode"/>
         <scheme val="none"/>
@@ -787,19 +818,19 @@
   <tableColumns count="11">
     <tableColumn id="1" name="Description" dataDxfId="10"/>
     <tableColumn id="2" name="Mfg Part #" dataDxfId="9"/>
-    <tableColumn id="3" name="Package" dataDxfId="0"/>
-    <tableColumn id="5" name="Default Supplier" dataDxfId="8"/>
-    <tableColumn id="10" name="Supplier On Hand" dataDxfId="7"/>
-    <tableColumn id="4" name="Qty per board" dataDxfId="6"/>
-    <tableColumn id="6" name="Total Qty Needed" dataDxfId="5">
+    <tableColumn id="3" name="Package" dataDxfId="8"/>
+    <tableColumn id="5" name="Default Supplier" dataDxfId="7"/>
+    <tableColumn id="10" name="Supplier On Hand" dataDxfId="6"/>
+    <tableColumn id="4" name="Qty per board" dataDxfId="5"/>
+    <tableColumn id="6" name="Total Qty Needed" dataDxfId="4">
       <calculatedColumnFormula>SUM(Table4[[#This Row],[Qty per board]]*Goal)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Price per part at Qty" dataDxfId="4"/>
-    <tableColumn id="7" name="Total Price" dataDxfId="3">
+    <tableColumn id="11" name="Price per part at Qty" dataDxfId="3"/>
+    <tableColumn id="7" name="Total Price" dataDxfId="2">
       <calculatedColumnFormula>SUM(H6*G6)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Notes" dataDxfId="2"/>
-    <tableColumn id="9" name="Part References" dataDxfId="1"/>
+    <tableColumn id="8" name="Notes" dataDxfId="1"/>
+    <tableColumn id="9" name="Part References" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Projects and Stuff" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1095,14 +1126,14 @@
   <dimension ref="A1:K200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.28515625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" style="3" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" style="11" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
@@ -1115,17 +1146,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
       <c r="J1" s="8" t="s">
         <v>4</v>
       </c>
@@ -1134,17 +1165,17 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
     </row>
@@ -1167,7 +1198,7 @@
       </c>
       <c r="B4" s="14">
         <f>SUM(I6:I200)</f>
-        <v>4254.63</v>
+        <v>4761.579999999999</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -1221,7 +1252,7 @@
       <c r="B6" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="26" t="s">
         <v>17</v>
       </c>
       <c r="D6" s="19" t="s">
@@ -1249,21 +1280,21 @@
       </c>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="27" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B7" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="29" t="s">
-        <v>22</v>
+      <c r="C7" s="27" t="s">
+        <v>21</v>
       </c>
       <c r="D7" s="19" t="s">
         <v>18</v>
       </c>
       <c r="E7" s="17">
-        <v>3796</v>
+        <v>22159</v>
       </c>
       <c r="F7" s="15">
         <v>1</v>
@@ -1273,32 +1304,32 @@
         <v>1000</v>
       </c>
       <c r="H7" s="18">
-        <v>0.16</v>
+        <v>9.4759999999999997E-2</v>
       </c>
       <c r="I7" s="24">
         <f>SUM(H7*G7)</f>
-        <v>160</v>
+        <v>94.759999999999991</v>
       </c>
       <c r="J7" s="19" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K7" s="19"/>
     </row>
-    <row r="8" spans="1:11" ht="27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
-        <v>27</v>
+        <v>89</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>24</v>
+        <v>88</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>26</v>
       </c>
       <c r="D8" s="19" t="s">
         <v>18</v>
       </c>
       <c r="E8" s="17">
-        <v>22159</v>
+        <v>186142</v>
       </c>
       <c r="F8" s="15">
         <v>1</v>
@@ -1308,32 +1339,32 @@
         <v>1000</v>
       </c>
       <c r="H8" s="18">
-        <v>9.4759999999999997E-2</v>
+        <v>0.28799999999999998</v>
       </c>
       <c r="I8" s="24">
         <f>SUM(H8*G8)</f>
-        <v>94.759999999999991</v>
+        <v>288</v>
       </c>
       <c r="J8" s="19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K8" s="19"/>
     </row>
     <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>26</v>
       </c>
       <c r="D9" s="19" t="s">
         <v>18</v>
       </c>
       <c r="E9" s="17">
-        <v>39210</v>
+        <v>116496</v>
       </c>
       <c r="F9" s="15">
         <v>1</v>
@@ -1343,32 +1374,32 @@
         <v>1000</v>
       </c>
       <c r="H9" s="18">
-        <v>0.45100000000000001</v>
+        <v>3.8249999999999999E-2</v>
       </c>
       <c r="I9" s="24">
         <f t="shared" ref="I9:I69" si="0">SUM(H9*G9)</f>
-        <v>451</v>
+        <v>38.25</v>
       </c>
       <c r="J9" s="19" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="K9" s="19"/>
     </row>
     <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="29" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>32</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="E10" s="17">
-        <v>116496</v>
+        <v>1375</v>
       </c>
       <c r="F10" s="15">
         <v>1</v>
@@ -1378,33 +1409,31 @@
         <v>1000</v>
       </c>
       <c r="H10" s="18">
-        <v>3.8249999999999999E-2</v>
+        <v>0.95</v>
       </c>
       <c r="I10" s="24">
         <f t="shared" si="0"/>
-        <v>38.25</v>
+        <v>950</v>
       </c>
       <c r="J10" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K10" s="19"/>
     </row>
-    <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="54" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="17">
-        <v>1375</v>
-      </c>
+      <c r="E11" s="17"/>
       <c r="F11" s="15">
         <v>1</v>
       </c>
@@ -1413,31 +1442,33 @@
         <v>1000</v>
       </c>
       <c r="H11" s="18">
-        <v>0.95</v>
+        <v>1.66</v>
       </c>
       <c r="I11" s="24">
         <f t="shared" si="0"/>
-        <v>950</v>
+        <v>1660</v>
       </c>
       <c r="J11" s="19" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="K11" s="19"/>
     </row>
-    <row r="12" spans="1:11" ht="54" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="27" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="29" t="s">
-        <v>45</v>
+        <v>39</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>86</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="17"/>
+        <v>40</v>
+      </c>
+      <c r="E12" s="17">
+        <v>4000</v>
+      </c>
       <c r="F12" s="15">
         <v>1</v>
       </c>
@@ -1446,129 +1477,129 @@
         <v>1000</v>
       </c>
       <c r="H12" s="18">
-        <v>1.66</v>
+        <v>0.3024</v>
       </c>
       <c r="I12" s="24">
         <f t="shared" si="0"/>
-        <v>1660</v>
+        <v>302.39999999999998</v>
       </c>
       <c r="J12" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K12" s="19"/>
     </row>
     <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E13" s="17">
-        <v>9900</v>
+        <v>7417</v>
       </c>
       <c r="F13" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G13" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="H13" s="18">
-        <v>0.53761999999999999</v>
+        <v>1.6500000000000001E-2</v>
       </c>
       <c r="I13" s="24">
         <f t="shared" si="0"/>
-        <v>537.62</v>
+        <v>33</v>
       </c>
       <c r="J13" s="19" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="K13" s="19"/>
     </row>
     <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>51</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="B14" s="20"/>
       <c r="C14" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="E14" s="17">
-        <v>7417</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="D14" s="19"/>
+      <c r="E14" s="17"/>
       <c r="F14" s="15">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G14" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>2000</v>
-      </c>
-      <c r="H14" s="18">
-        <v>1.6500000000000001E-2</v>
-      </c>
+        <v>5000</v>
+      </c>
+      <c r="H14" s="18"/>
       <c r="I14" s="24">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="J14" s="19" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="K14" s="19"/>
     </row>
     <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="B15" s="20"/>
-      <c r="C15" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="D15" s="19"/>
-      <c r="E15" s="17"/>
+        <v>49</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="23">
+        <v>1206</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="17">
+        <v>151361</v>
+      </c>
       <c r="F15" s="15">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G15" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>5000</v>
-      </c>
-      <c r="H15" s="18"/>
+        <v>2000</v>
+      </c>
+      <c r="H15" s="18">
+        <v>4.47E-3</v>
+      </c>
       <c r="I15" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.94</v>
       </c>
       <c r="J15" s="19" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="K15" s="19"/>
     </row>
     <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" s="23">
-        <v>1206</v>
+        <v>53</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>54</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E16" s="17">
-        <v>195000</v>
+        <v>38808</v>
       </c>
       <c r="F16" s="15">
         <v>1</v>
@@ -1577,31 +1608,33 @@
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
         <v>1000</v>
       </c>
-      <c r="H16" s="18"/>
+      <c r="H16" s="18">
+        <v>4.47E-3</v>
+      </c>
       <c r="I16" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.47</v>
       </c>
       <c r="J16" s="19" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="K16" s="19"/>
     </row>
     <row r="17" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>63</v>
+        <v>57</v>
+      </c>
+      <c r="C17" s="23">
+        <v>1206</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E17" s="17">
-        <v>53903</v>
+        <v>55807</v>
       </c>
       <c r="F17" s="15">
         <v>1</v>
@@ -1610,97 +1643,103 @@
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
         <v>1000</v>
       </c>
-      <c r="H17" s="18"/>
+      <c r="H17" s="18">
+        <v>2.52E-2</v>
+      </c>
       <c r="I17" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>25.2</v>
       </c>
       <c r="J17" s="19" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="K17" s="19"/>
     </row>
     <row r="18" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="17">
+        <v>112229</v>
+      </c>
+      <c r="F18" s="15">
+        <v>2</v>
+      </c>
+      <c r="G18" s="25">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>2000</v>
+      </c>
+      <c r="H18" s="18">
+        <v>0.12870000000000001</v>
+      </c>
+      <c r="I18" s="24">
+        <f t="shared" si="0"/>
+        <v>257.40000000000003</v>
+      </c>
+      <c r="J18" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="K18" s="19"/>
+    </row>
+    <row r="19" spans="1:11" ht="27" x14ac:dyDescent="0.25">
+      <c r="A19" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="B18" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" s="23">
-        <v>1206</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="E18" s="17">
-        <v>56717</v>
-      </c>
-      <c r="F18" s="15">
-        <v>1</v>
-      </c>
-      <c r="G18" s="25">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>1000</v>
-      </c>
-      <c r="H18" s="18"/>
-      <c r="I18" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J18" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="K18" s="19"/>
-    </row>
-    <row r="19" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="C19" s="23" t="s">
-        <v>70</v>
-      </c>
       <c r="D19" s="19" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E19" s="17">
-        <v>88036</v>
+        <v>2440</v>
       </c>
       <c r="F19" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G19" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>1000</v>
-      </c>
-      <c r="H19" s="18"/>
+        <v>2000</v>
+      </c>
+      <c r="H19" s="18">
+        <v>6.9750000000000006E-2</v>
+      </c>
       <c r="I19" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>139.5</v>
       </c>
       <c r="J19" s="19" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="K19" s="19"/>
     </row>
     <row r="20" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E20" s="17">
-        <v>2440</v>
+        <v>586403</v>
       </c>
       <c r="F20" s="15">
         <v>1</v>
@@ -1709,141 +1748,197 @@
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
         <v>1000</v>
       </c>
-      <c r="H20" s="18"/>
+      <c r="H20" s="18">
+        <v>5.9799999999999999E-2</v>
+      </c>
       <c r="I20" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>59.8</v>
       </c>
       <c r="J20" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="K20" s="19"/>
+    </row>
+    <row r="21" spans="1:11" ht="27" x14ac:dyDescent="0.25">
+      <c r="A21" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="23">
+        <v>1206</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="17">
+        <v>310439</v>
+      </c>
+      <c r="F21" s="15">
+        <v>9</v>
+      </c>
+      <c r="G21" s="25">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>9000</v>
+      </c>
+      <c r="H21" s="18">
+        <v>1.4069999999999999E-2</v>
+      </c>
+      <c r="I21" s="24">
+        <f t="shared" si="0"/>
+        <v>126.63</v>
+      </c>
+      <c r="J21" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="K21" s="19"/>
+    </row>
+    <row r="22" spans="1:11" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="17">
+        <v>100000</v>
+      </c>
+      <c r="F22" s="15">
+        <v>6</v>
+      </c>
+      <c r="G22" s="25">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>6000</v>
+      </c>
+      <c r="H22" s="18">
+        <v>2.8300000000000001E-3</v>
+      </c>
+      <c r="I22" s="24">
+        <f t="shared" si="0"/>
+        <v>16.98</v>
+      </c>
+      <c r="J22" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="K20" s="19"/>
-    </row>
-    <row r="21" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="21" t="s">
+      <c r="K22" s="19"/>
+    </row>
+    <row r="23" spans="1:11" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="B21" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="C21" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="E21" s="17">
-        <v>586403</v>
-      </c>
-      <c r="F21" s="15">
+      <c r="C23" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" s="17">
+        <v>80000</v>
+      </c>
+      <c r="F23" s="15">
+        <v>10</v>
+      </c>
+      <c r="G23" s="25">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>10000</v>
+      </c>
+      <c r="H23" s="18">
+        <v>2.64E-3</v>
+      </c>
+      <c r="I23" s="24">
+        <f t="shared" si="0"/>
+        <v>26.4</v>
+      </c>
+      <c r="J23" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="K23" s="19"/>
+    </row>
+    <row r="24" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="17">
+        <v>1480000</v>
+      </c>
+      <c r="F24" s="15">
+        <v>5</v>
+      </c>
+      <c r="G24" s="25">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>5000</v>
+      </c>
+      <c r="H24" s="18">
+        <v>2.8300000000000001E-3</v>
+      </c>
+      <c r="I24" s="24">
+        <f t="shared" si="0"/>
+        <v>14.15</v>
+      </c>
+      <c r="J24" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="K24" s="19"/>
+    </row>
+    <row r="25" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" s="17">
+        <v>19970</v>
+      </c>
+      <c r="F25" s="15">
         <v>1</v>
       </c>
-      <c r="G21" s="25">
+      <c r="G25" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
         <v>1000</v>
       </c>
-      <c r="H21" s="18"/>
-      <c r="I21" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J21" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="K21" s="19"/>
-    </row>
-    <row r="22" spans="1:11" ht="27" x14ac:dyDescent="0.25">
-      <c r="A22" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="B22" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="C22" s="23">
-        <v>1206</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="E22" s="17">
-        <v>310439</v>
-      </c>
-      <c r="F22" s="15"/>
-      <c r="G22" s="25">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="H22" s="18"/>
-      <c r="I22" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J22" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="K22" s="19"/>
-    </row>
-    <row r="23" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="21"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="25">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="H23" s="18"/>
-      <c r="I23" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
-    </row>
-    <row r="24" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="25">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="H24" s="18"/>
-      <c r="I24" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19"/>
-    </row>
-    <row r="25" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="21"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="25">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="H25" s="18"/>
+      <c r="H25" s="18">
+        <v>0.38569999999999999</v>
+      </c>
       <c r="I25" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J25" s="19"/>
+        <v>385.7</v>
+      </c>
+      <c r="J25" s="19" t="s">
+        <v>85</v>
+      </c>
       <c r="K25" s="19"/>
     </row>
     <row r="26" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="21"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="29"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="27"/>
       <c r="D26" s="19"/>
       <c r="E26" s="17"/>
       <c r="F26" s="15"/>
@@ -1862,7 +1957,7 @@
     <row r="27" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="21"/>
       <c r="B27" s="20"/>
-      <c r="C27" s="29"/>
+      <c r="C27" s="27"/>
       <c r="D27" s="19"/>
       <c r="E27" s="17"/>
       <c r="F27" s="15"/>
@@ -1881,7 +1976,7 @@
     <row r="28" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="21"/>
       <c r="B28" s="20"/>
-      <c r="C28" s="29"/>
+      <c r="C28" s="27"/>
       <c r="D28" s="19"/>
       <c r="E28" s="17"/>
       <c r="F28" s="15"/>
@@ -1900,7 +1995,7 @@
     <row r="29" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="21"/>
       <c r="B29" s="20"/>
-      <c r="C29" s="29"/>
+      <c r="C29" s="27"/>
       <c r="D29" s="19"/>
       <c r="E29" s="17"/>
       <c r="F29" s="15"/>
@@ -1919,7 +2014,7 @@
     <row r="30" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="21"/>
       <c r="B30" s="20"/>
-      <c r="C30" s="29"/>
+      <c r="C30" s="27"/>
       <c r="D30" s="19"/>
       <c r="E30" s="17"/>
       <c r="F30" s="15"/>
@@ -1938,7 +2033,7 @@
     <row r="31" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="21"/>
       <c r="B31" s="20"/>
-      <c r="C31" s="29"/>
+      <c r="C31" s="27"/>
       <c r="D31" s="19"/>
       <c r="E31" s="17"/>
       <c r="F31" s="15"/>
@@ -1957,7 +2052,7 @@
     <row r="32" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="21"/>
       <c r="B32" s="20"/>
-      <c r="C32" s="29"/>
+      <c r="C32" s="27"/>
       <c r="D32" s="19"/>
       <c r="E32" s="17"/>
       <c r="F32" s="15"/>
@@ -1976,7 +2071,7 @@
     <row r="33" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="21"/>
       <c r="B33" s="20"/>
-      <c r="C33" s="29"/>
+      <c r="C33" s="27"/>
       <c r="D33" s="19"/>
       <c r="E33" s="17"/>
       <c r="F33" s="15"/>
@@ -1995,7 +2090,7 @@
     <row r="34" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="21"/>
       <c r="B34" s="20"/>
-      <c r="C34" s="29"/>
+      <c r="C34" s="27"/>
       <c r="D34" s="19"/>
       <c r="E34" s="17"/>
       <c r="F34" s="15"/>
@@ -2014,7 +2109,7 @@
     <row r="35" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="21"/>
       <c r="B35" s="20"/>
-      <c r="C35" s="29"/>
+      <c r="C35" s="27"/>
       <c r="D35" s="19"/>
       <c r="E35" s="17"/>
       <c r="F35" s="15"/>
@@ -2033,7 +2128,7 @@
     <row r="36" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="21"/>
       <c r="B36" s="20"/>
-      <c r="C36" s="29"/>
+      <c r="C36" s="27"/>
       <c r="D36" s="19"/>
       <c r="E36" s="17"/>
       <c r="F36" s="15"/>
@@ -2052,7 +2147,7 @@
     <row r="37" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="21"/>
       <c r="B37" s="20"/>
-      <c r="C37" s="29"/>
+      <c r="C37" s="27"/>
       <c r="D37" s="19"/>
       <c r="E37" s="17"/>
       <c r="F37" s="15"/>
@@ -2071,7 +2166,7 @@
     <row r="38" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="21"/>
       <c r="B38" s="20"/>
-      <c r="C38" s="29"/>
+      <c r="C38" s="27"/>
       <c r="D38" s="19"/>
       <c r="E38" s="17"/>
       <c r="F38" s="15"/>
@@ -2090,7 +2185,7 @@
     <row r="39" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="21"/>
       <c r="B39" s="20"/>
-      <c r="C39" s="29"/>
+      <c r="C39" s="27"/>
       <c r="D39" s="19"/>
       <c r="E39" s="17"/>
       <c r="F39" s="15"/>
@@ -2109,7 +2204,7 @@
     <row r="40" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="21"/>
       <c r="B40" s="20"/>
-      <c r="C40" s="29"/>
+      <c r="C40" s="27"/>
       <c r="D40" s="19"/>
       <c r="E40" s="17"/>
       <c r="F40" s="15"/>
@@ -2128,7 +2223,7 @@
     <row r="41" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="21"/>
       <c r="B41" s="20"/>
-      <c r="C41" s="29"/>
+      <c r="C41" s="27"/>
       <c r="D41" s="19"/>
       <c r="E41" s="17"/>
       <c r="F41" s="15"/>
@@ -2147,7 +2242,7 @@
     <row r="42" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="21"/>
       <c r="B42" s="20"/>
-      <c r="C42" s="29"/>
+      <c r="C42" s="27"/>
       <c r="D42" s="19"/>
       <c r="E42" s="17"/>
       <c r="F42" s="15"/>
@@ -2166,7 +2261,7 @@
     <row r="43" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="21"/>
       <c r="B43" s="20"/>
-      <c r="C43" s="29"/>
+      <c r="C43" s="27"/>
       <c r="D43" s="19"/>
       <c r="E43" s="17"/>
       <c r="F43" s="15"/>
@@ -2185,7 +2280,7 @@
     <row r="44" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="21"/>
       <c r="B44" s="20"/>
-      <c r="C44" s="29"/>
+      <c r="C44" s="27"/>
       <c r="D44" s="19"/>
       <c r="E44" s="17"/>
       <c r="F44" s="15"/>
@@ -2204,7 +2299,7 @@
     <row r="45" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="21"/>
       <c r="B45" s="20"/>
-      <c r="C45" s="29"/>
+      <c r="C45" s="27"/>
       <c r="D45" s="19"/>
       <c r="E45" s="17"/>
       <c r="F45" s="15"/>
@@ -2223,7 +2318,7 @@
     <row r="46" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="21"/>
       <c r="B46" s="20"/>
-      <c r="C46" s="29"/>
+      <c r="C46" s="27"/>
       <c r="D46" s="19"/>
       <c r="E46" s="17"/>
       <c r="F46" s="15"/>
@@ -2242,7 +2337,7 @@
     <row r="47" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="21"/>
       <c r="B47" s="20"/>
-      <c r="C47" s="29"/>
+      <c r="C47" s="27"/>
       <c r="D47" s="19"/>
       <c r="E47" s="17"/>
       <c r="F47" s="15"/>
@@ -2261,7 +2356,7 @@
     <row r="48" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="21"/>
       <c r="B48" s="20"/>
-      <c r="C48" s="29"/>
+      <c r="C48" s="27"/>
       <c r="D48" s="19"/>
       <c r="E48" s="17"/>
       <c r="F48" s="15"/>
@@ -2280,7 +2375,7 @@
     <row r="49" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="21"/>
       <c r="B49" s="20"/>
-      <c r="C49" s="29"/>
+      <c r="C49" s="27"/>
       <c r="D49" s="19"/>
       <c r="E49" s="17"/>
       <c r="F49" s="15"/>
@@ -2299,7 +2394,7 @@
     <row r="50" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="21"/>
       <c r="B50" s="20"/>
-      <c r="C50" s="29"/>
+      <c r="C50" s="27"/>
       <c r="D50" s="19"/>
       <c r="E50" s="17"/>
       <c r="F50" s="15"/>
@@ -2318,7 +2413,7 @@
     <row r="51" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="21"/>
       <c r="B51" s="20"/>
-      <c r="C51" s="29"/>
+      <c r="C51" s="27"/>
       <c r="D51" s="19"/>
       <c r="E51" s="17"/>
       <c r="F51" s="15"/>
@@ -2337,7 +2432,7 @@
     <row r="52" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="21"/>
       <c r="B52" s="20"/>
-      <c r="C52" s="29"/>
+      <c r="C52" s="27"/>
       <c r="D52" s="19"/>
       <c r="E52" s="17"/>
       <c r="F52" s="15"/>
@@ -2356,7 +2451,7 @@
     <row r="53" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="21"/>
       <c r="B53" s="20"/>
-      <c r="C53" s="29"/>
+      <c r="C53" s="27"/>
       <c r="D53" s="19"/>
       <c r="E53" s="17"/>
       <c r="F53" s="15"/>
@@ -2375,7 +2470,7 @@
     <row r="54" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="21"/>
       <c r="B54" s="20"/>
-      <c r="C54" s="29"/>
+      <c r="C54" s="27"/>
       <c r="D54" s="19"/>
       <c r="E54" s="17"/>
       <c r="F54" s="15"/>
@@ -2394,7 +2489,7 @@
     <row r="55" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="21"/>
       <c r="B55" s="20"/>
-      <c r="C55" s="29"/>
+      <c r="C55" s="27"/>
       <c r="D55" s="19"/>
       <c r="E55" s="17"/>
       <c r="F55" s="15"/>
@@ -2413,7 +2508,7 @@
     <row r="56" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="21"/>
       <c r="B56" s="20"/>
-      <c r="C56" s="29"/>
+      <c r="C56" s="27"/>
       <c r="D56" s="19"/>
       <c r="E56" s="17"/>
       <c r="F56" s="15"/>
@@ -2432,7 +2527,7 @@
     <row r="57" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="21"/>
       <c r="B57" s="20"/>
-      <c r="C57" s="29"/>
+      <c r="C57" s="27"/>
       <c r="D57" s="19"/>
       <c r="E57" s="17"/>
       <c r="F57" s="15"/>
@@ -2451,7 +2546,7 @@
     <row r="58" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="21"/>
       <c r="B58" s="20"/>
-      <c r="C58" s="29"/>
+      <c r="C58" s="27"/>
       <c r="D58" s="19"/>
       <c r="E58" s="17"/>
       <c r="F58" s="15"/>
@@ -2470,7 +2565,7 @@
     <row r="59" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="21"/>
       <c r="B59" s="20"/>
-      <c r="C59" s="29"/>
+      <c r="C59" s="27"/>
       <c r="D59" s="19"/>
       <c r="E59" s="17"/>
       <c r="F59" s="15"/>
@@ -2489,7 +2584,7 @@
     <row r="60" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="21"/>
       <c r="B60" s="20"/>
-      <c r="C60" s="29"/>
+      <c r="C60" s="27"/>
       <c r="D60" s="19"/>
       <c r="E60" s="17"/>
       <c r="F60" s="15"/>
@@ -2508,7 +2603,7 @@
     <row r="61" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="21"/>
       <c r="B61" s="20"/>
-      <c r="C61" s="29"/>
+      <c r="C61" s="27"/>
       <c r="D61" s="19"/>
       <c r="E61" s="17"/>
       <c r="F61" s="15"/>
@@ -2527,7 +2622,7 @@
     <row r="62" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="21"/>
       <c r="B62" s="20"/>
-      <c r="C62" s="29"/>
+      <c r="C62" s="27"/>
       <c r="D62" s="19"/>
       <c r="E62" s="17"/>
       <c r="F62" s="15"/>
@@ -2546,7 +2641,7 @@
     <row r="63" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="21"/>
       <c r="B63" s="20"/>
-      <c r="C63" s="29"/>
+      <c r="C63" s="27"/>
       <c r="D63" s="19"/>
       <c r="E63" s="17"/>
       <c r="F63" s="15"/>
@@ -2565,7 +2660,7 @@
     <row r="64" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="21"/>
       <c r="B64" s="20"/>
-      <c r="C64" s="29"/>
+      <c r="C64" s="27"/>
       <c r="D64" s="19"/>
       <c r="E64" s="17"/>
       <c r="F64" s="15"/>
@@ -2584,7 +2679,7 @@
     <row r="65" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="21"/>
       <c r="B65" s="20"/>
-      <c r="C65" s="29"/>
+      <c r="C65" s="27"/>
       <c r="D65" s="19"/>
       <c r="E65" s="17"/>
       <c r="F65" s="15"/>
@@ -2603,7 +2698,7 @@
     <row r="66" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="21"/>
       <c r="B66" s="20"/>
-      <c r="C66" s="29"/>
+      <c r="C66" s="27"/>
       <c r="D66" s="19"/>
       <c r="E66" s="17"/>
       <c r="F66" s="15"/>
@@ -2622,7 +2717,7 @@
     <row r="67" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="21"/>
       <c r="B67" s="20"/>
-      <c r="C67" s="29"/>
+      <c r="C67" s="27"/>
       <c r="D67" s="19"/>
       <c r="E67" s="17"/>
       <c r="F67" s="15"/>
@@ -2641,7 +2736,7 @@
     <row r="68" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="21"/>
       <c r="B68" s="20"/>
-      <c r="C68" s="29"/>
+      <c r="C68" s="27"/>
       <c r="D68" s="19"/>
       <c r="E68" s="17"/>
       <c r="F68" s="15"/>
@@ -2660,7 +2755,7 @@
     <row r="69" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="21"/>
       <c r="B69" s="20"/>
-      <c r="C69" s="29"/>
+      <c r="C69" s="27"/>
       <c r="D69" s="19"/>
       <c r="E69" s="17"/>
       <c r="F69" s="15"/>
@@ -2679,7 +2774,7 @@
     <row r="70" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="21"/>
       <c r="B70" s="20"/>
-      <c r="C70" s="29"/>
+      <c r="C70" s="27"/>
       <c r="D70" s="19"/>
       <c r="E70" s="17"/>
       <c r="F70" s="15"/>
@@ -2698,7 +2793,7 @@
     <row r="71" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="21"/>
       <c r="B71" s="20"/>
-      <c r="C71" s="29"/>
+      <c r="C71" s="27"/>
       <c r="D71" s="19"/>
       <c r="E71" s="17"/>
       <c r="F71" s="15"/>
@@ -2717,7 +2812,7 @@
     <row r="72" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="21"/>
       <c r="B72" s="20"/>
-      <c r="C72" s="29"/>
+      <c r="C72" s="27"/>
       <c r="D72" s="19"/>
       <c r="E72" s="17"/>
       <c r="F72" s="15"/>
@@ -2736,7 +2831,7 @@
     <row r="73" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="21"/>
       <c r="B73" s="20"/>
-      <c r="C73" s="29"/>
+      <c r="C73" s="27"/>
       <c r="D73" s="19"/>
       <c r="E73" s="17"/>
       <c r="F73" s="15"/>
@@ -2755,7 +2850,7 @@
     <row r="74" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="21"/>
       <c r="B74" s="20"/>
-      <c r="C74" s="29"/>
+      <c r="C74" s="27"/>
       <c r="D74" s="19"/>
       <c r="E74" s="17"/>
       <c r="F74" s="15"/>
@@ -2774,7 +2869,7 @@
     <row r="75" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="21"/>
       <c r="B75" s="20"/>
-      <c r="C75" s="29"/>
+      <c r="C75" s="27"/>
       <c r="D75" s="19"/>
       <c r="E75" s="17"/>
       <c r="F75" s="15"/>
@@ -2793,7 +2888,7 @@
     <row r="76" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="21"/>
       <c r="B76" s="20"/>
-      <c r="C76" s="29"/>
+      <c r="C76" s="27"/>
       <c r="D76" s="19"/>
       <c r="E76" s="17"/>
       <c r="F76" s="15"/>
@@ -2812,7 +2907,7 @@
     <row r="77" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="21"/>
       <c r="B77" s="20"/>
-      <c r="C77" s="29"/>
+      <c r="C77" s="27"/>
       <c r="D77" s="19"/>
       <c r="E77" s="17"/>
       <c r="F77" s="15"/>
@@ -2831,7 +2926,7 @@
     <row r="78" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="21"/>
       <c r="B78" s="20"/>
-      <c r="C78" s="29"/>
+      <c r="C78" s="27"/>
       <c r="D78" s="19"/>
       <c r="E78" s="17"/>
       <c r="F78" s="15"/>
@@ -2850,7 +2945,7 @@
     <row r="79" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="21"/>
       <c r="B79" s="20"/>
-      <c r="C79" s="29"/>
+      <c r="C79" s="27"/>
       <c r="D79" s="19"/>
       <c r="E79" s="17"/>
       <c r="F79" s="15"/>
@@ -2869,7 +2964,7 @@
     <row r="80" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="21"/>
       <c r="B80" s="20"/>
-      <c r="C80" s="29"/>
+      <c r="C80" s="27"/>
       <c r="D80" s="19"/>
       <c r="E80" s="17"/>
       <c r="F80" s="15"/>
@@ -2888,7 +2983,7 @@
     <row r="81" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="21"/>
       <c r="B81" s="20"/>
-      <c r="C81" s="29"/>
+      <c r="C81" s="27"/>
       <c r="D81" s="19"/>
       <c r="E81" s="17"/>
       <c r="F81" s="15"/>
@@ -2907,7 +3002,7 @@
     <row r="82" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="21"/>
       <c r="B82" s="20"/>
-      <c r="C82" s="29"/>
+      <c r="C82" s="27"/>
       <c r="D82" s="19"/>
       <c r="E82" s="17"/>
       <c r="F82" s="15"/>
@@ -2926,7 +3021,7 @@
     <row r="83" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="21"/>
       <c r="B83" s="20"/>
-      <c r="C83" s="29"/>
+      <c r="C83" s="27"/>
       <c r="D83" s="19"/>
       <c r="E83" s="17"/>
       <c r="F83" s="15"/>
@@ -2945,7 +3040,7 @@
     <row r="84" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="21"/>
       <c r="B84" s="20"/>
-      <c r="C84" s="29"/>
+      <c r="C84" s="27"/>
       <c r="D84" s="19"/>
       <c r="E84" s="17"/>
       <c r="F84" s="15"/>
@@ -2964,7 +3059,7 @@
     <row r="85" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="21"/>
       <c r="B85" s="20"/>
-      <c r="C85" s="29"/>
+      <c r="C85" s="27"/>
       <c r="D85" s="19"/>
       <c r="E85" s="17"/>
       <c r="F85" s="15"/>
@@ -2983,7 +3078,7 @@
     <row r="86" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="21"/>
       <c r="B86" s="20"/>
-      <c r="C86" s="29"/>
+      <c r="C86" s="27"/>
       <c r="D86" s="19"/>
       <c r="E86" s="17"/>
       <c r="F86" s="15"/>
@@ -3002,7 +3097,7 @@
     <row r="87" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="21"/>
       <c r="B87" s="20"/>
-      <c r="C87" s="29"/>
+      <c r="C87" s="27"/>
       <c r="D87" s="19"/>
       <c r="E87" s="17"/>
       <c r="F87" s="15"/>
@@ -3021,7 +3116,7 @@
     <row r="88" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="21"/>
       <c r="B88" s="20"/>
-      <c r="C88" s="29"/>
+      <c r="C88" s="27"/>
       <c r="D88" s="19"/>
       <c r="E88" s="17"/>
       <c r="F88" s="15"/>
@@ -3040,7 +3135,7 @@
     <row r="89" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="21"/>
       <c r="B89" s="20"/>
-      <c r="C89" s="29"/>
+      <c r="C89" s="27"/>
       <c r="D89" s="19"/>
       <c r="E89" s="17"/>
       <c r="F89" s="15"/>
@@ -3059,7 +3154,7 @@
     <row r="90" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="21"/>
       <c r="B90" s="20"/>
-      <c r="C90" s="29"/>
+      <c r="C90" s="27"/>
       <c r="D90" s="19"/>
       <c r="E90" s="17"/>
       <c r="F90" s="15"/>
@@ -3078,7 +3173,7 @@
     <row r="91" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="21"/>
       <c r="B91" s="20"/>
-      <c r="C91" s="29"/>
+      <c r="C91" s="27"/>
       <c r="D91" s="19"/>
       <c r="E91" s="17"/>
       <c r="F91" s="15"/>
@@ -3097,7 +3192,7 @@
     <row r="92" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="21"/>
       <c r="B92" s="20"/>
-      <c r="C92" s="29"/>
+      <c r="C92" s="27"/>
       <c r="D92" s="19"/>
       <c r="E92" s="17"/>
       <c r="F92" s="15"/>
@@ -3116,7 +3211,7 @@
     <row r="93" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="21"/>
       <c r="B93" s="20"/>
-      <c r="C93" s="29"/>
+      <c r="C93" s="27"/>
       <c r="D93" s="19"/>
       <c r="E93" s="17"/>
       <c r="F93" s="15"/>
@@ -3135,7 +3230,7 @@
     <row r="94" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="21"/>
       <c r="B94" s="20"/>
-      <c r="C94" s="29"/>
+      <c r="C94" s="27"/>
       <c r="D94" s="19"/>
       <c r="E94" s="17"/>
       <c r="F94" s="15"/>
@@ -3154,7 +3249,7 @@
     <row r="95" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="21"/>
       <c r="B95" s="20"/>
-      <c r="C95" s="29"/>
+      <c r="C95" s="27"/>
       <c r="D95" s="19"/>
       <c r="E95" s="17"/>
       <c r="F95" s="15"/>
@@ -3173,7 +3268,7 @@
     <row r="96" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="21"/>
       <c r="B96" s="20"/>
-      <c r="C96" s="29"/>
+      <c r="C96" s="27"/>
       <c r="D96" s="19"/>
       <c r="E96" s="17"/>
       <c r="F96" s="15"/>
@@ -3192,7 +3287,7 @@
     <row r="97" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="21"/>
       <c r="B97" s="20"/>
-      <c r="C97" s="29"/>
+      <c r="C97" s="27"/>
       <c r="D97" s="19"/>
       <c r="E97" s="17"/>
       <c r="F97" s="15"/>
@@ -3211,7 +3306,7 @@
     <row r="98" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="21"/>
       <c r="B98" s="20"/>
-      <c r="C98" s="29"/>
+      <c r="C98" s="27"/>
       <c r="D98" s="19"/>
       <c r="E98" s="17"/>
       <c r="F98" s="15"/>
@@ -3230,7 +3325,7 @@
     <row r="99" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="21"/>
       <c r="B99" s="20"/>
-      <c r="C99" s="29"/>
+      <c r="C99" s="27"/>
       <c r="D99" s="19"/>
       <c r="E99" s="17"/>
       <c r="F99" s="15"/>
@@ -3249,7 +3344,7 @@
     <row r="100" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="21"/>
       <c r="B100" s="20"/>
-      <c r="C100" s="29"/>
+      <c r="C100" s="27"/>
       <c r="D100" s="19"/>
       <c r="E100" s="17"/>
       <c r="F100" s="15"/>
@@ -3268,7 +3363,7 @@
     <row r="101" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" s="21"/>
       <c r="B101" s="20"/>
-      <c r="C101" s="29"/>
+      <c r="C101" s="27"/>
       <c r="D101" s="19"/>
       <c r="E101" s="17"/>
       <c r="F101" s="15"/>
@@ -3287,7 +3382,7 @@
     <row r="102" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" s="21"/>
       <c r="B102" s="20"/>
-      <c r="C102" s="29"/>
+      <c r="C102" s="27"/>
       <c r="D102" s="19"/>
       <c r="E102" s="17"/>
       <c r="F102" s="15"/>
@@ -3306,7 +3401,7 @@
     <row r="103" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A103" s="21"/>
       <c r="B103" s="20"/>
-      <c r="C103" s="29"/>
+      <c r="C103" s="27"/>
       <c r="D103" s="19"/>
       <c r="E103" s="17"/>
       <c r="F103" s="15"/>
@@ -3325,7 +3420,7 @@
     <row r="104" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A104" s="21"/>
       <c r="B104" s="20"/>
-      <c r="C104" s="29"/>
+      <c r="C104" s="27"/>
       <c r="D104" s="19"/>
       <c r="E104" s="17"/>
       <c r="F104" s="15"/>
@@ -3344,7 +3439,7 @@
     <row r="105" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A105" s="21"/>
       <c r="B105" s="20"/>
-      <c r="C105" s="29"/>
+      <c r="C105" s="27"/>
       <c r="D105" s="19"/>
       <c r="E105" s="17"/>
       <c r="F105" s="15"/>
@@ -3363,7 +3458,7 @@
     <row r="106" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A106" s="21"/>
       <c r="B106" s="20"/>
-      <c r="C106" s="29"/>
+      <c r="C106" s="27"/>
       <c r="D106" s="19"/>
       <c r="E106" s="17"/>
       <c r="F106" s="15"/>
@@ -3382,7 +3477,7 @@
     <row r="107" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A107" s="21"/>
       <c r="B107" s="20"/>
-      <c r="C107" s="29"/>
+      <c r="C107" s="27"/>
       <c r="D107" s="19"/>
       <c r="E107" s="17"/>
       <c r="F107" s="15"/>
@@ -3401,7 +3496,7 @@
     <row r="108" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A108" s="21"/>
       <c r="B108" s="20"/>
-      <c r="C108" s="29"/>
+      <c r="C108" s="27"/>
       <c r="D108" s="19"/>
       <c r="E108" s="17"/>
       <c r="F108" s="15"/>
@@ -3420,7 +3515,7 @@
     <row r="109" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A109" s="21"/>
       <c r="B109" s="20"/>
-      <c r="C109" s="29"/>
+      <c r="C109" s="27"/>
       <c r="D109" s="19"/>
       <c r="E109" s="17"/>
       <c r="F109" s="15"/>
@@ -3439,7 +3534,7 @@
     <row r="110" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A110" s="21"/>
       <c r="B110" s="20"/>
-      <c r="C110" s="29"/>
+      <c r="C110" s="27"/>
       <c r="D110" s="19"/>
       <c r="E110" s="17"/>
       <c r="F110" s="15"/>
@@ -3458,7 +3553,7 @@
     <row r="111" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A111" s="21"/>
       <c r="B111" s="20"/>
-      <c r="C111" s="29"/>
+      <c r="C111" s="27"/>
       <c r="D111" s="19"/>
       <c r="E111" s="17"/>
       <c r="F111" s="15"/>
@@ -3477,7 +3572,7 @@
     <row r="112" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A112" s="21"/>
       <c r="B112" s="20"/>
-      <c r="C112" s="29"/>
+      <c r="C112" s="27"/>
       <c r="D112" s="19"/>
       <c r="E112" s="17"/>
       <c r="F112" s="15"/>
@@ -3496,7 +3591,7 @@
     <row r="113" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A113" s="21"/>
       <c r="B113" s="20"/>
-      <c r="C113" s="29"/>
+      <c r="C113" s="27"/>
       <c r="D113" s="19"/>
       <c r="E113" s="17"/>
       <c r="F113" s="15"/>
@@ -3515,7 +3610,7 @@
     <row r="114" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A114" s="21"/>
       <c r="B114" s="20"/>
-      <c r="C114" s="29"/>
+      <c r="C114" s="27"/>
       <c r="D114" s="19"/>
       <c r="E114" s="17"/>
       <c r="F114" s="15"/>
@@ -3534,7 +3629,7 @@
     <row r="115" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A115" s="21"/>
       <c r="B115" s="20"/>
-      <c r="C115" s="29"/>
+      <c r="C115" s="27"/>
       <c r="D115" s="19"/>
       <c r="E115" s="17"/>
       <c r="F115" s="15"/>
@@ -3553,7 +3648,7 @@
     <row r="116" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A116" s="21"/>
       <c r="B116" s="20"/>
-      <c r="C116" s="29"/>
+      <c r="C116" s="27"/>
       <c r="D116" s="19"/>
       <c r="E116" s="17"/>
       <c r="F116" s="15"/>
@@ -3572,7 +3667,7 @@
     <row r="117" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A117" s="21"/>
       <c r="B117" s="20"/>
-      <c r="C117" s="29"/>
+      <c r="C117" s="27"/>
       <c r="D117" s="19"/>
       <c r="E117" s="17"/>
       <c r="F117" s="15"/>
@@ -3591,7 +3686,7 @@
     <row r="118" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A118" s="21"/>
       <c r="B118" s="20"/>
-      <c r="C118" s="29"/>
+      <c r="C118" s="27"/>
       <c r="D118" s="19"/>
       <c r="E118" s="17"/>
       <c r="F118" s="15"/>
@@ -3610,7 +3705,7 @@
     <row r="119" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A119" s="21"/>
       <c r="B119" s="20"/>
-      <c r="C119" s="29"/>
+      <c r="C119" s="27"/>
       <c r="D119" s="19"/>
       <c r="E119" s="17"/>
       <c r="F119" s="15"/>
@@ -3629,7 +3724,7 @@
     <row r="120" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A120" s="21"/>
       <c r="B120" s="20"/>
-      <c r="C120" s="29"/>
+      <c r="C120" s="27"/>
       <c r="D120" s="19"/>
       <c r="E120" s="17"/>
       <c r="F120" s="15"/>
@@ -3648,7 +3743,7 @@
     <row r="121" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A121" s="21"/>
       <c r="B121" s="20"/>
-      <c r="C121" s="29"/>
+      <c r="C121" s="27"/>
       <c r="D121" s="19"/>
       <c r="E121" s="17"/>
       <c r="F121" s="15"/>
@@ -3667,7 +3762,7 @@
     <row r="122" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A122" s="21"/>
       <c r="B122" s="20"/>
-      <c r="C122" s="29"/>
+      <c r="C122" s="27"/>
       <c r="D122" s="19"/>
       <c r="E122" s="17"/>
       <c r="F122" s="15"/>
@@ -3686,7 +3781,7 @@
     <row r="123" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A123" s="21"/>
       <c r="B123" s="20"/>
-      <c r="C123" s="29"/>
+      <c r="C123" s="27"/>
       <c r="D123" s="19"/>
       <c r="E123" s="17"/>
       <c r="F123" s="15"/>
@@ -3705,7 +3800,7 @@
     <row r="124" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A124" s="21"/>
       <c r="B124" s="20"/>
-      <c r="C124" s="29"/>
+      <c r="C124" s="27"/>
       <c r="D124" s="19"/>
       <c r="E124" s="17"/>
       <c r="F124" s="15"/>
@@ -3724,7 +3819,7 @@
     <row r="125" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A125" s="21"/>
       <c r="B125" s="20"/>
-      <c r="C125" s="29"/>
+      <c r="C125" s="27"/>
       <c r="D125" s="19"/>
       <c r="E125" s="17"/>
       <c r="F125" s="15"/>
@@ -3743,7 +3838,7 @@
     <row r="126" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A126" s="21"/>
       <c r="B126" s="20"/>
-      <c r="C126" s="29"/>
+      <c r="C126" s="27"/>
       <c r="D126" s="19"/>
       <c r="E126" s="17"/>
       <c r="F126" s="15"/>
@@ -3762,7 +3857,7 @@
     <row r="127" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A127" s="21"/>
       <c r="B127" s="20"/>
-      <c r="C127" s="29"/>
+      <c r="C127" s="27"/>
       <c r="D127" s="19"/>
       <c r="E127" s="17"/>
       <c r="F127" s="15"/>
@@ -3781,7 +3876,7 @@
     <row r="128" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A128" s="21"/>
       <c r="B128" s="20"/>
-      <c r="C128" s="29"/>
+      <c r="C128" s="27"/>
       <c r="D128" s="19"/>
       <c r="E128" s="17"/>
       <c r="F128" s="15"/>
@@ -3800,7 +3895,7 @@
     <row r="129" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A129" s="21"/>
       <c r="B129" s="20"/>
-      <c r="C129" s="29"/>
+      <c r="C129" s="27"/>
       <c r="D129" s="19"/>
       <c r="E129" s="17"/>
       <c r="F129" s="15"/>
@@ -3819,7 +3914,7 @@
     <row r="130" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A130" s="21"/>
       <c r="B130" s="20"/>
-      <c r="C130" s="29"/>
+      <c r="C130" s="27"/>
       <c r="D130" s="19"/>
       <c r="E130" s="17"/>
       <c r="F130" s="15"/>
@@ -3838,7 +3933,7 @@
     <row r="131" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A131" s="21"/>
       <c r="B131" s="20"/>
-      <c r="C131" s="29"/>
+      <c r="C131" s="27"/>
       <c r="D131" s="19"/>
       <c r="E131" s="17"/>
       <c r="F131" s="15"/>
@@ -3857,7 +3952,7 @@
     <row r="132" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A132" s="21"/>
       <c r="B132" s="20"/>
-      <c r="C132" s="29"/>
+      <c r="C132" s="27"/>
       <c r="D132" s="19"/>
       <c r="E132" s="17"/>
       <c r="F132" s="15"/>
@@ -3876,7 +3971,7 @@
     <row r="133" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A133" s="21"/>
       <c r="B133" s="20"/>
-      <c r="C133" s="29"/>
+      <c r="C133" s="27"/>
       <c r="D133" s="19"/>
       <c r="E133" s="17"/>
       <c r="F133" s="15"/>
@@ -3895,7 +3990,7 @@
     <row r="134" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A134" s="21"/>
       <c r="B134" s="20"/>
-      <c r="C134" s="29"/>
+      <c r="C134" s="27"/>
       <c r="D134" s="19"/>
       <c r="E134" s="17"/>
       <c r="F134" s="15"/>
@@ -3914,7 +4009,7 @@
     <row r="135" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A135" s="21"/>
       <c r="B135" s="20"/>
-      <c r="C135" s="29"/>
+      <c r="C135" s="27"/>
       <c r="D135" s="19"/>
       <c r="E135" s="17"/>
       <c r="F135" s="15"/>
@@ -3933,7 +4028,7 @@
     <row r="136" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A136" s="21"/>
       <c r="B136" s="20"/>
-      <c r="C136" s="29"/>
+      <c r="C136" s="27"/>
       <c r="D136" s="19"/>
       <c r="E136" s="17"/>
       <c r="F136" s="15"/>
@@ -3952,7 +4047,7 @@
     <row r="137" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A137" s="21"/>
       <c r="B137" s="20"/>
-      <c r="C137" s="29"/>
+      <c r="C137" s="27"/>
       <c r="D137" s="19"/>
       <c r="E137" s="17"/>
       <c r="F137" s="15"/>
@@ -3971,7 +4066,7 @@
     <row r="138" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A138" s="21"/>
       <c r="B138" s="20"/>
-      <c r="C138" s="29"/>
+      <c r="C138" s="27"/>
       <c r="D138" s="19"/>
       <c r="E138" s="17"/>
       <c r="F138" s="15"/>
@@ -3990,7 +4085,7 @@
     <row r="139" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A139" s="21"/>
       <c r="B139" s="20"/>
-      <c r="C139" s="29"/>
+      <c r="C139" s="27"/>
       <c r="D139" s="19"/>
       <c r="E139" s="17"/>
       <c r="F139" s="15"/>
@@ -4009,7 +4104,7 @@
     <row r="140" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A140" s="21"/>
       <c r="B140" s="20"/>
-      <c r="C140" s="29"/>
+      <c r="C140" s="27"/>
       <c r="D140" s="19"/>
       <c r="E140" s="17"/>
       <c r="F140" s="15"/>
@@ -4028,7 +4123,7 @@
     <row r="141" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A141" s="21"/>
       <c r="B141" s="20"/>
-      <c r="C141" s="29"/>
+      <c r="C141" s="27"/>
       <c r="D141" s="19"/>
       <c r="E141" s="17"/>
       <c r="F141" s="15"/>
@@ -4047,7 +4142,7 @@
     <row r="142" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A142" s="21"/>
       <c r="B142" s="20"/>
-      <c r="C142" s="29"/>
+      <c r="C142" s="27"/>
       <c r="D142" s="19"/>
       <c r="E142" s="17"/>
       <c r="F142" s="15"/>
@@ -4066,7 +4161,7 @@
     <row r="143" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A143" s="21"/>
       <c r="B143" s="20"/>
-      <c r="C143" s="29"/>
+      <c r="C143" s="27"/>
       <c r="D143" s="19"/>
       <c r="E143" s="17"/>
       <c r="F143" s="15"/>
@@ -4085,7 +4180,7 @@
     <row r="144" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A144" s="21"/>
       <c r="B144" s="20"/>
-      <c r="C144" s="29"/>
+      <c r="C144" s="27"/>
       <c r="D144" s="19"/>
       <c r="E144" s="17"/>
       <c r="F144" s="15"/>
@@ -4104,7 +4199,7 @@
     <row r="145" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A145" s="21"/>
       <c r="B145" s="20"/>
-      <c r="C145" s="29"/>
+      <c r="C145" s="27"/>
       <c r="D145" s="19"/>
       <c r="E145" s="17"/>
       <c r="F145" s="15"/>
@@ -4123,7 +4218,7 @@
     <row r="146" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A146" s="21"/>
       <c r="B146" s="20"/>
-      <c r="C146" s="29"/>
+      <c r="C146" s="27"/>
       <c r="D146" s="19"/>
       <c r="E146" s="17"/>
       <c r="F146" s="15"/>
@@ -4142,7 +4237,7 @@
     <row r="147" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A147" s="21"/>
       <c r="B147" s="20"/>
-      <c r="C147" s="29"/>
+      <c r="C147" s="27"/>
       <c r="D147" s="19"/>
       <c r="E147" s="17"/>
       <c r="F147" s="15"/>
@@ -4161,7 +4256,7 @@
     <row r="148" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A148" s="21"/>
       <c r="B148" s="20"/>
-      <c r="C148" s="29"/>
+      <c r="C148" s="27"/>
       <c r="D148" s="19"/>
       <c r="E148" s="17"/>
       <c r="F148" s="15"/>
@@ -4180,7 +4275,7 @@
     <row r="149" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A149" s="21"/>
       <c r="B149" s="20"/>
-      <c r="C149" s="29"/>
+      <c r="C149" s="27"/>
       <c r="D149" s="19"/>
       <c r="E149" s="17"/>
       <c r="F149" s="15"/>
@@ -4199,7 +4294,7 @@
     <row r="150" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A150" s="21"/>
       <c r="B150" s="20"/>
-      <c r="C150" s="29"/>
+      <c r="C150" s="27"/>
       <c r="D150" s="19"/>
       <c r="E150" s="17"/>
       <c r="F150" s="15"/>
@@ -4218,7 +4313,7 @@
     <row r="151" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A151" s="21"/>
       <c r="B151" s="20"/>
-      <c r="C151" s="29"/>
+      <c r="C151" s="27"/>
       <c r="D151" s="19"/>
       <c r="E151" s="17"/>
       <c r="F151" s="15"/>
@@ -4237,7 +4332,7 @@
     <row r="152" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A152" s="21"/>
       <c r="B152" s="20"/>
-      <c r="C152" s="29"/>
+      <c r="C152" s="27"/>
       <c r="D152" s="19"/>
       <c r="E152" s="17"/>
       <c r="F152" s="15"/>
@@ -4256,7 +4351,7 @@
     <row r="153" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A153" s="21"/>
       <c r="B153" s="20"/>
-      <c r="C153" s="29"/>
+      <c r="C153" s="27"/>
       <c r="D153" s="19"/>
       <c r="E153" s="17"/>
       <c r="F153" s="15"/>
@@ -4275,7 +4370,7 @@
     <row r="154" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A154" s="21"/>
       <c r="B154" s="20"/>
-      <c r="C154" s="29"/>
+      <c r="C154" s="27"/>
       <c r="D154" s="19"/>
       <c r="E154" s="17"/>
       <c r="F154" s="15"/>
@@ -4294,7 +4389,7 @@
     <row r="155" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A155" s="21"/>
       <c r="B155" s="20"/>
-      <c r="C155" s="29"/>
+      <c r="C155" s="27"/>
       <c r="D155" s="19"/>
       <c r="E155" s="17"/>
       <c r="F155" s="15"/>
@@ -4313,7 +4408,7 @@
     <row r="156" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A156" s="21"/>
       <c r="B156" s="20"/>
-      <c r="C156" s="29"/>
+      <c r="C156" s="27"/>
       <c r="D156" s="19"/>
       <c r="E156" s="17"/>
       <c r="F156" s="15"/>
@@ -4332,7 +4427,7 @@
     <row r="157" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A157" s="21"/>
       <c r="B157" s="20"/>
-      <c r="C157" s="29"/>
+      <c r="C157" s="27"/>
       <c r="D157" s="19"/>
       <c r="E157" s="17"/>
       <c r="F157" s="15"/>
@@ -4351,7 +4446,7 @@
     <row r="158" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A158" s="21"/>
       <c r="B158" s="20"/>
-      <c r="C158" s="29"/>
+      <c r="C158" s="27"/>
       <c r="D158" s="19"/>
       <c r="E158" s="17"/>
       <c r="F158" s="15"/>
@@ -4370,7 +4465,7 @@
     <row r="159" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A159" s="21"/>
       <c r="B159" s="20"/>
-      <c r="C159" s="29"/>
+      <c r="C159" s="27"/>
       <c r="D159" s="19"/>
       <c r="E159" s="17"/>
       <c r="F159" s="15"/>
@@ -4389,7 +4484,7 @@
     <row r="160" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A160" s="21"/>
       <c r="B160" s="20"/>
-      <c r="C160" s="29"/>
+      <c r="C160" s="27"/>
       <c r="D160" s="19"/>
       <c r="E160" s="17"/>
       <c r="F160" s="15"/>
@@ -4408,7 +4503,7 @@
     <row r="161" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A161" s="21"/>
       <c r="B161" s="20"/>
-      <c r="C161" s="29"/>
+      <c r="C161" s="27"/>
       <c r="D161" s="19"/>
       <c r="E161" s="17"/>
       <c r="F161" s="15"/>
@@ -4427,7 +4522,7 @@
     <row r="162" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A162" s="21"/>
       <c r="B162" s="20"/>
-      <c r="C162" s="29"/>
+      <c r="C162" s="27"/>
       <c r="D162" s="19"/>
       <c r="E162" s="17"/>
       <c r="F162" s="15"/>
@@ -4446,7 +4541,7 @@
     <row r="163" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A163" s="21"/>
       <c r="B163" s="20"/>
-      <c r="C163" s="29"/>
+      <c r="C163" s="27"/>
       <c r="D163" s="19"/>
       <c r="E163" s="17"/>
       <c r="F163" s="15"/>
@@ -4465,7 +4560,7 @@
     <row r="164" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A164" s="21"/>
       <c r="B164" s="20"/>
-      <c r="C164" s="29"/>
+      <c r="C164" s="27"/>
       <c r="D164" s="19"/>
       <c r="E164" s="17"/>
       <c r="F164" s="15"/>
@@ -4484,7 +4579,7 @@
     <row r="165" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A165" s="21"/>
       <c r="B165" s="20"/>
-      <c r="C165" s="29"/>
+      <c r="C165" s="27"/>
       <c r="D165" s="19"/>
       <c r="E165" s="17"/>
       <c r="F165" s="15"/>
@@ -4503,7 +4598,7 @@
     <row r="166" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A166" s="21"/>
       <c r="B166" s="20"/>
-      <c r="C166" s="29"/>
+      <c r="C166" s="27"/>
       <c r="D166" s="19"/>
       <c r="E166" s="17"/>
       <c r="F166" s="15"/>
@@ -4522,7 +4617,7 @@
     <row r="167" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A167" s="21"/>
       <c r="B167" s="20"/>
-      <c r="C167" s="29"/>
+      <c r="C167" s="27"/>
       <c r="D167" s="19"/>
       <c r="E167" s="17"/>
       <c r="F167" s="15"/>
@@ -4541,7 +4636,7 @@
     <row r="168" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A168" s="21"/>
       <c r="B168" s="20"/>
-      <c r="C168" s="29"/>
+      <c r="C168" s="27"/>
       <c r="D168" s="19"/>
       <c r="E168" s="17"/>
       <c r="F168" s="15"/>
@@ -4560,7 +4655,7 @@
     <row r="169" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A169" s="21"/>
       <c r="B169" s="20"/>
-      <c r="C169" s="29"/>
+      <c r="C169" s="27"/>
       <c r="D169" s="19"/>
       <c r="E169" s="17"/>
       <c r="F169" s="15"/>
@@ -4579,7 +4674,7 @@
     <row r="170" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A170" s="21"/>
       <c r="B170" s="20"/>
-      <c r="C170" s="29"/>
+      <c r="C170" s="27"/>
       <c r="D170" s="19"/>
       <c r="E170" s="17"/>
       <c r="F170" s="15"/>
@@ -4598,7 +4693,7 @@
     <row r="171" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A171" s="21"/>
       <c r="B171" s="20"/>
-      <c r="C171" s="29"/>
+      <c r="C171" s="27"/>
       <c r="D171" s="19"/>
       <c r="E171" s="17"/>
       <c r="F171" s="15"/>
@@ -4617,7 +4712,7 @@
     <row r="172" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A172" s="21"/>
       <c r="B172" s="20"/>
-      <c r="C172" s="29"/>
+      <c r="C172" s="27"/>
       <c r="D172" s="19"/>
       <c r="E172" s="17"/>
       <c r="F172" s="15"/>
@@ -4636,7 +4731,7 @@
     <row r="173" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A173" s="21"/>
       <c r="B173" s="20"/>
-      <c r="C173" s="29"/>
+      <c r="C173" s="27"/>
       <c r="D173" s="19"/>
       <c r="E173" s="17"/>
       <c r="F173" s="15"/>
@@ -4655,7 +4750,7 @@
     <row r="174" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A174" s="21"/>
       <c r="B174" s="20"/>
-      <c r="C174" s="29"/>
+      <c r="C174" s="27"/>
       <c r="D174" s="19"/>
       <c r="E174" s="17"/>
       <c r="F174" s="15"/>
@@ -4674,7 +4769,7 @@
     <row r="175" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A175" s="21"/>
       <c r="B175" s="20"/>
-      <c r="C175" s="29"/>
+      <c r="C175" s="27"/>
       <c r="D175" s="19"/>
       <c r="E175" s="17"/>
       <c r="F175" s="15"/>
@@ -4693,7 +4788,7 @@
     <row r="176" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A176" s="21"/>
       <c r="B176" s="20"/>
-      <c r="C176" s="29"/>
+      <c r="C176" s="27"/>
       <c r="D176" s="19"/>
       <c r="E176" s="17"/>
       <c r="F176" s="15"/>
@@ -4712,7 +4807,7 @@
     <row r="177" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A177" s="21"/>
       <c r="B177" s="20"/>
-      <c r="C177" s="29"/>
+      <c r="C177" s="27"/>
       <c r="D177" s="19"/>
       <c r="E177" s="17"/>
       <c r="F177" s="15"/>
@@ -4731,7 +4826,7 @@
     <row r="178" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A178" s="21"/>
       <c r="B178" s="20"/>
-      <c r="C178" s="29"/>
+      <c r="C178" s="27"/>
       <c r="D178" s="19"/>
       <c r="E178" s="17"/>
       <c r="F178" s="15"/>
@@ -4750,7 +4845,7 @@
     <row r="179" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A179" s="21"/>
       <c r="B179" s="20"/>
-      <c r="C179" s="29"/>
+      <c r="C179" s="27"/>
       <c r="D179" s="19"/>
       <c r="E179" s="17"/>
       <c r="F179" s="15"/>
@@ -4769,7 +4864,7 @@
     <row r="180" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A180" s="21"/>
       <c r="B180" s="20"/>
-      <c r="C180" s="29"/>
+      <c r="C180" s="27"/>
       <c r="D180" s="19"/>
       <c r="E180" s="17"/>
       <c r="F180" s="15"/>
@@ -4788,7 +4883,7 @@
     <row r="181" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A181" s="21"/>
       <c r="B181" s="20"/>
-      <c r="C181" s="29"/>
+      <c r="C181" s="27"/>
       <c r="D181" s="19"/>
       <c r="E181" s="17"/>
       <c r="F181" s="15"/>
@@ -4807,7 +4902,7 @@
     <row r="182" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A182" s="21"/>
       <c r="B182" s="20"/>
-      <c r="C182" s="29"/>
+      <c r="C182" s="27"/>
       <c r="D182" s="19"/>
       <c r="E182" s="17"/>
       <c r="F182" s="15"/>
@@ -4826,7 +4921,7 @@
     <row r="183" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A183" s="21"/>
       <c r="B183" s="20"/>
-      <c r="C183" s="29"/>
+      <c r="C183" s="27"/>
       <c r="D183" s="19"/>
       <c r="E183" s="17"/>
       <c r="F183" s="15"/>
@@ -4845,7 +4940,7 @@
     <row r="184" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A184" s="21"/>
       <c r="B184" s="20"/>
-      <c r="C184" s="29"/>
+      <c r="C184" s="27"/>
       <c r="D184" s="19"/>
       <c r="E184" s="17"/>
       <c r="F184" s="15"/>
@@ -4864,7 +4959,7 @@
     <row r="185" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A185" s="21"/>
       <c r="B185" s="20"/>
-      <c r="C185" s="29"/>
+      <c r="C185" s="27"/>
       <c r="D185" s="19"/>
       <c r="E185" s="17"/>
       <c r="F185" s="15"/>
@@ -4883,7 +4978,7 @@
     <row r="186" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A186" s="21"/>
       <c r="B186" s="20"/>
-      <c r="C186" s="29"/>
+      <c r="C186" s="27"/>
       <c r="D186" s="19"/>
       <c r="E186" s="17"/>
       <c r="F186" s="15"/>
@@ -4902,7 +4997,7 @@
     <row r="187" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A187" s="21"/>
       <c r="B187" s="20"/>
-      <c r="C187" s="29"/>
+      <c r="C187" s="27"/>
       <c r="D187" s="19"/>
       <c r="E187" s="17"/>
       <c r="F187" s="15"/>
@@ -4921,7 +5016,7 @@
     <row r="188" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A188" s="21"/>
       <c r="B188" s="20"/>
-      <c r="C188" s="29"/>
+      <c r="C188" s="27"/>
       <c r="D188" s="19"/>
       <c r="E188" s="17"/>
       <c r="F188" s="15"/>
@@ -4940,7 +5035,7 @@
     <row r="189" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A189" s="21"/>
       <c r="B189" s="20"/>
-      <c r="C189" s="29"/>
+      <c r="C189" s="27"/>
       <c r="D189" s="19"/>
       <c r="E189" s="17"/>
       <c r="F189" s="15"/>
@@ -4959,7 +5054,7 @@
     <row r="190" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A190" s="21"/>
       <c r="B190" s="20"/>
-      <c r="C190" s="29"/>
+      <c r="C190" s="27"/>
       <c r="D190" s="19"/>
       <c r="E190" s="17"/>
       <c r="F190" s="15"/>
@@ -4978,7 +5073,7 @@
     <row r="191" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A191" s="21"/>
       <c r="B191" s="20"/>
-      <c r="C191" s="29"/>
+      <c r="C191" s="27"/>
       <c r="D191" s="19"/>
       <c r="E191" s="17"/>
       <c r="F191" s="15"/>
@@ -4997,7 +5092,7 @@
     <row r="192" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A192" s="21"/>
       <c r="B192" s="20"/>
-      <c r="C192" s="29"/>
+      <c r="C192" s="27"/>
       <c r="D192" s="19"/>
       <c r="E192" s="17"/>
       <c r="F192" s="15"/>
@@ -5016,7 +5111,7 @@
     <row r="193" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A193" s="21"/>
       <c r="B193" s="20"/>
-      <c r="C193" s="29"/>
+      <c r="C193" s="27"/>
       <c r="D193" s="19"/>
       <c r="E193" s="17"/>
       <c r="F193" s="15"/>
@@ -5035,7 +5130,7 @@
     <row r="194" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A194" s="21"/>
       <c r="B194" s="20"/>
-      <c r="C194" s="29"/>
+      <c r="C194" s="27"/>
       <c r="D194" s="19"/>
       <c r="E194" s="17"/>
       <c r="F194" s="15"/>
@@ -5054,7 +5149,7 @@
     <row r="195" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A195" s="21"/>
       <c r="B195" s="20"/>
-      <c r="C195" s="29"/>
+      <c r="C195" s="27"/>
       <c r="D195" s="19"/>
       <c r="E195" s="17"/>
       <c r="F195" s="15"/>
@@ -5073,7 +5168,7 @@
     <row r="196" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A196" s="21"/>
       <c r="B196" s="20"/>
-      <c r="C196" s="29"/>
+      <c r="C196" s="27"/>
       <c r="D196" s="19"/>
       <c r="E196" s="17"/>
       <c r="F196" s="15"/>
@@ -5092,7 +5187,7 @@
     <row r="197" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A197" s="21"/>
       <c r="B197" s="20"/>
-      <c r="C197" s="29"/>
+      <c r="C197" s="27"/>
       <c r="D197" s="19"/>
       <c r="E197" s="17"/>
       <c r="F197" s="15"/>
@@ -5111,7 +5206,7 @@
     <row r="198" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A198" s="21"/>
       <c r="B198" s="20"/>
-      <c r="C198" s="29"/>
+      <c r="C198" s="27"/>
       <c r="D198" s="19"/>
       <c r="E198" s="17"/>
       <c r="F198" s="15"/>
@@ -5130,7 +5225,7 @@
     <row r="199" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A199" s="21"/>
       <c r="B199" s="20"/>
-      <c r="C199" s="29"/>
+      <c r="C199" s="27"/>
       <c r="D199" s="19"/>
       <c r="E199" s="17"/>
       <c r="F199" s="15"/>
@@ -5149,7 +5244,7 @@
     <row r="200" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A200" s="21"/>
       <c r="B200" s="20"/>
-      <c r="C200" s="29"/>
+      <c r="C200" s="27"/>
       <c r="D200" s="19"/>
       <c r="E200" s="17"/>
       <c r="F200" s="15"/>
@@ -5173,25 +5268,12 @@
   <hyperlinks>
     <hyperlink ref="A2:I2" r:id="rId1" display=" Projects and Stuff LLC - http://ww.projectsandstuff.com"/>
     <hyperlink ref="B6" r:id="rId2"/>
-    <hyperlink ref="B8" r:id="rId3"/>
-    <hyperlink ref="B7" r:id="rId4"/>
-    <hyperlink ref="B9" r:id="rId5"/>
-    <hyperlink ref="B10" r:id="rId6"/>
-    <hyperlink ref="B11" r:id="rId7"/>
-    <hyperlink ref="B13" r:id="rId8"/>
-    <hyperlink ref="B14" r:id="rId9"/>
-    <hyperlink ref="B16" r:id="rId10"/>
-    <hyperlink ref="B17" r:id="rId11"/>
-    <hyperlink ref="B18" r:id="rId12"/>
-    <hyperlink ref="B19" r:id="rId13"/>
-    <hyperlink ref="B20" r:id="rId14"/>
-    <hyperlink ref="B21" r:id="rId15"/>
-    <hyperlink ref="B22" r:id="rId16"/>
+    <hyperlink ref="B7" r:id="rId3" display="ZX62-B-5PA(11)"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId17"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
   <tableParts count="1">
-    <tablePart r:id="rId18"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Updated BOM with additional sheet for non-electronic parts
</commit_message>
<xml_diff>
--- a/Notes/Chameleon BOM.xlsx
+++ b/Notes/Chameleon BOM.xlsx
@@ -4,22 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24240" windowHeight="12075"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24240" windowHeight="12075" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Electronics" sheetId="1" r:id="rId1"/>
+    <sheet name="Other" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Goal">Sheet1!$K$1</definedName>
+    <definedName name="Goal" localSheetId="1">Other!$J$1</definedName>
+    <definedName name="Goal">Electronics!$K$1</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="121">
   <si>
     <t>Mfg Part #</t>
   </si>
@@ -63,9 +63,6 @@
     <t xml:space="preserve"> Projects and Stuff LLC - http://www.projectsandstuff.com</t>
   </si>
   <si>
-    <t>Bill of Materials - Chameleon Drink Coasters</t>
-  </si>
-  <si>
     <t>NCP1402SN50T1G</t>
   </si>
   <si>
@@ -367,6 +364,24 @@
   </si>
   <si>
     <t>5.0mm x 5.0mm</t>
+  </si>
+  <si>
+    <t>Bill of Materials - Chameleon Drink Coasters - Electronics</t>
+  </si>
+  <si>
+    <t>Bill of Materials - Chameleon Drink Coasters - Other</t>
+  </si>
+  <si>
+    <t>Indestructo Mailers</t>
+  </si>
+  <si>
+    <t>White or Kraft</t>
+  </si>
+  <si>
+    <t>ULINE</t>
+  </si>
+  <si>
+    <t>(Similar also available at http://www.packagingsupplies.com/White_Corrugated_Boxes__Mailers.html - they're cheaper, but may not be enough on hand)</t>
   </si>
 </sst>
 </file>
@@ -603,7 +618,231 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="27">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Lucida Sans Unicode"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Lucida Sans Unicode"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <name val="Lucida Sans Unicode"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Lucida Sans Unicode"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00000"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <name val="Lucida Sans Unicode"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Lucida Sans Unicode"/>
+        <scheme val="none"/>
+      </font>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Lucida Sans Unicode"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Lucida Sans Unicode"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1" tint="0.14996795556505021"/>
+        <name val="Lucida Sans Unicode"/>
+        <scheme val="none"/>
+      </font>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Lucida Sans Unicode"/>
+        <scheme val="none"/>
+      </font>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="Lucida Sans Unicode"/>
+        <scheme val="none"/>
+      </font>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Lucida Sans Unicode"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -870,8 +1109,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Projects and Stuff" pivot="0" count="2">
-      <tableStyleElement type="headerRow" dxfId="14"/>
-      <tableStyleElement type="secondRowStripe" dxfId="13"/>
+      <tableStyleElement type="headerRow" dxfId="26"/>
+      <tableStyleElement type="secondRowStripe" dxfId="25"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -883,21 +1122,44 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A5:K200" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A5:K200" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
   <autoFilter ref="A5:K200"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="Description" dataDxfId="10"/>
-    <tableColumn id="2" name="Mfg Part #" dataDxfId="9"/>
-    <tableColumn id="3" name="Package" dataDxfId="8"/>
+    <tableColumn id="1" name="Description" dataDxfId="22"/>
+    <tableColumn id="2" name="Mfg Part #" dataDxfId="21"/>
+    <tableColumn id="3" name="Package" dataDxfId="20"/>
+    <tableColumn id="5" name="Default Supplier" dataDxfId="19"/>
+    <tableColumn id="10" name="Supplier On Hand" dataDxfId="18"/>
+    <tableColumn id="4" name="Qty per board" dataDxfId="17"/>
+    <tableColumn id="6" name="Total Qty Needed" dataDxfId="16">
+      <calculatedColumnFormula>SUM(Table4[[#This Row],[Qty per board]]*Goal)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="11" name="Price per part at Qty" dataDxfId="15"/>
+    <tableColumn id="7" name="Total Price" dataDxfId="14">
+      <calculatedColumnFormula>SUM(H6*G6)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" name="Notes" dataDxfId="13"/>
+    <tableColumn id="9" name="Part References" dataDxfId="12"/>
+  </tableColumns>
+  <tableStyleInfo name="Projects and Stuff" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table42" displayName="Table42" ref="A5:J200" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A5:J200"/>
+  <tableColumns count="10">
+    <tableColumn id="1" name="Description" dataDxfId="9"/>
+    <tableColumn id="2" name="Mfg Part #" dataDxfId="8"/>
     <tableColumn id="5" name="Default Supplier" dataDxfId="7"/>
     <tableColumn id="10" name="Supplier On Hand" dataDxfId="6"/>
     <tableColumn id="4" name="Qty per board" dataDxfId="5"/>
     <tableColumn id="6" name="Total Qty Needed" dataDxfId="4">
-      <calculatedColumnFormula>SUM(Table4[[#This Row],[Qty per board]]*Goal)</calculatedColumnFormula>
+      <calculatedColumnFormula>SUM(Table42[[#This Row],[Qty per board]]*Goal)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="11" name="Price per part at Qty" dataDxfId="3"/>
     <tableColumn id="7" name="Total Price" dataDxfId="2">
-      <calculatedColumnFormula>SUM(H6*G6)</calculatedColumnFormula>
+      <calculatedColumnFormula>SUM(G6*F6)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" name="Notes" dataDxfId="1"/>
     <tableColumn id="9" name="Part References" dataDxfId="0"/>
@@ -1195,8 +1457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1217,7 +1479,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="28" t="s">
-        <v>14</v>
+        <v>115</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -1317,16 +1579,16 @@
     </row>
     <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="24" t="s">
+      <c r="D6" s="18" t="s">
         <v>17</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>18</v>
       </c>
       <c r="E6" s="16">
         <v>1335</v>
@@ -1346,24 +1608,24 @@
         <v>330</v>
       </c>
       <c r="J6" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="27" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="25" t="s">
-        <v>21</v>
-      </c>
       <c r="D7" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E7" s="16">
         <v>22159</v>
@@ -1383,24 +1645,24 @@
         <v>94.759999999999991</v>
       </c>
       <c r="J7" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E8" s="16">
         <v>186142</v>
@@ -1420,24 +1682,24 @@
         <v>288</v>
       </c>
       <c r="J8" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E9" s="16">
         <v>116496</v>
@@ -1457,24 +1719,24 @@
         <v>38.25</v>
       </c>
       <c r="J9" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="18" t="s">
         <v>29</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>30</v>
       </c>
       <c r="E10" s="16">
         <v>1375</v>
@@ -1494,24 +1756,24 @@
         <v>950</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="54" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="25" t="s">
-        <v>38</v>
-      </c>
       <c r="D11" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E11" s="16"/>
       <c r="F11" s="15">
@@ -1529,24 +1791,24 @@
         <v>1660</v>
       </c>
       <c r="J11" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="27" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="18" t="s">
         <v>39</v>
-      </c>
-      <c r="B12" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>40</v>
       </c>
       <c r="E12" s="16">
         <v>4000</v>
@@ -1566,24 +1828,24 @@
         <v>302.39999999999998</v>
       </c>
       <c r="J12" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B13" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="21" t="s">
-        <v>43</v>
-      </c>
       <c r="D13" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E13" s="16">
         <v>7417</v>
@@ -1603,19 +1865,19 @@
         <v>33</v>
       </c>
       <c r="J13" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" s="26"/>
       <c r="C14" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D14" s="18"/>
       <c r="E14" s="16"/>
@@ -1632,24 +1894,24 @@
         <v>0</v>
       </c>
       <c r="J14" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="26" t="s">
         <v>48</v>
-      </c>
-      <c r="B15" s="26" t="s">
-        <v>49</v>
       </c>
       <c r="C15" s="21">
         <v>1206</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E15" s="16">
         <v>151361</v>
@@ -1669,24 +1931,24 @@
         <v>8.94</v>
       </c>
       <c r="J15" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="26" t="s">
+      <c r="C16" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="21" t="s">
-        <v>53</v>
-      </c>
       <c r="D16" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E16" s="16">
         <v>38808</v>
@@ -1706,24 +1968,24 @@
         <v>4.47</v>
       </c>
       <c r="J16" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="26" t="s">
         <v>55</v>
-      </c>
-      <c r="B17" s="26" t="s">
-        <v>56</v>
       </c>
       <c r="C17" s="21">
         <v>1206</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E17" s="16">
         <v>55807</v>
@@ -1743,24 +2005,24 @@
         <v>25.2</v>
       </c>
       <c r="J17" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="C18" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="21" t="s">
-        <v>60</v>
-      </c>
       <c r="D18" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E18" s="16">
         <v>112229</v>
@@ -1780,24 +2042,24 @@
         <v>257.40000000000003</v>
       </c>
       <c r="J18" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="27" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="C19" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="21" t="s">
-        <v>63</v>
-      </c>
       <c r="D19" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E19" s="16">
         <v>2440</v>
@@ -1817,24 +2079,24 @@
         <v>139.5</v>
       </c>
       <c r="J19" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K19" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="B20" s="26" t="s">
-        <v>65</v>
-      </c>
       <c r="C20" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E20" s="16">
         <v>586403</v>
@@ -1854,24 +2116,24 @@
         <v>59.8</v>
       </c>
       <c r="J20" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="27" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="26" t="s">
         <v>66</v>
-      </c>
-      <c r="B21" s="26" t="s">
-        <v>67</v>
       </c>
       <c r="C21" s="21">
         <v>1206</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E21" s="16">
         <v>310439</v>
@@ -1891,24 +2153,24 @@
         <v>126.63</v>
       </c>
       <c r="J21" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E22" s="16">
         <v>100000</v>
@@ -1928,24 +2190,24 @@
         <v>16.98</v>
       </c>
       <c r="J22" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E23" s="16">
         <v>80000</v>
@@ -1965,24 +2227,24 @@
         <v>26.4</v>
       </c>
       <c r="J23" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="B24" s="26" t="s">
-        <v>77</v>
-      </c>
       <c r="C24" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E24" s="16">
         <v>1480000</v>
@@ -2002,24 +2264,24 @@
         <v>14.15</v>
       </c>
       <c r="J24" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B25" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="B25" s="26" t="s">
-        <v>81</v>
-      </c>
       <c r="C25" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E25" s="16">
         <v>19970</v>
@@ -2039,24 +2301,24 @@
         <v>385.7</v>
       </c>
       <c r="J25" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E26" s="16">
         <v>2735</v>
@@ -2076,10 +2338,10 @@
         <v>1590.68</v>
       </c>
       <c r="J26" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15" x14ac:dyDescent="0.25">
@@ -5425,24 +5687,3655 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J200"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="35.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="11" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="13" style="5" customWidth="1"/>
+    <col min="9" max="9" width="39.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.7109375" style="12" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="9">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+    </row>
+    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="14">
+        <f>SUM(H6:H200)</f>
+        <v>240</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+    </row>
+    <row r="5" spans="1:10" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="54" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" s="16"/>
+      <c r="E6" s="15">
+        <v>1</v>
+      </c>
+      <c r="F6" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>1000</v>
+      </c>
+      <c r="G6" s="17">
+        <v>0.24</v>
+      </c>
+      <c r="H6" s="22">
+        <f>SUM(G6*F6)</f>
+        <v>240</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="J6"/>
+    </row>
+    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="20"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="17"/>
+      <c r="H7" s="22">
+        <f>SUM(G7*F7)</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="18"/>
+      <c r="J7"/>
+    </row>
+    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="20"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="17"/>
+      <c r="H8" s="22">
+        <f>SUM(G8*F8)</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="18"/>
+      <c r="J8"/>
+    </row>
+    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="20"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="17"/>
+      <c r="H9" s="22">
+        <f t="shared" ref="H9:H72" si="0">SUM(G9*F9)</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="18"/>
+      <c r="J9"/>
+    </row>
+    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="20"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="17"/>
+      <c r="H10" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="18"/>
+      <c r="J10"/>
+    </row>
+    <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="20"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="17"/>
+      <c r="H11" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="18"/>
+      <c r="J11"/>
+    </row>
+    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="20"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="17"/>
+      <c r="H12" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="18"/>
+      <c r="J12"/>
+    </row>
+    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="20"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="17"/>
+      <c r="H13" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="18"/>
+      <c r="J13"/>
+    </row>
+    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="20"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="17"/>
+      <c r="H14" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="18"/>
+      <c r="J14"/>
+    </row>
+    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="20"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G15" s="17"/>
+      <c r="H15" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="18"/>
+      <c r="J15"/>
+    </row>
+    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="20"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="17"/>
+      <c r="H16" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="18"/>
+      <c r="J16"/>
+    </row>
+    <row r="17" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="20"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G17" s="17"/>
+      <c r="H17" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="18"/>
+      <c r="J17"/>
+    </row>
+    <row r="18" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="20"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="17"/>
+      <c r="H18" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="18"/>
+      <c r="J18"/>
+    </row>
+    <row r="19" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="20"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G19" s="17"/>
+      <c r="H19" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+    </row>
+    <row r="20" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="20"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G20" s="17"/>
+      <c r="H20" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="18"/>
+      <c r="J20"/>
+    </row>
+    <row r="21" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="20"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G21" s="17"/>
+      <c r="H21" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="18"/>
+      <c r="J21"/>
+    </row>
+    <row r="22" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="20"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G22" s="17"/>
+      <c r="H22" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="18"/>
+      <c r="J22"/>
+    </row>
+    <row r="23" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="20"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G23" s="17"/>
+      <c r="H23" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="18"/>
+      <c r="J23"/>
+    </row>
+    <row r="24" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="20"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G24" s="17"/>
+      <c r="H24" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="18"/>
+      <c r="J24"/>
+    </row>
+    <row r="25" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="20"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G25" s="17"/>
+      <c r="H25" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I25" s="18"/>
+      <c r="J25"/>
+    </row>
+    <row r="26" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="20"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G26" s="17"/>
+      <c r="H26" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I26" s="18"/>
+      <c r="J26"/>
+    </row>
+    <row r="27" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="20"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G27" s="17"/>
+      <c r="H27" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+    </row>
+    <row r="28" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="20"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G28" s="17"/>
+      <c r="H28" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+    </row>
+    <row r="29" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="20"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G29" s="17"/>
+      <c r="H29" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
+    </row>
+    <row r="30" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="20"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G30" s="17"/>
+      <c r="H30" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I30" s="18"/>
+      <c r="J30" s="18"/>
+    </row>
+    <row r="31" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="20"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G31" s="17"/>
+      <c r="H31" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
+    </row>
+    <row r="32" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="20"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G32" s="17"/>
+      <c r="H32" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+    </row>
+    <row r="33" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="20"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G33" s="17"/>
+      <c r="H33" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+    </row>
+    <row r="34" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="20"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G34" s="17"/>
+      <c r="H34" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
+    </row>
+    <row r="35" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="20"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G35" s="17"/>
+      <c r="H35" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I35" s="18"/>
+      <c r="J35" s="18"/>
+    </row>
+    <row r="36" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="20"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G36" s="17"/>
+      <c r="H36" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I36" s="18"/>
+      <c r="J36" s="18"/>
+    </row>
+    <row r="37" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="20"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G37" s="17"/>
+      <c r="H37" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I37" s="18"/>
+      <c r="J37" s="18"/>
+    </row>
+    <row r="38" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" s="20"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G38" s="17"/>
+      <c r="H38" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I38" s="18"/>
+      <c r="J38" s="18"/>
+    </row>
+    <row r="39" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" s="20"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G39" s="17"/>
+      <c r="H39" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I39" s="18"/>
+      <c r="J39" s="18"/>
+    </row>
+    <row r="40" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="20"/>
+      <c r="B40" s="19"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G40" s="17"/>
+      <c r="H40" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I40" s="18"/>
+      <c r="J40" s="18"/>
+    </row>
+    <row r="41" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="20"/>
+      <c r="B41" s="19"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G41" s="17"/>
+      <c r="H41" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I41" s="18"/>
+      <c r="J41" s="18"/>
+    </row>
+    <row r="42" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="20"/>
+      <c r="B42" s="19"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G42" s="17"/>
+      <c r="H42" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I42" s="18"/>
+      <c r="J42" s="18"/>
+    </row>
+    <row r="43" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="20"/>
+      <c r="B43" s="19"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G43" s="17"/>
+      <c r="H43" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I43" s="18"/>
+      <c r="J43" s="18"/>
+    </row>
+    <row r="44" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="20"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G44" s="17"/>
+      <c r="H44" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I44" s="18"/>
+      <c r="J44" s="18"/>
+    </row>
+    <row r="45" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45" s="20"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G45" s="17"/>
+      <c r="H45" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I45" s="18"/>
+      <c r="J45" s="18"/>
+    </row>
+    <row r="46" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46" s="20"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G46" s="17"/>
+      <c r="H46" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
+    </row>
+    <row r="47" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="20"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G47" s="17"/>
+      <c r="H47" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I47" s="18"/>
+      <c r="J47" s="18"/>
+    </row>
+    <row r="48" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="20"/>
+      <c r="B48" s="19"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="15"/>
+      <c r="F48" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G48" s="17"/>
+      <c r="H48" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I48" s="18"/>
+      <c r="J48" s="18"/>
+    </row>
+    <row r="49" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49" s="20"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="15"/>
+      <c r="F49" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G49" s="17"/>
+      <c r="H49" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I49" s="18"/>
+      <c r="J49" s="18"/>
+    </row>
+    <row r="50" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A50" s="20"/>
+      <c r="B50" s="19"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="16"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G50" s="17"/>
+      <c r="H50" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I50" s="18"/>
+      <c r="J50" s="18"/>
+    </row>
+    <row r="51" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A51" s="20"/>
+      <c r="B51" s="19"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="16"/>
+      <c r="E51" s="15"/>
+      <c r="F51" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G51" s="17"/>
+      <c r="H51" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I51" s="18"/>
+      <c r="J51" s="18"/>
+    </row>
+    <row r="52" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A52" s="20"/>
+      <c r="B52" s="19"/>
+      <c r="C52" s="18"/>
+      <c r="D52" s="16"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G52" s="17"/>
+      <c r="H52" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I52" s="18"/>
+      <c r="J52" s="18"/>
+    </row>
+    <row r="53" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53" s="20"/>
+      <c r="B53" s="19"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="16"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G53" s="17"/>
+      <c r="H53" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I53" s="18"/>
+      <c r="J53" s="18"/>
+    </row>
+    <row r="54" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A54" s="20"/>
+      <c r="B54" s="19"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="16"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G54" s="17"/>
+      <c r="H54" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I54" s="18"/>
+      <c r="J54" s="18"/>
+    </row>
+    <row r="55" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A55" s="20"/>
+      <c r="B55" s="19"/>
+      <c r="C55" s="18"/>
+      <c r="D55" s="16"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G55" s="17"/>
+      <c r="H55" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I55" s="18"/>
+      <c r="J55" s="18"/>
+    </row>
+    <row r="56" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A56" s="20"/>
+      <c r="B56" s="19"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G56" s="17"/>
+      <c r="H56" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I56" s="18"/>
+      <c r="J56" s="18"/>
+    </row>
+    <row r="57" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A57" s="20"/>
+      <c r="B57" s="19"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="16"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G57" s="17"/>
+      <c r="H57" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I57" s="18"/>
+      <c r="J57" s="18"/>
+    </row>
+    <row r="58" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A58" s="20"/>
+      <c r="B58" s="19"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="16"/>
+      <c r="E58" s="15"/>
+      <c r="F58" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G58" s="17"/>
+      <c r="H58" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I58" s="18"/>
+      <c r="J58" s="18"/>
+    </row>
+    <row r="59" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A59" s="20"/>
+      <c r="B59" s="19"/>
+      <c r="C59" s="18"/>
+      <c r="D59" s="16"/>
+      <c r="E59" s="15"/>
+      <c r="F59" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G59" s="17"/>
+      <c r="H59" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I59" s="18"/>
+      <c r="J59" s="18"/>
+    </row>
+    <row r="60" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A60" s="20"/>
+      <c r="B60" s="19"/>
+      <c r="C60" s="18"/>
+      <c r="D60" s="16"/>
+      <c r="E60" s="15"/>
+      <c r="F60" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G60" s="17"/>
+      <c r="H60" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I60" s="18"/>
+      <c r="J60" s="18"/>
+    </row>
+    <row r="61" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A61" s="20"/>
+      <c r="B61" s="19"/>
+      <c r="C61" s="18"/>
+      <c r="D61" s="16"/>
+      <c r="E61" s="15"/>
+      <c r="F61" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G61" s="17"/>
+      <c r="H61" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I61" s="18"/>
+      <c r="J61" s="18"/>
+    </row>
+    <row r="62" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A62" s="20"/>
+      <c r="B62" s="19"/>
+      <c r="C62" s="18"/>
+      <c r="D62" s="16"/>
+      <c r="E62" s="15"/>
+      <c r="F62" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G62" s="17"/>
+      <c r="H62" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I62" s="18"/>
+      <c r="J62" s="18"/>
+    </row>
+    <row r="63" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A63" s="20"/>
+      <c r="B63" s="19"/>
+      <c r="C63" s="18"/>
+      <c r="D63" s="16"/>
+      <c r="E63" s="15"/>
+      <c r="F63" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G63" s="17"/>
+      <c r="H63" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I63" s="18"/>
+      <c r="J63" s="18"/>
+    </row>
+    <row r="64" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A64" s="20"/>
+      <c r="B64" s="19"/>
+      <c r="C64" s="18"/>
+      <c r="D64" s="16"/>
+      <c r="E64" s="15"/>
+      <c r="F64" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G64" s="17"/>
+      <c r="H64" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I64" s="18"/>
+      <c r="J64" s="18"/>
+    </row>
+    <row r="65" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A65" s="20"/>
+      <c r="B65" s="19"/>
+      <c r="C65" s="18"/>
+      <c r="D65" s="16"/>
+      <c r="E65" s="15"/>
+      <c r="F65" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G65" s="17"/>
+      <c r="H65" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I65" s="18"/>
+      <c r="J65" s="18"/>
+    </row>
+    <row r="66" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A66" s="20"/>
+      <c r="B66" s="19"/>
+      <c r="C66" s="18"/>
+      <c r="D66" s="16"/>
+      <c r="E66" s="15"/>
+      <c r="F66" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G66" s="17"/>
+      <c r="H66" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I66" s="18"/>
+      <c r="J66" s="18"/>
+    </row>
+    <row r="67" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A67" s="20"/>
+      <c r="B67" s="19"/>
+      <c r="C67" s="18"/>
+      <c r="D67" s="16"/>
+      <c r="E67" s="15"/>
+      <c r="F67" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G67" s="17"/>
+      <c r="H67" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I67" s="18"/>
+      <c r="J67" s="18"/>
+    </row>
+    <row r="68" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A68" s="20"/>
+      <c r="B68" s="19"/>
+      <c r="C68" s="18"/>
+      <c r="D68" s="16"/>
+      <c r="E68" s="15"/>
+      <c r="F68" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G68" s="17"/>
+      <c r="H68" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I68" s="18"/>
+      <c r="J68" s="18"/>
+    </row>
+    <row r="69" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A69" s="20"/>
+      <c r="B69" s="19"/>
+      <c r="C69" s="18"/>
+      <c r="D69" s="16"/>
+      <c r="E69" s="15"/>
+      <c r="F69" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G69" s="17"/>
+      <c r="H69" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I69" s="18"/>
+      <c r="J69" s="18"/>
+    </row>
+    <row r="70" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A70" s="20"/>
+      <c r="B70" s="19"/>
+      <c r="C70" s="18"/>
+      <c r="D70" s="16"/>
+      <c r="E70" s="15"/>
+      <c r="F70" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G70" s="17"/>
+      <c r="H70" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I70" s="18"/>
+      <c r="J70" s="18"/>
+    </row>
+    <row r="71" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A71" s="20"/>
+      <c r="B71" s="19"/>
+      <c r="C71" s="18"/>
+      <c r="D71" s="16"/>
+      <c r="E71" s="15"/>
+      <c r="F71" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G71" s="17"/>
+      <c r="H71" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I71" s="18"/>
+      <c r="J71" s="18"/>
+    </row>
+    <row r="72" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A72" s="20"/>
+      <c r="B72" s="19"/>
+      <c r="C72" s="18"/>
+      <c r="D72" s="16"/>
+      <c r="E72" s="15"/>
+      <c r="F72" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G72" s="17"/>
+      <c r="H72" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I72" s="18"/>
+      <c r="J72" s="18"/>
+    </row>
+    <row r="73" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A73" s="20"/>
+      <c r="B73" s="19"/>
+      <c r="C73" s="18"/>
+      <c r="D73" s="16"/>
+      <c r="E73" s="15"/>
+      <c r="F73" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G73" s="17"/>
+      <c r="H73" s="22">
+        <f t="shared" ref="H73:H136" si="1">SUM(G73*F73)</f>
+        <v>0</v>
+      </c>
+      <c r="I73" s="18"/>
+      <c r="J73" s="18"/>
+    </row>
+    <row r="74" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A74" s="20"/>
+      <c r="B74" s="19"/>
+      <c r="C74" s="18"/>
+      <c r="D74" s="16"/>
+      <c r="E74" s="15"/>
+      <c r="F74" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G74" s="17"/>
+      <c r="H74" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I74" s="18"/>
+      <c r="J74" s="18"/>
+    </row>
+    <row r="75" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A75" s="20"/>
+      <c r="B75" s="19"/>
+      <c r="C75" s="18"/>
+      <c r="D75" s="16"/>
+      <c r="E75" s="15"/>
+      <c r="F75" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G75" s="17"/>
+      <c r="H75" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I75" s="18"/>
+      <c r="J75" s="18"/>
+    </row>
+    <row r="76" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A76" s="20"/>
+      <c r="B76" s="19"/>
+      <c r="C76" s="18"/>
+      <c r="D76" s="16"/>
+      <c r="E76" s="15"/>
+      <c r="F76" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G76" s="17"/>
+      <c r="H76" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I76" s="18"/>
+      <c r="J76" s="18"/>
+    </row>
+    <row r="77" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A77" s="20"/>
+      <c r="B77" s="19"/>
+      <c r="C77" s="18"/>
+      <c r="D77" s="16"/>
+      <c r="E77" s="15"/>
+      <c r="F77" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G77" s="17"/>
+      <c r="H77" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I77" s="18"/>
+      <c r="J77" s="18"/>
+    </row>
+    <row r="78" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A78" s="20"/>
+      <c r="B78" s="19"/>
+      <c r="C78" s="18"/>
+      <c r="D78" s="16"/>
+      <c r="E78" s="15"/>
+      <c r="F78" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G78" s="17"/>
+      <c r="H78" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I78" s="18"/>
+      <c r="J78" s="18"/>
+    </row>
+    <row r="79" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A79" s="20"/>
+      <c r="B79" s="19"/>
+      <c r="C79" s="18"/>
+      <c r="D79" s="16"/>
+      <c r="E79" s="15"/>
+      <c r="F79" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G79" s="17"/>
+      <c r="H79" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I79" s="18"/>
+      <c r="J79" s="18"/>
+    </row>
+    <row r="80" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A80" s="20"/>
+      <c r="B80" s="19"/>
+      <c r="C80" s="18"/>
+      <c r="D80" s="16"/>
+      <c r="E80" s="15"/>
+      <c r="F80" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G80" s="17"/>
+      <c r="H80" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I80" s="18"/>
+      <c r="J80" s="18"/>
+    </row>
+    <row r="81" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A81" s="20"/>
+      <c r="B81" s="19"/>
+      <c r="C81" s="18"/>
+      <c r="D81" s="16"/>
+      <c r="E81" s="15"/>
+      <c r="F81" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G81" s="17"/>
+      <c r="H81" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I81" s="18"/>
+      <c r="J81" s="18"/>
+    </row>
+    <row r="82" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A82" s="20"/>
+      <c r="B82" s="19"/>
+      <c r="C82" s="18"/>
+      <c r="D82" s="16"/>
+      <c r="E82" s="15"/>
+      <c r="F82" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G82" s="17"/>
+      <c r="H82" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I82" s="18"/>
+      <c r="J82" s="18"/>
+    </row>
+    <row r="83" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A83" s="20"/>
+      <c r="B83" s="19"/>
+      <c r="C83" s="18"/>
+      <c r="D83" s="16"/>
+      <c r="E83" s="15"/>
+      <c r="F83" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G83" s="17"/>
+      <c r="H83" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I83" s="18"/>
+      <c r="J83" s="18"/>
+    </row>
+    <row r="84" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A84" s="20"/>
+      <c r="B84" s="19"/>
+      <c r="C84" s="18"/>
+      <c r="D84" s="16"/>
+      <c r="E84" s="15"/>
+      <c r="F84" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G84" s="17"/>
+      <c r="H84" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I84" s="18"/>
+      <c r="J84" s="18"/>
+    </row>
+    <row r="85" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A85" s="20"/>
+      <c r="B85" s="19"/>
+      <c r="C85" s="18"/>
+      <c r="D85" s="16"/>
+      <c r="E85" s="15"/>
+      <c r="F85" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G85" s="17"/>
+      <c r="H85" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I85" s="18"/>
+      <c r="J85" s="18"/>
+    </row>
+    <row r="86" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A86" s="20"/>
+      <c r="B86" s="19"/>
+      <c r="C86" s="18"/>
+      <c r="D86" s="16"/>
+      <c r="E86" s="15"/>
+      <c r="F86" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G86" s="17"/>
+      <c r="H86" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I86" s="18"/>
+      <c r="J86" s="18"/>
+    </row>
+    <row r="87" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A87" s="20"/>
+      <c r="B87" s="19"/>
+      <c r="C87" s="18"/>
+      <c r="D87" s="16"/>
+      <c r="E87" s="15"/>
+      <c r="F87" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G87" s="17"/>
+      <c r="H87" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I87" s="18"/>
+      <c r="J87" s="18"/>
+    </row>
+    <row r="88" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A88" s="20"/>
+      <c r="B88" s="19"/>
+      <c r="C88" s="18"/>
+      <c r="D88" s="16"/>
+      <c r="E88" s="15"/>
+      <c r="F88" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G88" s="17"/>
+      <c r="H88" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I88" s="18"/>
+      <c r="J88" s="18"/>
+    </row>
+    <row r="89" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A89" s="20"/>
+      <c r="B89" s="19"/>
+      <c r="C89" s="18"/>
+      <c r="D89" s="16"/>
+      <c r="E89" s="15"/>
+      <c r="F89" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G89" s="17"/>
+      <c r="H89" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I89" s="18"/>
+      <c r="J89" s="18"/>
+    </row>
+    <row r="90" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A90" s="20"/>
+      <c r="B90" s="19"/>
+      <c r="C90" s="18"/>
+      <c r="D90" s="16"/>
+      <c r="E90" s="15"/>
+      <c r="F90" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G90" s="17"/>
+      <c r="H90" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I90" s="18"/>
+      <c r="J90" s="18"/>
+    </row>
+    <row r="91" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A91" s="20"/>
+      <c r="B91" s="19"/>
+      <c r="C91" s="18"/>
+      <c r="D91" s="16"/>
+      <c r="E91" s="15"/>
+      <c r="F91" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G91" s="17"/>
+      <c r="H91" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I91" s="18"/>
+      <c r="J91" s="18"/>
+    </row>
+    <row r="92" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A92" s="20"/>
+      <c r="B92" s="19"/>
+      <c r="C92" s="18"/>
+      <c r="D92" s="16"/>
+      <c r="E92" s="15"/>
+      <c r="F92" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G92" s="17"/>
+      <c r="H92" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I92" s="18"/>
+      <c r="J92" s="18"/>
+    </row>
+    <row r="93" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A93" s="20"/>
+      <c r="B93" s="19"/>
+      <c r="C93" s="18"/>
+      <c r="D93" s="16"/>
+      <c r="E93" s="15"/>
+      <c r="F93" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G93" s="17"/>
+      <c r="H93" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I93" s="18"/>
+      <c r="J93" s="18"/>
+    </row>
+    <row r="94" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A94" s="20"/>
+      <c r="B94" s="19"/>
+      <c r="C94" s="18"/>
+      <c r="D94" s="16"/>
+      <c r="E94" s="15"/>
+      <c r="F94" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G94" s="17"/>
+      <c r="H94" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I94" s="18"/>
+      <c r="J94" s="18"/>
+    </row>
+    <row r="95" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A95" s="20"/>
+      <c r="B95" s="19"/>
+      <c r="C95" s="18"/>
+      <c r="D95" s="16"/>
+      <c r="E95" s="15"/>
+      <c r="F95" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G95" s="17"/>
+      <c r="H95" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I95" s="18"/>
+      <c r="J95" s="18"/>
+    </row>
+    <row r="96" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A96" s="20"/>
+      <c r="B96" s="19"/>
+      <c r="C96" s="18"/>
+      <c r="D96" s="16"/>
+      <c r="E96" s="15"/>
+      <c r="F96" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G96" s="17"/>
+      <c r="H96" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I96" s="18"/>
+      <c r="J96" s="18"/>
+    </row>
+    <row r="97" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A97" s="20"/>
+      <c r="B97" s="19"/>
+      <c r="C97" s="18"/>
+      <c r="D97" s="16"/>
+      <c r="E97" s="15"/>
+      <c r="F97" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G97" s="17"/>
+      <c r="H97" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I97" s="18"/>
+      <c r="J97" s="18"/>
+    </row>
+    <row r="98" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A98" s="20"/>
+      <c r="B98" s="19"/>
+      <c r="C98" s="18"/>
+      <c r="D98" s="16"/>
+      <c r="E98" s="15"/>
+      <c r="F98" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G98" s="17"/>
+      <c r="H98" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I98" s="18"/>
+      <c r="J98" s="18"/>
+    </row>
+    <row r="99" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A99" s="20"/>
+      <c r="B99" s="19"/>
+      <c r="C99" s="18"/>
+      <c r="D99" s="16"/>
+      <c r="E99" s="15"/>
+      <c r="F99" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G99" s="17"/>
+      <c r="H99" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I99" s="18"/>
+      <c r="J99" s="18"/>
+    </row>
+    <row r="100" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A100" s="20"/>
+      <c r="B100" s="19"/>
+      <c r="C100" s="18"/>
+      <c r="D100" s="16"/>
+      <c r="E100" s="15"/>
+      <c r="F100" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G100" s="17"/>
+      <c r="H100" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I100" s="18"/>
+      <c r="J100" s="18"/>
+    </row>
+    <row r="101" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A101" s="20"/>
+      <c r="B101" s="19"/>
+      <c r="C101" s="18"/>
+      <c r="D101" s="16"/>
+      <c r="E101" s="15"/>
+      <c r="F101" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G101" s="17"/>
+      <c r="H101" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I101" s="18"/>
+      <c r="J101" s="18"/>
+    </row>
+    <row r="102" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A102" s="20"/>
+      <c r="B102" s="19"/>
+      <c r="C102" s="18"/>
+      <c r="D102" s="16"/>
+      <c r="E102" s="15"/>
+      <c r="F102" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G102" s="17"/>
+      <c r="H102" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I102" s="18"/>
+      <c r="J102" s="18"/>
+    </row>
+    <row r="103" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A103" s="20"/>
+      <c r="B103" s="19"/>
+      <c r="C103" s="18"/>
+      <c r="D103" s="16"/>
+      <c r="E103" s="15"/>
+      <c r="F103" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G103" s="17"/>
+      <c r="H103" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I103" s="18"/>
+      <c r="J103" s="18"/>
+    </row>
+    <row r="104" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A104" s="20"/>
+      <c r="B104" s="19"/>
+      <c r="C104" s="18"/>
+      <c r="D104" s="16"/>
+      <c r="E104" s="15"/>
+      <c r="F104" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G104" s="17"/>
+      <c r="H104" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I104" s="18"/>
+      <c r="J104" s="18"/>
+    </row>
+    <row r="105" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A105" s="20"/>
+      <c r="B105" s="19"/>
+      <c r="C105" s="18"/>
+      <c r="D105" s="16"/>
+      <c r="E105" s="15"/>
+      <c r="F105" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G105" s="17"/>
+      <c r="H105" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I105" s="18"/>
+      <c r="J105" s="18"/>
+    </row>
+    <row r="106" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A106" s="20"/>
+      <c r="B106" s="19"/>
+      <c r="C106" s="18"/>
+      <c r="D106" s="16"/>
+      <c r="E106" s="15"/>
+      <c r="F106" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G106" s="17"/>
+      <c r="H106" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I106" s="18"/>
+      <c r="J106" s="18"/>
+    </row>
+    <row r="107" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A107" s="20"/>
+      <c r="B107" s="19"/>
+      <c r="C107" s="18"/>
+      <c r="D107" s="16"/>
+      <c r="E107" s="15"/>
+      <c r="F107" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G107" s="17"/>
+      <c r="H107" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I107" s="18"/>
+      <c r="J107" s="18"/>
+    </row>
+    <row r="108" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A108" s="20"/>
+      <c r="B108" s="19"/>
+      <c r="C108" s="18"/>
+      <c r="D108" s="16"/>
+      <c r="E108" s="15"/>
+      <c r="F108" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G108" s="17"/>
+      <c r="H108" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I108" s="18"/>
+      <c r="J108" s="18"/>
+    </row>
+    <row r="109" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A109" s="20"/>
+      <c r="B109" s="19"/>
+      <c r="C109" s="18"/>
+      <c r="D109" s="16"/>
+      <c r="E109" s="15"/>
+      <c r="F109" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G109" s="17"/>
+      <c r="H109" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I109" s="18"/>
+      <c r="J109" s="18"/>
+    </row>
+    <row r="110" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A110" s="20"/>
+      <c r="B110" s="19"/>
+      <c r="C110" s="18"/>
+      <c r="D110" s="16"/>
+      <c r="E110" s="15"/>
+      <c r="F110" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G110" s="17"/>
+      <c r="H110" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I110" s="18"/>
+      <c r="J110" s="18"/>
+    </row>
+    <row r="111" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A111" s="20"/>
+      <c r="B111" s="19"/>
+      <c r="C111" s="18"/>
+      <c r="D111" s="16"/>
+      <c r="E111" s="15"/>
+      <c r="F111" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G111" s="17"/>
+      <c r="H111" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I111" s="18"/>
+      <c r="J111" s="18"/>
+    </row>
+    <row r="112" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A112" s="20"/>
+      <c r="B112" s="19"/>
+      <c r="C112" s="18"/>
+      <c r="D112" s="16"/>
+      <c r="E112" s="15"/>
+      <c r="F112" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G112" s="17"/>
+      <c r="H112" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I112" s="18"/>
+      <c r="J112" s="18"/>
+    </row>
+    <row r="113" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A113" s="20"/>
+      <c r="B113" s="19"/>
+      <c r="C113" s="18"/>
+      <c r="D113" s="16"/>
+      <c r="E113" s="15"/>
+      <c r="F113" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G113" s="17"/>
+      <c r="H113" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I113" s="18"/>
+      <c r="J113" s="18"/>
+    </row>
+    <row r="114" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A114" s="20"/>
+      <c r="B114" s="19"/>
+      <c r="C114" s="18"/>
+      <c r="D114" s="16"/>
+      <c r="E114" s="15"/>
+      <c r="F114" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G114" s="17"/>
+      <c r="H114" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I114" s="18"/>
+      <c r="J114" s="18"/>
+    </row>
+    <row r="115" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A115" s="20"/>
+      <c r="B115" s="19"/>
+      <c r="C115" s="18"/>
+      <c r="D115" s="16"/>
+      <c r="E115" s="15"/>
+      <c r="F115" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G115" s="17"/>
+      <c r="H115" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I115" s="18"/>
+      <c r="J115" s="18"/>
+    </row>
+    <row r="116" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A116" s="20"/>
+      <c r="B116" s="19"/>
+      <c r="C116" s="18"/>
+      <c r="D116" s="16"/>
+      <c r="E116" s="15"/>
+      <c r="F116" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G116" s="17"/>
+      <c r="H116" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I116" s="18"/>
+      <c r="J116" s="18"/>
+    </row>
+    <row r="117" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A117" s="20"/>
+      <c r="B117" s="19"/>
+      <c r="C117" s="18"/>
+      <c r="D117" s="16"/>
+      <c r="E117" s="15"/>
+      <c r="F117" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G117" s="17"/>
+      <c r="H117" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I117" s="18"/>
+      <c r="J117" s="18"/>
+    </row>
+    <row r="118" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A118" s="20"/>
+      <c r="B118" s="19"/>
+      <c r="C118" s="18"/>
+      <c r="D118" s="16"/>
+      <c r="E118" s="15"/>
+      <c r="F118" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G118" s="17"/>
+      <c r="H118" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I118" s="18"/>
+      <c r="J118" s="18"/>
+    </row>
+    <row r="119" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A119" s="20"/>
+      <c r="B119" s="19"/>
+      <c r="C119" s="18"/>
+      <c r="D119" s="16"/>
+      <c r="E119" s="15"/>
+      <c r="F119" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G119" s="17"/>
+      <c r="H119" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I119" s="18"/>
+      <c r="J119" s="18"/>
+    </row>
+    <row r="120" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A120" s="20"/>
+      <c r="B120" s="19"/>
+      <c r="C120" s="18"/>
+      <c r="D120" s="16"/>
+      <c r="E120" s="15"/>
+      <c r="F120" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G120" s="17"/>
+      <c r="H120" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I120" s="18"/>
+      <c r="J120" s="18"/>
+    </row>
+    <row r="121" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A121" s="20"/>
+      <c r="B121" s="19"/>
+      <c r="C121" s="18"/>
+      <c r="D121" s="16"/>
+      <c r="E121" s="15"/>
+      <c r="F121" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G121" s="17"/>
+      <c r="H121" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I121" s="18"/>
+      <c r="J121" s="18"/>
+    </row>
+    <row r="122" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A122" s="20"/>
+      <c r="B122" s="19"/>
+      <c r="C122" s="18"/>
+      <c r="D122" s="16"/>
+      <c r="E122" s="15"/>
+      <c r="F122" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G122" s="17"/>
+      <c r="H122" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I122" s="18"/>
+      <c r="J122" s="18"/>
+    </row>
+    <row r="123" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A123" s="20"/>
+      <c r="B123" s="19"/>
+      <c r="C123" s="18"/>
+      <c r="D123" s="16"/>
+      <c r="E123" s="15"/>
+      <c r="F123" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G123" s="17"/>
+      <c r="H123" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I123" s="18"/>
+      <c r="J123" s="18"/>
+    </row>
+    <row r="124" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A124" s="20"/>
+      <c r="B124" s="19"/>
+      <c r="C124" s="18"/>
+      <c r="D124" s="16"/>
+      <c r="E124" s="15"/>
+      <c r="F124" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G124" s="17"/>
+      <c r="H124" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I124" s="18"/>
+      <c r="J124" s="18"/>
+    </row>
+    <row r="125" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A125" s="20"/>
+      <c r="B125" s="19"/>
+      <c r="C125" s="18"/>
+      <c r="D125" s="16"/>
+      <c r="E125" s="15"/>
+      <c r="F125" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G125" s="17"/>
+      <c r="H125" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I125" s="18"/>
+      <c r="J125" s="18"/>
+    </row>
+    <row r="126" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A126" s="20"/>
+      <c r="B126" s="19"/>
+      <c r="C126" s="18"/>
+      <c r="D126" s="16"/>
+      <c r="E126" s="15"/>
+      <c r="F126" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G126" s="17"/>
+      <c r="H126" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I126" s="18"/>
+      <c r="J126" s="18"/>
+    </row>
+    <row r="127" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A127" s="20"/>
+      <c r="B127" s="19"/>
+      <c r="C127" s="18"/>
+      <c r="D127" s="16"/>
+      <c r="E127" s="15"/>
+      <c r="F127" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G127" s="17"/>
+      <c r="H127" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I127" s="18"/>
+      <c r="J127" s="18"/>
+    </row>
+    <row r="128" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A128" s="20"/>
+      <c r="B128" s="19"/>
+      <c r="C128" s="18"/>
+      <c r="D128" s="16"/>
+      <c r="E128" s="15"/>
+      <c r="F128" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G128" s="17"/>
+      <c r="H128" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I128" s="18"/>
+      <c r="J128" s="18"/>
+    </row>
+    <row r="129" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A129" s="20"/>
+      <c r="B129" s="19"/>
+      <c r="C129" s="18"/>
+      <c r="D129" s="16"/>
+      <c r="E129" s="15"/>
+      <c r="F129" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G129" s="17"/>
+      <c r="H129" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I129" s="18"/>
+      <c r="J129" s="18"/>
+    </row>
+    <row r="130" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A130" s="20"/>
+      <c r="B130" s="19"/>
+      <c r="C130" s="18"/>
+      <c r="D130" s="16"/>
+      <c r="E130" s="15"/>
+      <c r="F130" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G130" s="17"/>
+      <c r="H130" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I130" s="18"/>
+      <c r="J130" s="18"/>
+    </row>
+    <row r="131" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A131" s="20"/>
+      <c r="B131" s="19"/>
+      <c r="C131" s="18"/>
+      <c r="D131" s="16"/>
+      <c r="E131" s="15"/>
+      <c r="F131" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G131" s="17"/>
+      <c r="H131" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I131" s="18"/>
+      <c r="J131" s="18"/>
+    </row>
+    <row r="132" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A132" s="20"/>
+      <c r="B132" s="19"/>
+      <c r="C132" s="18"/>
+      <c r="D132" s="16"/>
+      <c r="E132" s="15"/>
+      <c r="F132" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G132" s="17"/>
+      <c r="H132" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I132" s="18"/>
+      <c r="J132" s="18"/>
+    </row>
+    <row r="133" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A133" s="20"/>
+      <c r="B133" s="19"/>
+      <c r="C133" s="18"/>
+      <c r="D133" s="16"/>
+      <c r="E133" s="15"/>
+      <c r="F133" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G133" s="17"/>
+      <c r="H133" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I133" s="18"/>
+      <c r="J133" s="18"/>
+    </row>
+    <row r="134" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A134" s="20"/>
+      <c r="B134" s="19"/>
+      <c r="C134" s="18"/>
+      <c r="D134" s="16"/>
+      <c r="E134" s="15"/>
+      <c r="F134" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G134" s="17"/>
+      <c r="H134" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I134" s="18"/>
+      <c r="J134" s="18"/>
+    </row>
+    <row r="135" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A135" s="20"/>
+      <c r="B135" s="19"/>
+      <c r="C135" s="18"/>
+      <c r="D135" s="16"/>
+      <c r="E135" s="15"/>
+      <c r="F135" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G135" s="17"/>
+      <c r="H135" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I135" s="18"/>
+      <c r="J135" s="18"/>
+    </row>
+    <row r="136" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A136" s="20"/>
+      <c r="B136" s="19"/>
+      <c r="C136" s="18"/>
+      <c r="D136" s="16"/>
+      <c r="E136" s="15"/>
+      <c r="F136" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G136" s="17"/>
+      <c r="H136" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I136" s="18"/>
+      <c r="J136" s="18"/>
+    </row>
+    <row r="137" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A137" s="20"/>
+      <c r="B137" s="19"/>
+      <c r="C137" s="18"/>
+      <c r="D137" s="16"/>
+      <c r="E137" s="15"/>
+      <c r="F137" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G137" s="17"/>
+      <c r="H137" s="22">
+        <f t="shared" ref="H137:H200" si="2">SUM(G137*F137)</f>
+        <v>0</v>
+      </c>
+      <c r="I137" s="18"/>
+      <c r="J137" s="18"/>
+    </row>
+    <row r="138" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A138" s="20"/>
+      <c r="B138" s="19"/>
+      <c r="C138" s="18"/>
+      <c r="D138" s="16"/>
+      <c r="E138" s="15"/>
+      <c r="F138" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G138" s="17"/>
+      <c r="H138" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I138" s="18"/>
+      <c r="J138" s="18"/>
+    </row>
+    <row r="139" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A139" s="20"/>
+      <c r="B139" s="19"/>
+      <c r="C139" s="18"/>
+      <c r="D139" s="16"/>
+      <c r="E139" s="15"/>
+      <c r="F139" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G139" s="17"/>
+      <c r="H139" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I139" s="18"/>
+      <c r="J139" s="18"/>
+    </row>
+    <row r="140" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A140" s="20"/>
+      <c r="B140" s="19"/>
+      <c r="C140" s="18"/>
+      <c r="D140" s="16"/>
+      <c r="E140" s="15"/>
+      <c r="F140" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G140" s="17"/>
+      <c r="H140" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I140" s="18"/>
+      <c r="J140" s="18"/>
+    </row>
+    <row r="141" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A141" s="20"/>
+      <c r="B141" s="19"/>
+      <c r="C141" s="18"/>
+      <c r="D141" s="16"/>
+      <c r="E141" s="15"/>
+      <c r="F141" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G141" s="17"/>
+      <c r="H141" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I141" s="18"/>
+      <c r="J141" s="18"/>
+    </row>
+    <row r="142" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A142" s="20"/>
+      <c r="B142" s="19"/>
+      <c r="C142" s="18"/>
+      <c r="D142" s="16"/>
+      <c r="E142" s="15"/>
+      <c r="F142" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G142" s="17"/>
+      <c r="H142" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I142" s="18"/>
+      <c r="J142" s="18"/>
+    </row>
+    <row r="143" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A143" s="20"/>
+      <c r="B143" s="19"/>
+      <c r="C143" s="18"/>
+      <c r="D143" s="16"/>
+      <c r="E143" s="15"/>
+      <c r="F143" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G143" s="17"/>
+      <c r="H143" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I143" s="18"/>
+      <c r="J143" s="18"/>
+    </row>
+    <row r="144" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A144" s="20"/>
+      <c r="B144" s="19"/>
+      <c r="C144" s="18"/>
+      <c r="D144" s="16"/>
+      <c r="E144" s="15"/>
+      <c r="F144" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G144" s="17"/>
+      <c r="H144" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I144" s="18"/>
+      <c r="J144" s="18"/>
+    </row>
+    <row r="145" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A145" s="20"/>
+      <c r="B145" s="19"/>
+      <c r="C145" s="18"/>
+      <c r="D145" s="16"/>
+      <c r="E145" s="15"/>
+      <c r="F145" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G145" s="17"/>
+      <c r="H145" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I145" s="18"/>
+      <c r="J145" s="18"/>
+    </row>
+    <row r="146" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A146" s="20"/>
+      <c r="B146" s="19"/>
+      <c r="C146" s="18"/>
+      <c r="D146" s="16"/>
+      <c r="E146" s="15"/>
+      <c r="F146" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G146" s="17"/>
+      <c r="H146" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I146" s="18"/>
+      <c r="J146" s="18"/>
+    </row>
+    <row r="147" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A147" s="20"/>
+      <c r="B147" s="19"/>
+      <c r="C147" s="18"/>
+      <c r="D147" s="16"/>
+      <c r="E147" s="15"/>
+      <c r="F147" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G147" s="17"/>
+      <c r="H147" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I147" s="18"/>
+      <c r="J147" s="18"/>
+    </row>
+    <row r="148" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A148" s="20"/>
+      <c r="B148" s="19"/>
+      <c r="C148" s="18"/>
+      <c r="D148" s="16"/>
+      <c r="E148" s="15"/>
+      <c r="F148" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G148" s="17"/>
+      <c r="H148" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I148" s="18"/>
+      <c r="J148" s="18"/>
+    </row>
+    <row r="149" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A149" s="20"/>
+      <c r="B149" s="19"/>
+      <c r="C149" s="18"/>
+      <c r="D149" s="16"/>
+      <c r="E149" s="15"/>
+      <c r="F149" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G149" s="17"/>
+      <c r="H149" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I149" s="18"/>
+      <c r="J149" s="18"/>
+    </row>
+    <row r="150" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A150" s="20"/>
+      <c r="B150" s="19"/>
+      <c r="C150" s="18"/>
+      <c r="D150" s="16"/>
+      <c r="E150" s="15"/>
+      <c r="F150" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G150" s="17"/>
+      <c r="H150" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I150" s="18"/>
+      <c r="J150" s="18"/>
+    </row>
+    <row r="151" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A151" s="20"/>
+      <c r="B151" s="19"/>
+      <c r="C151" s="18"/>
+      <c r="D151" s="16"/>
+      <c r="E151" s="15"/>
+      <c r="F151" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G151" s="17"/>
+      <c r="H151" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I151" s="18"/>
+      <c r="J151" s="18"/>
+    </row>
+    <row r="152" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A152" s="20"/>
+      <c r="B152" s="19"/>
+      <c r="C152" s="18"/>
+      <c r="D152" s="16"/>
+      <c r="E152" s="15"/>
+      <c r="F152" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G152" s="17"/>
+      <c r="H152" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I152" s="18"/>
+      <c r="J152" s="18"/>
+    </row>
+    <row r="153" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A153" s="20"/>
+      <c r="B153" s="19"/>
+      <c r="C153" s="18"/>
+      <c r="D153" s="16"/>
+      <c r="E153" s="15"/>
+      <c r="F153" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G153" s="17"/>
+      <c r="H153" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I153" s="18"/>
+      <c r="J153" s="18"/>
+    </row>
+    <row r="154" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A154" s="20"/>
+      <c r="B154" s="19"/>
+      <c r="C154" s="18"/>
+      <c r="D154" s="16"/>
+      <c r="E154" s="15"/>
+      <c r="F154" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G154" s="17"/>
+      <c r="H154" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I154" s="18"/>
+      <c r="J154" s="18"/>
+    </row>
+    <row r="155" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A155" s="20"/>
+      <c r="B155" s="19"/>
+      <c r="C155" s="18"/>
+      <c r="D155" s="16"/>
+      <c r="E155" s="15"/>
+      <c r="F155" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G155" s="17"/>
+      <c r="H155" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I155" s="18"/>
+      <c r="J155" s="18"/>
+    </row>
+    <row r="156" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A156" s="20"/>
+      <c r="B156" s="19"/>
+      <c r="C156" s="18"/>
+      <c r="D156" s="16"/>
+      <c r="E156" s="15"/>
+      <c r="F156" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G156" s="17"/>
+      <c r="H156" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I156" s="18"/>
+      <c r="J156" s="18"/>
+    </row>
+    <row r="157" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A157" s="20"/>
+      <c r="B157" s="19"/>
+      <c r="C157" s="18"/>
+      <c r="D157" s="16"/>
+      <c r="E157" s="15"/>
+      <c r="F157" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G157" s="17"/>
+      <c r="H157" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I157" s="18"/>
+      <c r="J157" s="18"/>
+    </row>
+    <row r="158" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A158" s="20"/>
+      <c r="B158" s="19"/>
+      <c r="C158" s="18"/>
+      <c r="D158" s="16"/>
+      <c r="E158" s="15"/>
+      <c r="F158" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G158" s="17"/>
+      <c r="H158" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I158" s="18"/>
+      <c r="J158" s="18"/>
+    </row>
+    <row r="159" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A159" s="20"/>
+      <c r="B159" s="19"/>
+      <c r="C159" s="18"/>
+      <c r="D159" s="16"/>
+      <c r="E159" s="15"/>
+      <c r="F159" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G159" s="17"/>
+      <c r="H159" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I159" s="18"/>
+      <c r="J159" s="18"/>
+    </row>
+    <row r="160" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A160" s="20"/>
+      <c r="B160" s="19"/>
+      <c r="C160" s="18"/>
+      <c r="D160" s="16"/>
+      <c r="E160" s="15"/>
+      <c r="F160" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G160" s="17"/>
+      <c r="H160" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I160" s="18"/>
+      <c r="J160" s="18"/>
+    </row>
+    <row r="161" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A161" s="20"/>
+      <c r="B161" s="19"/>
+      <c r="C161" s="18"/>
+      <c r="D161" s="16"/>
+      <c r="E161" s="15"/>
+      <c r="F161" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G161" s="17"/>
+      <c r="H161" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I161" s="18"/>
+      <c r="J161" s="18"/>
+    </row>
+    <row r="162" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A162" s="20"/>
+      <c r="B162" s="19"/>
+      <c r="C162" s="18"/>
+      <c r="D162" s="16"/>
+      <c r="E162" s="15"/>
+      <c r="F162" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G162" s="17"/>
+      <c r="H162" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I162" s="18"/>
+      <c r="J162" s="18"/>
+    </row>
+    <row r="163" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A163" s="20"/>
+      <c r="B163" s="19"/>
+      <c r="C163" s="18"/>
+      <c r="D163" s="16"/>
+      <c r="E163" s="15"/>
+      <c r="F163" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G163" s="17"/>
+      <c r="H163" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I163" s="18"/>
+      <c r="J163" s="18"/>
+    </row>
+    <row r="164" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A164" s="20"/>
+      <c r="B164" s="19"/>
+      <c r="C164" s="18"/>
+      <c r="D164" s="16"/>
+      <c r="E164" s="15"/>
+      <c r="F164" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G164" s="17"/>
+      <c r="H164" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I164" s="18"/>
+      <c r="J164" s="18"/>
+    </row>
+    <row r="165" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A165" s="20"/>
+      <c r="B165" s="19"/>
+      <c r="C165" s="18"/>
+      <c r="D165" s="16"/>
+      <c r="E165" s="15"/>
+      <c r="F165" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G165" s="17"/>
+      <c r="H165" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I165" s="18"/>
+      <c r="J165" s="18"/>
+    </row>
+    <row r="166" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A166" s="20"/>
+      <c r="B166" s="19"/>
+      <c r="C166" s="18"/>
+      <c r="D166" s="16"/>
+      <c r="E166" s="15"/>
+      <c r="F166" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G166" s="17"/>
+      <c r="H166" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I166" s="18"/>
+      <c r="J166" s="18"/>
+    </row>
+    <row r="167" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A167" s="20"/>
+      <c r="B167" s="19"/>
+      <c r="C167" s="18"/>
+      <c r="D167" s="16"/>
+      <c r="E167" s="15"/>
+      <c r="F167" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G167" s="17"/>
+      <c r="H167" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I167" s="18"/>
+      <c r="J167" s="18"/>
+    </row>
+    <row r="168" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A168" s="20"/>
+      <c r="B168" s="19"/>
+      <c r="C168" s="18"/>
+      <c r="D168" s="16"/>
+      <c r="E168" s="15"/>
+      <c r="F168" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G168" s="17"/>
+      <c r="H168" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I168" s="18"/>
+      <c r="J168" s="18"/>
+    </row>
+    <row r="169" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A169" s="20"/>
+      <c r="B169" s="19"/>
+      <c r="C169" s="18"/>
+      <c r="D169" s="16"/>
+      <c r="E169" s="15"/>
+      <c r="F169" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G169" s="17"/>
+      <c r="H169" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I169" s="18"/>
+      <c r="J169" s="18"/>
+    </row>
+    <row r="170" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A170" s="20"/>
+      <c r="B170" s="19"/>
+      <c r="C170" s="18"/>
+      <c r="D170" s="16"/>
+      <c r="E170" s="15"/>
+      <c r="F170" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G170" s="17"/>
+      <c r="H170" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I170" s="18"/>
+      <c r="J170" s="18"/>
+    </row>
+    <row r="171" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A171" s="20"/>
+      <c r="B171" s="19"/>
+      <c r="C171" s="18"/>
+      <c r="D171" s="16"/>
+      <c r="E171" s="15"/>
+      <c r="F171" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G171" s="17"/>
+      <c r="H171" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I171" s="18"/>
+      <c r="J171" s="18"/>
+    </row>
+    <row r="172" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A172" s="20"/>
+      <c r="B172" s="19"/>
+      <c r="C172" s="18"/>
+      <c r="D172" s="16"/>
+      <c r="E172" s="15"/>
+      <c r="F172" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G172" s="17"/>
+      <c r="H172" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I172" s="18"/>
+      <c r="J172" s="18"/>
+    </row>
+    <row r="173" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A173" s="20"/>
+      <c r="B173" s="19"/>
+      <c r="C173" s="18"/>
+      <c r="D173" s="16"/>
+      <c r="E173" s="15"/>
+      <c r="F173" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G173" s="17"/>
+      <c r="H173" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I173" s="18"/>
+      <c r="J173" s="18"/>
+    </row>
+    <row r="174" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A174" s="20"/>
+      <c r="B174" s="19"/>
+      <c r="C174" s="18"/>
+      <c r="D174" s="16"/>
+      <c r="E174" s="15"/>
+      <c r="F174" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G174" s="17"/>
+      <c r="H174" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I174" s="18"/>
+      <c r="J174" s="18"/>
+    </row>
+    <row r="175" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A175" s="20"/>
+      <c r="B175" s="19"/>
+      <c r="C175" s="18"/>
+      <c r="D175" s="16"/>
+      <c r="E175" s="15"/>
+      <c r="F175" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G175" s="17"/>
+      <c r="H175" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I175" s="18"/>
+      <c r="J175" s="18"/>
+    </row>
+    <row r="176" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A176" s="20"/>
+      <c r="B176" s="19"/>
+      <c r="C176" s="18"/>
+      <c r="D176" s="16"/>
+      <c r="E176" s="15"/>
+      <c r="F176" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G176" s="17"/>
+      <c r="H176" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I176" s="18"/>
+      <c r="J176" s="18"/>
+    </row>
+    <row r="177" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A177" s="20"/>
+      <c r="B177" s="19"/>
+      <c r="C177" s="18"/>
+      <c r="D177" s="16"/>
+      <c r="E177" s="15"/>
+      <c r="F177" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G177" s="17"/>
+      <c r="H177" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I177" s="18"/>
+      <c r="J177" s="18"/>
+    </row>
+    <row r="178" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A178" s="20"/>
+      <c r="B178" s="19"/>
+      <c r="C178" s="18"/>
+      <c r="D178" s="16"/>
+      <c r="E178" s="15"/>
+      <c r="F178" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G178" s="17"/>
+      <c r="H178" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I178" s="18"/>
+      <c r="J178" s="18"/>
+    </row>
+    <row r="179" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A179" s="20"/>
+      <c r="B179" s="19"/>
+      <c r="C179" s="18"/>
+      <c r="D179" s="16"/>
+      <c r="E179" s="15"/>
+      <c r="F179" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G179" s="17"/>
+      <c r="H179" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I179" s="18"/>
+      <c r="J179" s="18"/>
+    </row>
+    <row r="180" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A180" s="20"/>
+      <c r="B180" s="19"/>
+      <c r="C180" s="18"/>
+      <c r="D180" s="16"/>
+      <c r="E180" s="15"/>
+      <c r="F180" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G180" s="17"/>
+      <c r="H180" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I180" s="18"/>
+      <c r="J180" s="18"/>
+    </row>
+    <row r="181" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A181" s="20"/>
+      <c r="B181" s="19"/>
+      <c r="C181" s="18"/>
+      <c r="D181" s="16"/>
+      <c r="E181" s="15"/>
+      <c r="F181" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G181" s="17"/>
+      <c r="H181" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I181" s="18"/>
+      <c r="J181" s="18"/>
+    </row>
+    <row r="182" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A182" s="20"/>
+      <c r="B182" s="19"/>
+      <c r="C182" s="18"/>
+      <c r="D182" s="16"/>
+      <c r="E182" s="15"/>
+      <c r="F182" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G182" s="17"/>
+      <c r="H182" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I182" s="18"/>
+      <c r="J182" s="18"/>
+    </row>
+    <row r="183" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A183" s="20"/>
+      <c r="B183" s="19"/>
+      <c r="C183" s="18"/>
+      <c r="D183" s="16"/>
+      <c r="E183" s="15"/>
+      <c r="F183" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G183" s="17"/>
+      <c r="H183" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I183" s="18"/>
+      <c r="J183" s="18"/>
+    </row>
+    <row r="184" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A184" s="20"/>
+      <c r="B184" s="19"/>
+      <c r="C184" s="18"/>
+      <c r="D184" s="16"/>
+      <c r="E184" s="15"/>
+      <c r="F184" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G184" s="17"/>
+      <c r="H184" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I184" s="18"/>
+      <c r="J184" s="18"/>
+    </row>
+    <row r="185" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A185" s="20"/>
+      <c r="B185" s="19"/>
+      <c r="C185" s="18"/>
+      <c r="D185" s="16"/>
+      <c r="E185" s="15"/>
+      <c r="F185" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G185" s="17"/>
+      <c r="H185" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I185" s="18"/>
+      <c r="J185" s="18"/>
+    </row>
+    <row r="186" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A186" s="20"/>
+      <c r="B186" s="19"/>
+      <c r="C186" s="18"/>
+      <c r="D186" s="16"/>
+      <c r="E186" s="15"/>
+      <c r="F186" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G186" s="17"/>
+      <c r="H186" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I186" s="18"/>
+      <c r="J186" s="18"/>
+    </row>
+    <row r="187" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A187" s="20"/>
+      <c r="B187" s="19"/>
+      <c r="C187" s="18"/>
+      <c r="D187" s="16"/>
+      <c r="E187" s="15"/>
+      <c r="F187" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G187" s="17"/>
+      <c r="H187" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I187" s="18"/>
+      <c r="J187" s="18"/>
+    </row>
+    <row r="188" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A188" s="20"/>
+      <c r="B188" s="19"/>
+      <c r="C188" s="18"/>
+      <c r="D188" s="16"/>
+      <c r="E188" s="15"/>
+      <c r="F188" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G188" s="17"/>
+      <c r="H188" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I188" s="18"/>
+      <c r="J188" s="18"/>
+    </row>
+    <row r="189" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A189" s="20"/>
+      <c r="B189" s="19"/>
+      <c r="C189" s="18"/>
+      <c r="D189" s="16"/>
+      <c r="E189" s="15"/>
+      <c r="F189" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G189" s="17"/>
+      <c r="H189" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I189" s="18"/>
+      <c r="J189" s="18"/>
+    </row>
+    <row r="190" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A190" s="20"/>
+      <c r="B190" s="19"/>
+      <c r="C190" s="18"/>
+      <c r="D190" s="16"/>
+      <c r="E190" s="15"/>
+      <c r="F190" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G190" s="17"/>
+      <c r="H190" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I190" s="18"/>
+      <c r="J190" s="18"/>
+    </row>
+    <row r="191" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A191" s="20"/>
+      <c r="B191" s="19"/>
+      <c r="C191" s="18"/>
+      <c r="D191" s="16"/>
+      <c r="E191" s="15"/>
+      <c r="F191" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G191" s="17"/>
+      <c r="H191" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I191" s="18"/>
+      <c r="J191" s="18"/>
+    </row>
+    <row r="192" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A192" s="20"/>
+      <c r="B192" s="19"/>
+      <c r="C192" s="18"/>
+      <c r="D192" s="16"/>
+      <c r="E192" s="15"/>
+      <c r="F192" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G192" s="17"/>
+      <c r="H192" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I192" s="18"/>
+      <c r="J192" s="18"/>
+    </row>
+    <row r="193" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A193" s="20"/>
+      <c r="B193" s="19"/>
+      <c r="C193" s="18"/>
+      <c r="D193" s="16"/>
+      <c r="E193" s="15"/>
+      <c r="F193" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G193" s="17"/>
+      <c r="H193" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I193" s="18"/>
+      <c r="J193" s="18"/>
+    </row>
+    <row r="194" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A194" s="20"/>
+      <c r="B194" s="19"/>
+      <c r="C194" s="18"/>
+      <c r="D194" s="16"/>
+      <c r="E194" s="15"/>
+      <c r="F194" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G194" s="17"/>
+      <c r="H194" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I194" s="18"/>
+      <c r="J194" s="18"/>
+    </row>
+    <row r="195" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A195" s="20"/>
+      <c r="B195" s="19"/>
+      <c r="C195" s="18"/>
+      <c r="D195" s="16"/>
+      <c r="E195" s="15"/>
+      <c r="F195" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G195" s="17"/>
+      <c r="H195" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I195" s="18"/>
+      <c r="J195" s="18"/>
+    </row>
+    <row r="196" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A196" s="20"/>
+      <c r="B196" s="19"/>
+      <c r="C196" s="18"/>
+      <c r="D196" s="16"/>
+      <c r="E196" s="15"/>
+      <c r="F196" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G196" s="17"/>
+      <c r="H196" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I196" s="18"/>
+      <c r="J196" s="18"/>
+    </row>
+    <row r="197" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A197" s="20"/>
+      <c r="B197" s="19"/>
+      <c r="C197" s="18"/>
+      <c r="D197" s="16"/>
+      <c r="E197" s="15"/>
+      <c r="F197" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G197" s="17"/>
+      <c r="H197" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I197" s="18"/>
+      <c r="J197" s="18"/>
+    </row>
+    <row r="198" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A198" s="20"/>
+      <c r="B198" s="19"/>
+      <c r="C198" s="18"/>
+      <c r="D198" s="16"/>
+      <c r="E198" s="15"/>
+      <c r="F198" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G198" s="17"/>
+      <c r="H198" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I198" s="18"/>
+      <c r="J198" s="18"/>
+    </row>
+    <row r="199" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A199" s="20"/>
+      <c r="B199" s="19"/>
+      <c r="C199" s="18"/>
+      <c r="D199" s="16"/>
+      <c r="E199" s="15"/>
+      <c r="F199" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G199" s="17"/>
+      <c r="H199" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I199" s="18"/>
+      <c r="J199" s="18"/>
+    </row>
+    <row r="200" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A200" s="20"/>
+      <c r="B200" s="19"/>
+      <c r="C200" s="18"/>
+      <c r="D200" s="16"/>
+      <c r="E200" s="15"/>
+      <c r="F200" s="23">
+        <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="G200" s="17"/>
+      <c r="H200" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I200" s="18"/>
+      <c r="J200" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A2:H2" r:id="rId1" display=" Projects and Stuff LLC - http://ww.projectsandstuff.com"/>
+    <hyperlink ref="B6" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId4"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Corrected the majority of known issues in Schematics and PCB, and updated BOM and Project Log
</commit_message>
<xml_diff>
--- a/Notes/Chameleon BOM.xlsx
+++ b/Notes/Chameleon BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24240" windowHeight="12075" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24240" windowHeight="12075"/>
   </bookViews>
   <sheets>
     <sheet name="Electronics" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="101">
   <si>
     <t>Mfg Part #</t>
   </si>
@@ -96,9 +96,6 @@
     <t>Input Capacitor used with Boost Regulator</t>
   </si>
   <si>
-    <t>3.2mm x 1.6mm</t>
-  </si>
-  <si>
     <t>C3216Y5V1A106Z/0.85</t>
   </si>
   <si>
@@ -225,27 +222,12 @@
     <t>Used for Power Input/Output filtering and Decoupling</t>
   </si>
   <si>
-    <t>3.1 mm x 1.6 mm</t>
-  </si>
-  <si>
     <t>RC1206JR-07220RL</t>
   </si>
   <si>
-    <t>Current Limiting for Ble &amp; Green LEDs (Any resistor around 150 Ohms and with the same package will do)</t>
-  </si>
-  <si>
-    <t>Current Limiting for Red LEDs (Any resistor around 220 Ohms and with the same package will do)</t>
-  </si>
-  <si>
-    <t>RMCF1206JT150R</t>
-  </si>
-  <si>
     <t>Resistor 220Ω 1/4W 5%</t>
   </si>
   <si>
-    <t>Resistor 150Ω 1/4W 5%</t>
-  </si>
-  <si>
     <t>Resistor 10kΩ 1/4W 5%</t>
   </si>
   <si>
@@ -282,84 +264,15 @@
     <t>Used with AVR Analog Reference Filtering and Boost Regulator</t>
   </si>
   <si>
-    <t>LED1, LED2, LED3, LED4, LED5</t>
-  </si>
-  <si>
-    <t>C1, C2, C3, C6, C7, C8, C10, C11, C13</t>
-  </si>
-  <si>
-    <t>C4, C5</t>
-  </si>
-  <si>
-    <t>BT1</t>
-  </si>
-  <si>
-    <t>R1, R2, R3, R4, R5</t>
-  </si>
-  <si>
-    <t>R12, R13, R14, R15, R16, R17, R18, R19, R20, R21</t>
-  </si>
-  <si>
-    <t>R6, R7, R8, R9, R10, R11</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>X1</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>C9, CS1</t>
-  </si>
-  <si>
-    <t>C12</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>RX0, RY0</t>
-  </si>
-  <si>
-    <t>RYB0</t>
-  </si>
-  <si>
-    <t>S1, S2</t>
-  </si>
-  <si>
     <t>AVR Reset and Mode Switch</t>
   </si>
   <si>
-    <t>L1, L2</t>
-  </si>
-  <si>
-    <t>IC1</t>
-  </si>
-  <si>
-    <t>D2</t>
-  </si>
-  <si>
     <t>Power/Status Indicator</t>
   </si>
   <si>
-    <t>CS0</t>
-  </si>
-  <si>
     <t>14 SOIC</t>
   </si>
   <si>
-    <t>ATTINY44-20SSUR</t>
-  </si>
-  <si>
-    <t>Microcontroller AVR 4KB 20MHZ</t>
-  </si>
-  <si>
     <t>Microcontroller</t>
   </si>
   <si>
@@ -382,6 +295,33 @@
   </si>
   <si>
     <t>(Similar also available at http://www.packagingsupplies.com/White_Corrugated_Boxes__Mailers.html - they're cheaper, but may not be enough on hand)</t>
+  </si>
+  <si>
+    <t>ATTINY84A-SSUR</t>
+  </si>
+  <si>
+    <t>Microcontroller AVR 8KB 20MHZ</t>
+  </si>
+  <si>
+    <t>Resistor 330Ω 1/4W 5%</t>
+  </si>
+  <si>
+    <t>RC1206JR-07330RL</t>
+  </si>
+  <si>
+    <t>Current Limiting for Blue &amp; Green LEDs (Any resistor around 220 Ohms and with the same package will do)</t>
+  </si>
+  <si>
+    <t>Current Limiting for Red LEDs (Any resistor around 330 Ohms and with the same package will do)</t>
+  </si>
+  <si>
+    <t>Resistor 1.5kΩ 1/4W 5%</t>
+  </si>
+  <si>
+    <t>RC1206JR-071K5L</t>
+  </si>
+  <si>
+    <t>Pull-up resistors for I2C SCK and SDA lines</t>
   </si>
 </sst>
 </file>
@@ -1457,8 +1397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K200"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:I1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1479,7 +1419,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="28" t="s">
-        <v>115</v>
+        <v>86</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -1530,7 +1470,7 @@
       </c>
       <c r="B4" s="14">
         <f>SUM(I6:I200)</f>
-        <v>6352.2599999999993</v>
+        <v>5597.0199999999995</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -1610,9 +1550,7 @@
       <c r="J6" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="K6" t="s">
-        <v>100</v>
-      </c>
+      <c r="K6"/>
     </row>
     <row r="7" spans="1:11" ht="27" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
@@ -1647,19 +1585,17 @@
       <c r="J7" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="K7" t="s">
-        <v>99</v>
-      </c>
+      <c r="K7"/>
     </row>
     <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>25</v>
+        <v>78</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>51</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>17</v>
@@ -1684,19 +1620,17 @@
       <c r="J8" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="K8" t="s">
-        <v>98</v>
-      </c>
+      <c r="K8"/>
     </row>
     <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="25" t="s">
         <v>25</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>51</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>17</v>
@@ -1721,22 +1655,20 @@
       <c r="J9" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="K9" t="s">
-        <v>97</v>
-      </c>
+      <c r="K9"/>
     </row>
     <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="18" t="s">
         <v>28</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>29</v>
       </c>
       <c r="E10" s="16">
         <v>1375</v>
@@ -1756,24 +1688,22 @@
         <v>950</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="K10" t="s">
-        <v>96</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="K10"/>
     </row>
     <row r="11" spans="1:11" ht="54" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="25" t="s">
-        <v>37</v>
-      </c>
       <c r="D11" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E11" s="16"/>
       <c r="F11" s="15">
@@ -1791,24 +1721,22 @@
         <v>1660</v>
       </c>
       <c r="J11" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="K11" t="s">
-        <v>90</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="K11"/>
     </row>
     <row r="12" spans="1:11" ht="27" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="18" t="s">
         <v>38</v>
-      </c>
-      <c r="B12" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>39</v>
       </c>
       <c r="E12" s="16">
         <v>4000</v>
@@ -1828,24 +1756,22 @@
         <v>302.39999999999998</v>
       </c>
       <c r="J12" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="K12" t="s">
-        <v>95</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="K12"/>
     </row>
     <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="21" t="s">
-        <v>42</v>
-      </c>
       <c r="D13" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E13" s="16">
         <v>7417</v>
@@ -1865,19 +1791,17 @@
         <v>33</v>
       </c>
       <c r="J13" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="K13" t="s">
-        <v>89</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="K13"/>
     </row>
     <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B14" s="26"/>
       <c r="C14" s="21" t="s">
-        <v>114</v>
+        <v>85</v>
       </c>
       <c r="D14" s="18"/>
       <c r="E14" s="16"/>
@@ -1894,24 +1818,22 @@
         <v>0</v>
       </c>
       <c r="J14" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="K14" t="s">
-        <v>87</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="K14"/>
     </row>
     <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="26" t="s">
         <v>47</v>
-      </c>
-      <c r="B15" s="26" t="s">
-        <v>48</v>
       </c>
       <c r="C15" s="21">
         <v>1206</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E15" s="16">
         <v>151361</v>
@@ -1931,24 +1853,22 @@
         <v>8.94</v>
       </c>
       <c r="J15" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="K15" t="s">
-        <v>101</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="K15"/>
     </row>
     <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="26" t="s">
+      <c r="C16" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="21" t="s">
-        <v>52</v>
-      </c>
       <c r="D16" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E16" s="16">
         <v>38808</v>
@@ -1968,24 +1888,22 @@
         <v>4.47</v>
       </c>
       <c r="J16" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="K16" t="s">
-        <v>102</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="K16"/>
     </row>
     <row r="17" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="26" t="s">
         <v>54</v>
-      </c>
-      <c r="B17" s="26" t="s">
-        <v>55</v>
       </c>
       <c r="C17" s="21">
         <v>1206</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E17" s="16">
         <v>55807</v>
@@ -2005,24 +1923,22 @@
         <v>25.2</v>
       </c>
       <c r="J17" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="K17" t="s">
-        <v>109</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="K17"/>
     </row>
     <row r="18" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="C18" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="21" t="s">
-        <v>59</v>
-      </c>
       <c r="D18" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E18" s="16">
         <v>112229</v>
@@ -2042,24 +1958,22 @@
         <v>257.40000000000003</v>
       </c>
       <c r="J18" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="K18" t="s">
-        <v>103</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="K18"/>
     </row>
     <row r="19" spans="1:11" ht="27" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="C19" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="21" t="s">
-        <v>62</v>
-      </c>
       <c r="D19" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E19" s="16">
         <v>2440</v>
@@ -2079,24 +1993,22 @@
         <v>139.5</v>
       </c>
       <c r="J19" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="K19" s="18" t="s">
-        <v>105</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="K19" s="18"/>
     </row>
     <row r="20" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="26" t="s">
-        <v>64</v>
-      </c>
       <c r="C20" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E20" s="16">
         <v>586403</v>
@@ -2116,24 +2028,22 @@
         <v>59.8</v>
       </c>
       <c r="J20" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="K20" t="s">
-        <v>107</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="K20"/>
     </row>
     <row r="21" spans="1:11" ht="27" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" s="26" t="s">
         <v>65</v>
-      </c>
-      <c r="B21" s="26" t="s">
-        <v>66</v>
       </c>
       <c r="C21" s="21">
         <v>1206</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E21" s="16">
         <v>310439</v>
@@ -2153,21 +2063,19 @@
         <v>126.63</v>
       </c>
       <c r="J21" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="K21" t="s">
-        <v>88</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="K21"/>
     </row>
     <row r="22" spans="1:11" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="C22" t="s">
-        <v>68</v>
+        <v>67</v>
+      </c>
+      <c r="C22" s="21">
+        <v>1206</v>
       </c>
       <c r="D22" s="18" t="s">
         <v>17</v>
@@ -2176,75 +2084,71 @@
         <v>100000</v>
       </c>
       <c r="F22" s="15">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G22" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>6000</v>
+        <v>10000</v>
       </c>
       <c r="H22" s="17">
         <v>2.8300000000000001E-3</v>
       </c>
       <c r="I22" s="22">
         <f t="shared" si="0"/>
-        <v>16.98</v>
+        <v>28.3</v>
       </c>
       <c r="J22" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="K22" t="s">
-        <v>93</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="K22"/>
     </row>
     <row r="23" spans="1:11" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="C23" t="s">
-        <v>68</v>
+        <v>95</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>51</v>
       </c>
       <c r="D23" s="18" t="s">
         <v>17</v>
       </c>
       <c r="E23" s="16">
-        <v>80000</v>
+        <v>625000</v>
       </c>
       <c r="F23" s="15">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G23" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>10000</v>
+        <v>6000</v>
       </c>
       <c r="H23" s="17">
-        <v>2.64E-3</v>
+        <v>2.8300000000000001E-3</v>
       </c>
       <c r="I23" s="22">
         <f t="shared" si="0"/>
-        <v>26.4</v>
+        <v>16.98</v>
       </c>
       <c r="J23" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="K23" t="s">
-        <v>92</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="K23"/>
     </row>
     <row r="24" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E24" s="16">
         <v>1480000</v>
@@ -2264,21 +2168,19 @@
         <v>14.15</v>
       </c>
       <c r="J24" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="K24" t="s">
-        <v>91</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="K24"/>
     </row>
     <row r="25" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D25" s="18" t="s">
         <v>17</v>
@@ -2301,27 +2203,25 @@
         <v>385.7</v>
       </c>
       <c r="J25" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="K25" t="s">
-        <v>94</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="K25"/>
     </row>
     <row r="26" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>110</v>
+        <v>83</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>17</v>
       </c>
       <c r="E26" s="16">
-        <v>2735</v>
+        <v>1439</v>
       </c>
       <c r="F26" s="15">
         <v>1</v>
@@ -2331,36 +2231,50 @@
         <v>1000</v>
       </c>
       <c r="H26" s="17">
-        <v>1.5906800000000001</v>
+        <v>0.8246</v>
       </c>
       <c r="I26" s="22">
         <f t="shared" si="0"/>
-        <v>1590.68</v>
+        <v>824.6</v>
       </c>
       <c r="J26" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="K26" t="s">
-        <v>106</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="K26"/>
     </row>
     <row r="27" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="20"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="15"/>
+      <c r="A27" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="C27" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="16">
+        <v>132434</v>
+      </c>
+      <c r="F27" s="15">
+        <v>2</v>
+      </c>
       <c r="G27" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="H27" s="17"/>
+        <v>2000</v>
+      </c>
+      <c r="H27" s="17">
+        <v>4.47E-3</v>
+      </c>
       <c r="I27" s="22">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J27" s="18"/>
+        <v>8.94</v>
+      </c>
+      <c r="J27" s="18" t="s">
+        <v>100</v>
+      </c>
       <c r="K27" s="18"/>
     </row>
     <row r="28" spans="1:11" ht="15" x14ac:dyDescent="0.25">
@@ -5672,15 +5586,16 @@
     <hyperlink ref="B20" r:id="rId14"/>
     <hyperlink ref="B21" r:id="rId15"/>
     <hyperlink ref="B22" r:id="rId16"/>
-    <hyperlink ref="B23" r:id="rId17"/>
-    <hyperlink ref="B24" r:id="rId18"/>
-    <hyperlink ref="B25" r:id="rId19"/>
-    <hyperlink ref="B26" r:id="rId20"/>
+    <hyperlink ref="B24" r:id="rId17"/>
+    <hyperlink ref="B25" r:id="rId18"/>
+    <hyperlink ref="B26" r:id="rId19"/>
+    <hyperlink ref="B23" r:id="rId20"/>
+    <hyperlink ref="B27" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId21"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId22"/>
   <tableParts count="1">
-    <tablePart r:id="rId22"/>
+    <tablePart r:id="rId23"/>
   </tableParts>
 </worksheet>
 </file>
@@ -5689,7 +5604,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -5710,7 +5625,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="28" t="s">
-        <v>116</v>
+        <v>87</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -5803,13 +5718,13 @@
     </row>
     <row r="6" spans="1:10" ht="54" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>119</v>
+        <v>90</v>
       </c>
       <c r="D6" s="16"/>
       <c r="E6" s="15">
@@ -5827,7 +5742,7 @@
         <v>240</v>
       </c>
       <c r="I6" s="18" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
       <c r="J6"/>
     </row>

</xml_diff>

<commit_message>
Updated BOM, renamed CS1 to C14, Improved firmware slightly
</commit_message>
<xml_diff>
--- a/Notes/Chameleon BOM.xlsx
+++ b/Notes/Chameleon BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24240" windowHeight="12075"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24240" windowHeight="12075" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Electronics" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="104">
   <si>
     <t>Mfg Part #</t>
   </si>
@@ -322,6 +322,15 @@
   </si>
   <si>
     <t>Pull-up resistors for I2C SCK and SDA lines</t>
+  </si>
+  <si>
+    <t>Plastic Case</t>
+  </si>
+  <si>
+    <t>Foam Insert (D: 3.5" with battery cut-out)</t>
+  </si>
+  <si>
+    <t>Xingweicheng</t>
   </si>
 </sst>
 </file>
@@ -1397,7 +1406,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -5604,13 +5613,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J200"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.28515625" style="10" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" style="3" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" style="11" customWidth="1"/>
@@ -5673,7 +5682,7 @@
       </c>
       <c r="B4" s="14">
         <f>SUM(H6:H200)</f>
-        <v>240</v>
+        <v>330</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -5747,7 +5756,9 @@
       <c r="J6"/>
     </row>
     <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
+      <c r="A7" s="20" t="s">
+        <v>101</v>
+      </c>
       <c r="B7" s="26"/>
       <c r="C7" s="18"/>
       <c r="D7" s="16"/>
@@ -5765,19 +5776,27 @@
       <c r="J7"/>
     </row>
     <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
+      <c r="A8" s="20" t="s">
+        <v>102</v>
+      </c>
       <c r="B8" s="26"/>
-      <c r="C8" s="18"/>
+      <c r="C8" s="18" t="s">
+        <v>103</v>
+      </c>
       <c r="D8" s="16"/>
-      <c r="E8" s="15"/>
+      <c r="E8" s="15">
+        <v>1</v>
+      </c>
       <c r="F8" s="23">
         <f>SUM(Table42[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="17"/>
+        <v>1000</v>
+      </c>
+      <c r="G8" s="17">
+        <v>0.09</v>
+      </c>
       <c r="H8" s="22">
         <f>SUM(G8*F8)</f>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="I8" s="18"/>
       <c r="J8"/>

</xml_diff>

<commit_message>
Added I2C series resistors, updated Project Log, added PDF version of Project Log
</commit_message>
<xml_diff>
--- a/Notes/Chameleon BOM.xlsx
+++ b/Notes/Chameleon BOM.xlsx
@@ -321,9 +321,6 @@
     <t>RC1206JR-071K5L</t>
   </si>
   <si>
-    <t>Pull-up resistors for I2C SCK and SDA lines</t>
-  </si>
-  <si>
     <t>Plastic Case</t>
   </si>
   <si>
@@ -334,6 +331,9 @@
   </si>
   <si>
     <t>KiCad Footprint</t>
+  </si>
+  <si>
+    <t>Pull-up and series resistors for I2C SCK and SDA lines</t>
   </si>
 </sst>
 </file>
@@ -575,26 +575,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="28">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Lucida Sans Unicode"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1002,6 +982,26 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="9"/>
+        <color theme="1"/>
+        <name val="Lucida Sans Unicode"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
         <color theme="1" tint="0.14996795556505021"/>
         <name val="Lucida Sans Unicode"/>
         <scheme val="none"/>
@@ -1104,42 +1104,42 @@
     <tableColumn id="1" name="Description" dataDxfId="23"/>
     <tableColumn id="2" name="Mfg Part #" dataDxfId="22"/>
     <tableColumn id="3" name="Package" dataDxfId="21"/>
-    <tableColumn id="12" name="KiCad Footprint" dataDxfId="0"/>
-    <tableColumn id="5" name="Default Supplier" dataDxfId="20"/>
-    <tableColumn id="10" name="Supplier On Hand" dataDxfId="19"/>
-    <tableColumn id="4" name="Qty per board" dataDxfId="18"/>
-    <tableColumn id="6" name="Total Qty Needed" dataDxfId="17">
+    <tableColumn id="12" name="KiCad Footprint" dataDxfId="20"/>
+    <tableColumn id="5" name="Default Supplier" dataDxfId="19"/>
+    <tableColumn id="10" name="Supplier On Hand" dataDxfId="18"/>
+    <tableColumn id="4" name="Qty per board" dataDxfId="17"/>
+    <tableColumn id="6" name="Total Qty Needed" dataDxfId="16">
       <calculatedColumnFormula>SUM(Table4[[#This Row],[Qty per board]]*Goal)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Price per part at Qty" dataDxfId="16"/>
-    <tableColumn id="7" name="Total Price" dataDxfId="15">
+    <tableColumn id="11" name="Price per part at Qty" dataDxfId="15"/>
+    <tableColumn id="7" name="Total Price" dataDxfId="14">
       <calculatedColumnFormula>SUM(I6*H6)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Notes" dataDxfId="14"/>
-    <tableColumn id="9" name="Part References" dataDxfId="13"/>
+    <tableColumn id="8" name="Notes" dataDxfId="13"/>
+    <tableColumn id="9" name="Part References" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="Projects and Stuff" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table42" displayName="Table42" ref="A5:J200" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table42" displayName="Table42" ref="A5:J200" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A5:J200"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="Description" dataDxfId="10"/>
-    <tableColumn id="2" name="Mfg Part #" dataDxfId="9"/>
-    <tableColumn id="5" name="Default Supplier" dataDxfId="8"/>
-    <tableColumn id="10" name="Supplier On Hand" dataDxfId="7"/>
-    <tableColumn id="4" name="Qty per board" dataDxfId="6"/>
-    <tableColumn id="6" name="Total Qty Needed" dataDxfId="5">
+    <tableColumn id="1" name="Description" dataDxfId="9"/>
+    <tableColumn id="2" name="Mfg Part #" dataDxfId="8"/>
+    <tableColumn id="5" name="Default Supplier" dataDxfId="7"/>
+    <tableColumn id="10" name="Supplier On Hand" dataDxfId="6"/>
+    <tableColumn id="4" name="Qty per board" dataDxfId="5"/>
+    <tableColumn id="6" name="Total Qty Needed" dataDxfId="4">
       <calculatedColumnFormula>SUM(Table42[[#This Row],[Qty per board]]*Goal)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Price per part at Qty" dataDxfId="4"/>
-    <tableColumn id="7" name="Total Price" dataDxfId="3">
+    <tableColumn id="11" name="Price per part at Qty" dataDxfId="3"/>
+    <tableColumn id="7" name="Total Price" dataDxfId="2">
       <calculatedColumnFormula>SUM(G6*F6)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Notes" dataDxfId="2"/>
-    <tableColumn id="9" name="Part References" dataDxfId="1"/>
+    <tableColumn id="8" name="Notes" dataDxfId="1"/>
+    <tableColumn id="9" name="Part References" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Projects and Stuff" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1434,8 +1434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1511,7 +1511,7 @@
       </c>
       <c r="B4" s="14">
         <f>SUM(J6:J200)</f>
-        <v>5588.53</v>
+        <v>5597.47</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -1535,7 +1535,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>12</v>
@@ -2308,7 +2308,7 @@
       </c>
       <c r="L26"/>
     </row>
-    <row r="27" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="27" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
         <v>98</v>
       </c>
@@ -2326,21 +2326,21 @@
         <v>132434</v>
       </c>
       <c r="G27" s="15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H27" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="I27" s="17">
         <v>4.47E-3</v>
       </c>
       <c r="J27" s="22">
         <f t="shared" si="0"/>
-        <v>8.94</v>
+        <v>17.88</v>
       </c>
       <c r="K27" s="18" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="L27" s="18"/>
     </row>
@@ -5988,7 +5988,7 @@
     </row>
     <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B7" s="26"/>
       <c r="C7" s="18"/>
@@ -6008,11 +6008,11 @@
     </row>
     <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B8" s="26"/>
       <c r="C8" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="15">

</xml_diff>

<commit_message>
Updated schematics and Project Log with new resistor values, and added PDF BOM
</commit_message>
<xml_diff>
--- a/Notes/Chameleon BOM.xlsx
+++ b/Notes/Chameleon BOM.xlsx
@@ -13,13 +13,14 @@
   <definedNames>
     <definedName name="Goal" localSheetId="1">Other!$J$1</definedName>
     <definedName name="Goal">Electronics!$L$1</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Electronics!$A$1:$L$28</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="131">
   <si>
     <t>Mfg Part #</t>
   </si>
@@ -117,9 +118,6 @@
     <t>IC LED Driver RGBA</t>
   </si>
   <si>
-    <t>Battery (Li-Poly 500mAh)</t>
-  </si>
-  <si>
     <t>Nominal Voltage: 3.7V</t>
   </si>
   <si>
@@ -159,9 +157,6 @@
     <t>LED Lighting</t>
   </si>
   <si>
-    <t>Resistor 1.0kΩ 1/4W 5%</t>
-  </si>
-  <si>
     <t>RC1206JR-071KL</t>
   </si>
   <si>
@@ -300,9 +295,6 @@
     <t>ATTINY84A-SSUR</t>
   </si>
   <si>
-    <t>Microcontroller AVR 8KB 20MHZ</t>
-  </si>
-  <si>
     <t>Resistor 330Ω 1/4W 5%</t>
   </si>
   <si>
@@ -315,12 +307,6 @@
     <t>Current Limiting for Red LEDs (Any resistor around 330 Ohms and with the same package will do)</t>
   </si>
   <si>
-    <t>Resistor 1.5kΩ 1/4W 5%</t>
-  </si>
-  <si>
-    <t>RC1206JR-071K5L</t>
-  </si>
-  <si>
     <t>Plastic Case</t>
   </si>
   <si>
@@ -334,6 +320,99 @@
   </si>
   <si>
     <t>Pull-up and series resistors for I2C SCK and SDA lines</t>
+  </si>
+  <si>
+    <t>Resistor 1.8kΩ 1/4W 5%</t>
+  </si>
+  <si>
+    <t>RC1206JR-071K8L</t>
+  </si>
+  <si>
+    <t>Resistor 100Ω 1/4W 5%</t>
+  </si>
+  <si>
+    <t>RC1206JR-07100RL</t>
+  </si>
+  <si>
+    <t>Series resistors for SCK and SDA lines</t>
+  </si>
+  <si>
+    <t>IC Microcontroller AVR 8KB 20MHZ</t>
+  </si>
+  <si>
+    <t>C1, C2, C3, C6, C7, C8, C10, C11, C13</t>
+  </si>
+  <si>
+    <t>R1, R2</t>
+  </si>
+  <si>
+    <t>R3, R22</t>
+  </si>
+  <si>
+    <t>R4, R5</t>
+  </si>
+  <si>
+    <t>C9, C14</t>
+  </si>
+  <si>
+    <t>RX0, RY0</t>
+  </si>
+  <si>
+    <t>Resistor 1kΩ 1/4W 5%</t>
+  </si>
+  <si>
+    <t>R12, R13, R14, R15, R16, R17, R18, R19, R20, R21</t>
+  </si>
+  <si>
+    <t>R6, R7, R8, R9, R10, R11</t>
+  </si>
+  <si>
+    <t>Battery (Li-Poly 3.7V 500mAh)</t>
+  </si>
+  <si>
+    <t>BT1</t>
+  </si>
+  <si>
+    <t>L1, L2</t>
+  </si>
+  <si>
+    <t>CS0</t>
+  </si>
+  <si>
+    <t>RYB0</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>C4, C5</t>
+  </si>
+  <si>
+    <t>IC1</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>LED1, LED2, LED3, LED4, LED5</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>S1, S2</t>
   </si>
 </sst>
 </file>
@@ -483,7 +562,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -562,6 +641,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1432,10 +1514,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:L200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1456,18 +1541,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
+      <c r="A1" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
       <c r="K1" s="8" t="s">
         <v>4</v>
       </c>
@@ -1476,18 +1561,18 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
     </row>
@@ -1509,9 +1594,9 @@
       <c r="A4" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="29">
         <f>SUM(J6:J200)</f>
-        <v>5597.47</v>
+        <v>5635.72</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -1535,7 +1620,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>12</v>
@@ -1562,22 +1647,22 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>15</v>
+        <v>77</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="24"/>
+        <v>76</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="21"/>
       <c r="E6" s="18" t="s">
         <v>17</v>
       </c>
       <c r="F6" s="16">
-        <v>1335</v>
+        <v>186142</v>
       </c>
       <c r="G6" s="15">
         <v>1</v>
@@ -1587,141 +1672,149 @@
         <v>1000</v>
       </c>
       <c r="I6" s="17">
-        <v>0.33</v>
+        <v>0.28799999999999998</v>
       </c>
       <c r="J6" s="22">
-        <f>SUM(I6*H6)</f>
-        <v>330</v>
+        <f t="shared" ref="J6:J25" si="0">SUM(I6*H6)</f>
+        <v>288</v>
       </c>
       <c r="K6" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="L6"/>
-    </row>
-    <row r="7" spans="1:12" ht="27" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="L6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="25"/>
+        <v>25</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="21"/>
       <c r="E7" s="18" t="s">
         <v>17</v>
       </c>
       <c r="F7" s="16">
-        <v>22159</v>
+        <v>116496</v>
       </c>
       <c r="G7" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H7" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="I7" s="17">
-        <v>9.4759999999999997E-2</v>
+        <v>3.8249999999999999E-2</v>
       </c>
       <c r="J7" s="22">
-        <f>SUM(I7*H7)</f>
-        <v>94.759999999999991</v>
+        <f t="shared" si="0"/>
+        <v>76.5</v>
       </c>
       <c r="K7" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="L7"/>
+        <v>24</v>
+      </c>
+      <c r="L7" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="8" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>78</v>
+        <v>39</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="18" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="F8" s="16">
-        <v>186142</v>
+        <v>7417</v>
       </c>
       <c r="G8" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H8" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="I8" s="17">
-        <v>0.28799999999999998</v>
+        <v>1.6500000000000001E-2</v>
       </c>
       <c r="J8" s="22">
-        <f>SUM(I8*H8)</f>
-        <v>288</v>
+        <f t="shared" si="0"/>
+        <v>33</v>
       </c>
       <c r="K8" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="L8"/>
-    </row>
-    <row r="9" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="L8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="27" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>51</v>
+        <v>63</v>
+      </c>
+      <c r="C9" s="21">
+        <v>1206</v>
       </c>
       <c r="D9" s="21"/>
       <c r="E9" s="18" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="F9" s="16">
-        <v>116496</v>
+        <v>310439</v>
       </c>
       <c r="G9" s="15">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="H9" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>1000</v>
+        <v>9000</v>
       </c>
       <c r="I9" s="17">
-        <v>3.8249999999999999E-2</v>
+        <v>1.4069999999999999E-2</v>
       </c>
       <c r="J9" s="22">
-        <f t="shared" ref="J9:J69" si="0">SUM(I9*H9)</f>
-        <v>38.25</v>
+        <f t="shared" si="0"/>
+        <v>126.63</v>
       </c>
       <c r="K9" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="L9"/>
+        <v>64</v>
+      </c>
+      <c r="L9" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="25"/>
+        <v>52</v>
+      </c>
+      <c r="C10" s="21">
+        <v>1206</v>
+      </c>
+      <c r="D10" s="21"/>
       <c r="E10" s="18" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="F10" s="16">
-        <v>1375</v>
+        <v>55807</v>
       </c>
       <c r="G10" s="15">
         <v>1</v>
@@ -1731,67 +1824,73 @@
         <v>1000</v>
       </c>
       <c r="I10" s="17">
-        <v>0.95</v>
+        <v>2.52E-2</v>
       </c>
       <c r="J10" s="22">
         <f t="shared" si="0"/>
-        <v>950</v>
+        <v>25.2</v>
       </c>
       <c r="K10" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="L10"/>
-    </row>
-    <row r="11" spans="1:12" ht="54" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="L10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>32</v>
+        <v>112</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="25"/>
+        <v>45</v>
+      </c>
+      <c r="C11" s="21">
+        <v>1206</v>
+      </c>
+      <c r="D11" s="21"/>
       <c r="E11" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="16"/>
+        <v>37</v>
+      </c>
+      <c r="F11" s="16">
+        <v>151361</v>
+      </c>
       <c r="G11" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H11" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="I11" s="17">
-        <v>1.66</v>
+        <v>4.47E-3</v>
       </c>
       <c r="J11" s="22">
         <f t="shared" si="0"/>
-        <v>1660</v>
+        <v>8.94</v>
       </c>
       <c r="K11" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="L11"/>
-    </row>
-    <row r="12" spans="1:12" ht="27" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="L11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>76</v>
+        <v>49</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F12" s="16">
-        <v>4000</v>
+        <v>38808</v>
       </c>
       <c r="G12" s="15">
         <v>1</v>
@@ -1801,97 +1900,111 @@
         <v>1000</v>
       </c>
       <c r="I12" s="17">
-        <v>0.3024</v>
+        <v>4.47E-3</v>
       </c>
       <c r="J12" s="22">
         <f t="shared" si="0"/>
-        <v>302.39999999999998</v>
+        <v>4.47</v>
       </c>
       <c r="K12" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="L12"/>
-    </row>
-    <row r="13" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="L12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>41</v>
+        <v>65</v>
+      </c>
+      <c r="C13" s="21">
+        <v>1206</v>
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="18" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="F13" s="16">
-        <v>7417</v>
+        <v>100000</v>
       </c>
       <c r="G13" s="15">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H13" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>2000</v>
+        <v>10000</v>
       </c>
       <c r="I13" s="17">
-        <v>1.6500000000000001E-2</v>
+        <v>2.8300000000000001E-3</v>
       </c>
       <c r="J13" s="22">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>28.3</v>
       </c>
       <c r="K13" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="L13"/>
-    </row>
-    <row r="14" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="L13" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="16"/>
+        <v>91</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="25"/>
+      <c r="E14" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="16">
+        <v>625000</v>
+      </c>
       <c r="G14" s="15">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H14" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>5000</v>
-      </c>
-      <c r="I14" s="17"/>
+        <v>6000</v>
+      </c>
+      <c r="I14" s="17">
+        <v>2.8300000000000001E-3</v>
+      </c>
       <c r="J14" s="22">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16.98</v>
       </c>
       <c r="K14" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="L14"/>
+        <v>94</v>
+      </c>
+      <c r="L14" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="15" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="21">
-        <v>1206</v>
+        <v>68</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>49</v>
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F15" s="16">
-        <v>151361</v>
+        <v>1480000</v>
       </c>
       <c r="G15" s="15">
         <v>2</v>
@@ -1901,105 +2014,111 @@
         <v>2000</v>
       </c>
       <c r="I15" s="17">
-        <v>4.47E-3</v>
+        <v>2.8300000000000001E-3</v>
       </c>
       <c r="J15" s="22">
         <f t="shared" si="0"/>
-        <v>8.94</v>
+        <v>5.66</v>
       </c>
       <c r="K15" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="L15"/>
-    </row>
-    <row r="16" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="L15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="27" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" s="21"/>
+      <c r="D16" s="25"/>
       <c r="E16" s="18" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="F16" s="16">
-        <v>38808</v>
+        <v>141711</v>
       </c>
       <c r="G16" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H16" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="I16" s="17">
         <v>4.47E-3</v>
       </c>
       <c r="J16" s="22">
         <f t="shared" si="0"/>
-        <v>4.47</v>
+        <v>8.94</v>
       </c>
       <c r="K16" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="L16"/>
+        <v>99</v>
+      </c>
+      <c r="L16" s="18" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="17" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" s="21">
-        <v>1206</v>
-      </c>
-      <c r="D17" s="21"/>
+        <v>103</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="25"/>
       <c r="E17" s="18" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="F17" s="16">
-        <v>55807</v>
+        <v>362104</v>
       </c>
       <c r="G17" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H17" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="I17" s="17">
-        <v>2.52E-2</v>
+        <v>4.47E-3</v>
       </c>
       <c r="J17" s="22">
         <f t="shared" si="0"/>
-        <v>25.2</v>
+        <v>8.94</v>
       </c>
       <c r="K17" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="L17"/>
-    </row>
-    <row r="18" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="L17" s="18" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="27" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D18" s="21"/>
       <c r="E18" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F18" s="16">
-        <v>112229</v>
+        <v>2440</v>
       </c>
       <c r="G18" s="15">
         <v>2</v>
@@ -2009,66 +2128,62 @@
         <v>2000</v>
       </c>
       <c r="I18" s="17">
-        <v>0.12870000000000001</v>
+        <v>6.9750000000000006E-2</v>
       </c>
       <c r="J18" s="22">
         <f t="shared" si="0"/>
-        <v>257.40000000000003</v>
+        <v>139.5</v>
       </c>
       <c r="K18" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="L18"/>
-    </row>
-    <row r="19" spans="1:12" ht="27" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="L18" s="18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="B19" s="26" t="s">
-        <v>60</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B19" s="26"/>
       <c r="C19" s="21" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="D19" s="21"/>
-      <c r="E19" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F19" s="16">
-        <v>2440</v>
-      </c>
+      <c r="E19" s="18"/>
+      <c r="F19" s="16"/>
       <c r="G19" s="15">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H19" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>2000</v>
-      </c>
-      <c r="I19" s="17">
-        <v>6.9750000000000006E-2</v>
-      </c>
+        <v>5000</v>
+      </c>
+      <c r="I19" s="17"/>
       <c r="J19" s="22">
         <f t="shared" si="0"/>
-        <v>139.5</v>
+        <v>0</v>
       </c>
       <c r="K19" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="L19" s="18"/>
+        <v>44</v>
+      </c>
+      <c r="L19" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="20" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F20" s="16">
         <v>586403</v>
@@ -2088,170 +2203,180 @@
         <v>59.8</v>
       </c>
       <c r="K20" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="L20"/>
+        <v>80</v>
+      </c>
+      <c r="L20" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="21" spans="1:12" ht="27" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="C21" s="21">
-        <v>1206</v>
-      </c>
-      <c r="D21" s="21"/>
+        <v>19</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="25"/>
       <c r="E21" s="18" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="F21" s="16">
-        <v>310439</v>
+        <v>22159</v>
       </c>
       <c r="G21" s="15">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="H21" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>9000</v>
+        <v>1000</v>
       </c>
       <c r="I21" s="17">
-        <v>1.4069999999999999E-2</v>
+        <v>9.4759999999999997E-2</v>
       </c>
       <c r="J21" s="22">
         <f t="shared" si="0"/>
-        <v>126.63</v>
+        <v>94.759999999999991</v>
       </c>
       <c r="K21" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="L21"/>
-    </row>
-    <row r="22" spans="1:12" ht="40.5" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="27" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="C22" s="21">
-        <v>1206</v>
+        <v>75</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>74</v>
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="18" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="F22" s="16">
-        <v>100000</v>
+        <v>4000</v>
       </c>
       <c r="G22" s="15">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H22" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="I22" s="17">
-        <v>2.8300000000000001E-3</v>
+        <v>0.3024</v>
       </c>
       <c r="J22" s="22">
         <f t="shared" si="0"/>
-        <v>28.3</v>
+        <v>302.39999999999998</v>
       </c>
       <c r="K22" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="L22"/>
-    </row>
-    <row r="23" spans="1:12" ht="40.5" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="L22" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>95</v>
-      </c>
-      <c r="C23" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="25"/>
+        <v>55</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="21"/>
       <c r="E23" s="18" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="F23" s="16">
-        <v>625000</v>
+        <v>112229</v>
       </c>
       <c r="G23" s="15">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H23" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>6000</v>
+        <v>2000</v>
       </c>
       <c r="I23" s="17">
-        <v>2.8300000000000001E-3</v>
+        <v>0.12870000000000001</v>
       </c>
       <c r="J23" s="22">
         <f t="shared" si="0"/>
-        <v>16.98</v>
+        <v>257.40000000000003</v>
       </c>
       <c r="K23" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="L23"/>
+        <v>79</v>
+      </c>
+      <c r="L23" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="24" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
-        <v>69</v>
+        <v>105</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="C24" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="D24" s="21"/>
+        <v>90</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="D24" s="25"/>
       <c r="E24" s="18" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="F24" s="16">
-        <v>1480000</v>
+        <v>1439</v>
       </c>
       <c r="G24" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H24" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="I24" s="17">
-        <v>2.8300000000000001E-3</v>
+        <v>0.8246</v>
       </c>
       <c r="J24" s="22">
         <f t="shared" si="0"/>
-        <v>5.66</v>
+        <v>824.6</v>
       </c>
       <c r="K24" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="L24"/>
-    </row>
-    <row r="25" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="L24" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
-        <v>73</v>
+        <v>15</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="C25" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="D25" s="25"/>
+        <v>14</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="24"/>
       <c r="E25" s="18" t="s">
         <v>17</v>
       </c>
       <c r="F25" s="16">
-        <v>19970</v>
+        <v>1335</v>
       </c>
       <c r="G25" s="15">
         <v>1</v>
@@ -2261,33 +2386,35 @@
         <v>1000</v>
       </c>
       <c r="I25" s="17">
-        <v>0.38569999999999999</v>
+        <v>0.33</v>
       </c>
       <c r="J25" s="22">
         <f t="shared" si="0"/>
-        <v>385.7</v>
+        <v>330</v>
       </c>
       <c r="K25" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="L25"/>
+        <v>18</v>
+      </c>
+      <c r="L25" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="26" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
-        <v>93</v>
+        <v>31</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>92</v>
+        <v>27</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>83</v>
+        <v>30</v>
       </c>
       <c r="D26" s="25"/>
       <c r="E26" s="18" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="F26" s="16">
-        <v>1439</v>
+        <v>1375</v>
       </c>
       <c r="G26" s="15">
         <v>1</v>
@@ -2297,72 +2424,92 @@
         <v>1000</v>
       </c>
       <c r="I26" s="17">
-        <v>0.8246</v>
+        <v>0.95</v>
       </c>
       <c r="J26" s="22">
-        <f t="shared" si="0"/>
-        <v>824.6</v>
+        <f t="shared" ref="J26:J69" si="1">SUM(I26*H26)</f>
+        <v>950</v>
       </c>
       <c r="K26" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="L26"/>
-    </row>
-    <row r="27" spans="1:12" ht="27" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="L26" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="54" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
-        <v>98</v>
+        <v>115</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>99</v>
+        <v>34</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="D27" s="25"/>
       <c r="E27" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27" s="16"/>
+      <c r="G27" s="15">
+        <v>1</v>
+      </c>
+      <c r="H27" s="23">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>1000</v>
+      </c>
+      <c r="I27" s="17">
+        <v>1.66</v>
+      </c>
+      <c r="J27" s="22">
+        <f t="shared" si="1"/>
+        <v>1660</v>
+      </c>
+      <c r="K27" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="L27" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="D28" s="25"/>
+      <c r="E28" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="F27" s="16">
-        <v>132434</v>
-      </c>
-      <c r="G27" s="15">
-        <v>4</v>
-      </c>
-      <c r="H27" s="23">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>4000</v>
-      </c>
-      <c r="I27" s="17">
-        <v>4.47E-3</v>
-      </c>
-      <c r="J27" s="22">
-        <f t="shared" si="0"/>
-        <v>17.88</v>
-      </c>
-      <c r="K27" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="L27" s="18"/>
-    </row>
-    <row r="28" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="20"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="15"/>
+      <c r="F28" s="16">
+        <v>19970</v>
+      </c>
+      <c r="G28" s="15">
+        <v>1</v>
+      </c>
       <c r="H28" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="I28" s="17"/>
+        <v>1000</v>
+      </c>
+      <c r="I28" s="17">
+        <v>0.38569999999999999</v>
+      </c>
       <c r="J28" s="22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18"/>
+        <f t="shared" si="1"/>
+        <v>385.7</v>
+      </c>
+      <c r="K28" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="L28" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="29" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="20"/>
@@ -2378,7 +2525,7 @@
       </c>
       <c r="I29" s="17"/>
       <c r="J29" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K29" s="18"/>
@@ -2398,7 +2545,7 @@
       </c>
       <c r="I30" s="17"/>
       <c r="J30" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K30" s="18"/>
@@ -2418,7 +2565,7 @@
       </c>
       <c r="I31" s="17"/>
       <c r="J31" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K31" s="18"/>
@@ -2438,7 +2585,7 @@
       </c>
       <c r="I32" s="17"/>
       <c r="J32" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K32" s="18"/>
@@ -2458,7 +2605,7 @@
       </c>
       <c r="I33" s="17"/>
       <c r="J33" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K33" s="18"/>
@@ -2478,7 +2625,7 @@
       </c>
       <c r="I34" s="17"/>
       <c r="J34" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K34" s="18"/>
@@ -2498,7 +2645,7 @@
       </c>
       <c r="I35" s="17"/>
       <c r="J35" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K35" s="18"/>
@@ -2518,7 +2665,7 @@
       </c>
       <c r="I36" s="17"/>
       <c r="J36" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K36" s="18"/>
@@ -2538,7 +2685,7 @@
       </c>
       <c r="I37" s="17"/>
       <c r="J37" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K37" s="18"/>
@@ -2558,7 +2705,7 @@
       </c>
       <c r="I38" s="17"/>
       <c r="J38" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K38" s="18"/>
@@ -2578,7 +2725,7 @@
       </c>
       <c r="I39" s="17"/>
       <c r="J39" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K39" s="18"/>
@@ -2598,7 +2745,7 @@
       </c>
       <c r="I40" s="17"/>
       <c r="J40" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K40" s="18"/>
@@ -2618,7 +2765,7 @@
       </c>
       <c r="I41" s="17"/>
       <c r="J41" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K41" s="18"/>
@@ -2638,7 +2785,7 @@
       </c>
       <c r="I42" s="17"/>
       <c r="J42" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K42" s="18"/>
@@ -2658,7 +2805,7 @@
       </c>
       <c r="I43" s="17"/>
       <c r="J43" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K43" s="18"/>
@@ -2678,7 +2825,7 @@
       </c>
       <c r="I44" s="17"/>
       <c r="J44" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K44" s="18"/>
@@ -2698,7 +2845,7 @@
       </c>
       <c r="I45" s="17"/>
       <c r="J45" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K45" s="18"/>
@@ -2718,7 +2865,7 @@
       </c>
       <c r="I46" s="17"/>
       <c r="J46" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K46" s="18"/>
@@ -2738,7 +2885,7 @@
       </c>
       <c r="I47" s="17"/>
       <c r="J47" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K47" s="18"/>
@@ -2758,7 +2905,7 @@
       </c>
       <c r="I48" s="17"/>
       <c r="J48" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K48" s="18"/>
@@ -2778,7 +2925,7 @@
       </c>
       <c r="I49" s="17"/>
       <c r="J49" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K49" s="18"/>
@@ -2798,7 +2945,7 @@
       </c>
       <c r="I50" s="17"/>
       <c r="J50" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K50" s="18"/>
@@ -2818,7 +2965,7 @@
       </c>
       <c r="I51" s="17"/>
       <c r="J51" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K51" s="18"/>
@@ -2838,7 +2985,7 @@
       </c>
       <c r="I52" s="17"/>
       <c r="J52" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K52" s="18"/>
@@ -2858,7 +3005,7 @@
       </c>
       <c r="I53" s="17"/>
       <c r="J53" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K53" s="18"/>
@@ -2878,7 +3025,7 @@
       </c>
       <c r="I54" s="17"/>
       <c r="J54" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K54" s="18"/>
@@ -2898,7 +3045,7 @@
       </c>
       <c r="I55" s="17"/>
       <c r="J55" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K55" s="18"/>
@@ -2918,7 +3065,7 @@
       </c>
       <c r="I56" s="17"/>
       <c r="J56" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K56" s="18"/>
@@ -2938,7 +3085,7 @@
       </c>
       <c r="I57" s="17"/>
       <c r="J57" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K57" s="18"/>
@@ -2958,7 +3105,7 @@
       </c>
       <c r="I58" s="17"/>
       <c r="J58" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K58" s="18"/>
@@ -2978,7 +3125,7 @@
       </c>
       <c r="I59" s="17"/>
       <c r="J59" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K59" s="18"/>
@@ -2998,7 +3145,7 @@
       </c>
       <c r="I60" s="17"/>
       <c r="J60" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K60" s="18"/>
@@ -3018,7 +3165,7 @@
       </c>
       <c r="I61" s="17"/>
       <c r="J61" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K61" s="18"/>
@@ -3038,7 +3185,7 @@
       </c>
       <c r="I62" s="17"/>
       <c r="J62" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K62" s="18"/>
@@ -3058,7 +3205,7 @@
       </c>
       <c r="I63" s="17"/>
       <c r="J63" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K63" s="18"/>
@@ -3078,7 +3225,7 @@
       </c>
       <c r="I64" s="17"/>
       <c r="J64" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K64" s="18"/>
@@ -3098,7 +3245,7 @@
       </c>
       <c r="I65" s="17"/>
       <c r="J65" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K65" s="18"/>
@@ -3118,7 +3265,7 @@
       </c>
       <c r="I66" s="17"/>
       <c r="J66" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K66" s="18"/>
@@ -3138,7 +3285,7 @@
       </c>
       <c r="I67" s="17"/>
       <c r="J67" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K67" s="18"/>
@@ -3158,7 +3305,7 @@
       </c>
       <c r="I68" s="17"/>
       <c r="J68" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K68" s="18"/>
@@ -3178,7 +3325,7 @@
       </c>
       <c r="I69" s="17"/>
       <c r="J69" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K69" s="18"/>
@@ -3198,7 +3345,7 @@
       </c>
       <c r="I70" s="17"/>
       <c r="J70" s="22">
-        <f t="shared" ref="J70:J133" si="1">SUM(I70*H70)</f>
+        <f t="shared" ref="J70:J133" si="2">SUM(I70*H70)</f>
         <v>0</v>
       </c>
       <c r="K70" s="18"/>
@@ -3218,7 +3365,7 @@
       </c>
       <c r="I71" s="17"/>
       <c r="J71" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K71" s="18"/>
@@ -3238,7 +3385,7 @@
       </c>
       <c r="I72" s="17"/>
       <c r="J72" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K72" s="18"/>
@@ -3258,7 +3405,7 @@
       </c>
       <c r="I73" s="17"/>
       <c r="J73" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K73" s="18"/>
@@ -3278,7 +3425,7 @@
       </c>
       <c r="I74" s="17"/>
       <c r="J74" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K74" s="18"/>
@@ -3298,7 +3445,7 @@
       </c>
       <c r="I75" s="17"/>
       <c r="J75" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K75" s="18"/>
@@ -3318,7 +3465,7 @@
       </c>
       <c r="I76" s="17"/>
       <c r="J76" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K76" s="18"/>
@@ -3338,7 +3485,7 @@
       </c>
       <c r="I77" s="17"/>
       <c r="J77" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K77" s="18"/>
@@ -3358,7 +3505,7 @@
       </c>
       <c r="I78" s="17"/>
       <c r="J78" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K78" s="18"/>
@@ -3378,7 +3525,7 @@
       </c>
       <c r="I79" s="17"/>
       <c r="J79" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K79" s="18"/>
@@ -3398,7 +3545,7 @@
       </c>
       <c r="I80" s="17"/>
       <c r="J80" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K80" s="18"/>
@@ -3418,7 +3565,7 @@
       </c>
       <c r="I81" s="17"/>
       <c r="J81" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K81" s="18"/>
@@ -3438,7 +3585,7 @@
       </c>
       <c r="I82" s="17"/>
       <c r="J82" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K82" s="18"/>
@@ -3458,7 +3605,7 @@
       </c>
       <c r="I83" s="17"/>
       <c r="J83" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K83" s="18"/>
@@ -3478,7 +3625,7 @@
       </c>
       <c r="I84" s="17"/>
       <c r="J84" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K84" s="18"/>
@@ -3498,7 +3645,7 @@
       </c>
       <c r="I85" s="17"/>
       <c r="J85" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K85" s="18"/>
@@ -3518,7 +3665,7 @@
       </c>
       <c r="I86" s="17"/>
       <c r="J86" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K86" s="18"/>
@@ -3538,7 +3685,7 @@
       </c>
       <c r="I87" s="17"/>
       <c r="J87" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K87" s="18"/>
@@ -3558,7 +3705,7 @@
       </c>
       <c r="I88" s="17"/>
       <c r="J88" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K88" s="18"/>
@@ -3578,7 +3725,7 @@
       </c>
       <c r="I89" s="17"/>
       <c r="J89" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K89" s="18"/>
@@ -3598,7 +3745,7 @@
       </c>
       <c r="I90" s="17"/>
       <c r="J90" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K90" s="18"/>
@@ -3618,7 +3765,7 @@
       </c>
       <c r="I91" s="17"/>
       <c r="J91" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K91" s="18"/>
@@ -3638,7 +3785,7 @@
       </c>
       <c r="I92" s="17"/>
       <c r="J92" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K92" s="18"/>
@@ -3658,7 +3805,7 @@
       </c>
       <c r="I93" s="17"/>
       <c r="J93" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K93" s="18"/>
@@ -3678,7 +3825,7 @@
       </c>
       <c r="I94" s="17"/>
       <c r="J94" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K94" s="18"/>
@@ -3698,7 +3845,7 @@
       </c>
       <c r="I95" s="17"/>
       <c r="J95" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K95" s="18"/>
@@ -3718,7 +3865,7 @@
       </c>
       <c r="I96" s="17"/>
       <c r="J96" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K96" s="18"/>
@@ -3738,7 +3885,7 @@
       </c>
       <c r="I97" s="17"/>
       <c r="J97" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K97" s="18"/>
@@ -3758,7 +3905,7 @@
       </c>
       <c r="I98" s="17"/>
       <c r="J98" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K98" s="18"/>
@@ -3778,7 +3925,7 @@
       </c>
       <c r="I99" s="17"/>
       <c r="J99" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K99" s="18"/>
@@ -3798,7 +3945,7 @@
       </c>
       <c r="I100" s="17"/>
       <c r="J100" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K100" s="18"/>
@@ -3818,7 +3965,7 @@
       </c>
       <c r="I101" s="17"/>
       <c r="J101" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K101" s="18"/>
@@ -3838,7 +3985,7 @@
       </c>
       <c r="I102" s="17"/>
       <c r="J102" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K102" s="18"/>
@@ -3858,7 +4005,7 @@
       </c>
       <c r="I103" s="17"/>
       <c r="J103" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K103" s="18"/>
@@ -3878,7 +4025,7 @@
       </c>
       <c r="I104" s="17"/>
       <c r="J104" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K104" s="18"/>
@@ -3898,7 +4045,7 @@
       </c>
       <c r="I105" s="17"/>
       <c r="J105" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K105" s="18"/>
@@ -3918,7 +4065,7 @@
       </c>
       <c r="I106" s="17"/>
       <c r="J106" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K106" s="18"/>
@@ -3938,7 +4085,7 @@
       </c>
       <c r="I107" s="17"/>
       <c r="J107" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K107" s="18"/>
@@ -3958,7 +4105,7 @@
       </c>
       <c r="I108" s="17"/>
       <c r="J108" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K108" s="18"/>
@@ -3978,7 +4125,7 @@
       </c>
       <c r="I109" s="17"/>
       <c r="J109" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K109" s="18"/>
@@ -3998,7 +4145,7 @@
       </c>
       <c r="I110" s="17"/>
       <c r="J110" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K110" s="18"/>
@@ -4018,7 +4165,7 @@
       </c>
       <c r="I111" s="17"/>
       <c r="J111" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K111" s="18"/>
@@ -4038,7 +4185,7 @@
       </c>
       <c r="I112" s="17"/>
       <c r="J112" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K112" s="18"/>
@@ -4058,7 +4205,7 @@
       </c>
       <c r="I113" s="17"/>
       <c r="J113" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K113" s="18"/>
@@ -4078,7 +4225,7 @@
       </c>
       <c r="I114" s="17"/>
       <c r="J114" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K114" s="18"/>
@@ -4098,7 +4245,7 @@
       </c>
       <c r="I115" s="17"/>
       <c r="J115" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K115" s="18"/>
@@ -4118,7 +4265,7 @@
       </c>
       <c r="I116" s="17"/>
       <c r="J116" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K116" s="18"/>
@@ -4138,7 +4285,7 @@
       </c>
       <c r="I117" s="17"/>
       <c r="J117" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K117" s="18"/>
@@ -4158,7 +4305,7 @@
       </c>
       <c r="I118" s="17"/>
       <c r="J118" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K118" s="18"/>
@@ -4178,7 +4325,7 @@
       </c>
       <c r="I119" s="17"/>
       <c r="J119" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K119" s="18"/>
@@ -4198,7 +4345,7 @@
       </c>
       <c r="I120" s="17"/>
       <c r="J120" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K120" s="18"/>
@@ -4218,7 +4365,7 @@
       </c>
       <c r="I121" s="17"/>
       <c r="J121" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K121" s="18"/>
@@ -4238,7 +4385,7 @@
       </c>
       <c r="I122" s="17"/>
       <c r="J122" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K122" s="18"/>
@@ -4258,7 +4405,7 @@
       </c>
       <c r="I123" s="17"/>
       <c r="J123" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K123" s="18"/>
@@ -4278,7 +4425,7 @@
       </c>
       <c r="I124" s="17"/>
       <c r="J124" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K124" s="18"/>
@@ -4298,7 +4445,7 @@
       </c>
       <c r="I125" s="17"/>
       <c r="J125" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K125" s="18"/>
@@ -4318,7 +4465,7 @@
       </c>
       <c r="I126" s="17"/>
       <c r="J126" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K126" s="18"/>
@@ -4338,7 +4485,7 @@
       </c>
       <c r="I127" s="17"/>
       <c r="J127" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K127" s="18"/>
@@ -4358,7 +4505,7 @@
       </c>
       <c r="I128" s="17"/>
       <c r="J128" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K128" s="18"/>
@@ -4378,7 +4525,7 @@
       </c>
       <c r="I129" s="17"/>
       <c r="J129" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K129" s="18"/>
@@ -4398,7 +4545,7 @@
       </c>
       <c r="I130" s="17"/>
       <c r="J130" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K130" s="18"/>
@@ -4418,7 +4565,7 @@
       </c>
       <c r="I131" s="17"/>
       <c r="J131" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K131" s="18"/>
@@ -4438,7 +4585,7 @@
       </c>
       <c r="I132" s="17"/>
       <c r="J132" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K132" s="18"/>
@@ -4458,7 +4605,7 @@
       </c>
       <c r="I133" s="17"/>
       <c r="J133" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K133" s="18"/>
@@ -4478,7 +4625,7 @@
       </c>
       <c r="I134" s="17"/>
       <c r="J134" s="22">
-        <f t="shared" ref="J134:J197" si="2">SUM(I134*H134)</f>
+        <f t="shared" ref="J134:J197" si="3">SUM(I134*H134)</f>
         <v>0</v>
       </c>
       <c r="K134" s="18"/>
@@ -4498,7 +4645,7 @@
       </c>
       <c r="I135" s="17"/>
       <c r="J135" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K135" s="18"/>
@@ -4518,7 +4665,7 @@
       </c>
       <c r="I136" s="17"/>
       <c r="J136" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K136" s="18"/>
@@ -4538,7 +4685,7 @@
       </c>
       <c r="I137" s="17"/>
       <c r="J137" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K137" s="18"/>
@@ -4558,7 +4705,7 @@
       </c>
       <c r="I138" s="17"/>
       <c r="J138" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K138" s="18"/>
@@ -4578,7 +4725,7 @@
       </c>
       <c r="I139" s="17"/>
       <c r="J139" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K139" s="18"/>
@@ -4598,7 +4745,7 @@
       </c>
       <c r="I140" s="17"/>
       <c r="J140" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K140" s="18"/>
@@ -4618,7 +4765,7 @@
       </c>
       <c r="I141" s="17"/>
       <c r="J141" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K141" s="18"/>
@@ -4638,7 +4785,7 @@
       </c>
       <c r="I142" s="17"/>
       <c r="J142" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K142" s="18"/>
@@ -4658,7 +4805,7 @@
       </c>
       <c r="I143" s="17"/>
       <c r="J143" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K143" s="18"/>
@@ -4678,7 +4825,7 @@
       </c>
       <c r="I144" s="17"/>
       <c r="J144" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K144" s="18"/>
@@ -4698,7 +4845,7 @@
       </c>
       <c r="I145" s="17"/>
       <c r="J145" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K145" s="18"/>
@@ -4718,7 +4865,7 @@
       </c>
       <c r="I146" s="17"/>
       <c r="J146" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K146" s="18"/>
@@ -4738,7 +4885,7 @@
       </c>
       <c r="I147" s="17"/>
       <c r="J147" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K147" s="18"/>
@@ -4758,7 +4905,7 @@
       </c>
       <c r="I148" s="17"/>
       <c r="J148" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K148" s="18"/>
@@ -4778,7 +4925,7 @@
       </c>
       <c r="I149" s="17"/>
       <c r="J149" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K149" s="18"/>
@@ -4798,7 +4945,7 @@
       </c>
       <c r="I150" s="17"/>
       <c r="J150" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K150" s="18"/>
@@ -4818,7 +4965,7 @@
       </c>
       <c r="I151" s="17"/>
       <c r="J151" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K151" s="18"/>
@@ -4838,7 +4985,7 @@
       </c>
       <c r="I152" s="17"/>
       <c r="J152" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K152" s="18"/>
@@ -4858,7 +5005,7 @@
       </c>
       <c r="I153" s="17"/>
       <c r="J153" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K153" s="18"/>
@@ -4878,7 +5025,7 @@
       </c>
       <c r="I154" s="17"/>
       <c r="J154" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K154" s="18"/>
@@ -4898,7 +5045,7 @@
       </c>
       <c r="I155" s="17"/>
       <c r="J155" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K155" s="18"/>
@@ -4918,7 +5065,7 @@
       </c>
       <c r="I156" s="17"/>
       <c r="J156" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K156" s="18"/>
@@ -4938,7 +5085,7 @@
       </c>
       <c r="I157" s="17"/>
       <c r="J157" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K157" s="18"/>
@@ -4958,7 +5105,7 @@
       </c>
       <c r="I158" s="17"/>
       <c r="J158" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K158" s="18"/>
@@ -4978,7 +5125,7 @@
       </c>
       <c r="I159" s="17"/>
       <c r="J159" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K159" s="18"/>
@@ -4998,7 +5145,7 @@
       </c>
       <c r="I160" s="17"/>
       <c r="J160" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K160" s="18"/>
@@ -5018,7 +5165,7 @@
       </c>
       <c r="I161" s="17"/>
       <c r="J161" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K161" s="18"/>
@@ -5038,7 +5185,7 @@
       </c>
       <c r="I162" s="17"/>
       <c r="J162" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K162" s="18"/>
@@ -5058,7 +5205,7 @@
       </c>
       <c r="I163" s="17"/>
       <c r="J163" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K163" s="18"/>
@@ -5078,7 +5225,7 @@
       </c>
       <c r="I164" s="17"/>
       <c r="J164" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K164" s="18"/>
@@ -5098,7 +5245,7 @@
       </c>
       <c r="I165" s="17"/>
       <c r="J165" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K165" s="18"/>
@@ -5118,7 +5265,7 @@
       </c>
       <c r="I166" s="17"/>
       <c r="J166" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K166" s="18"/>
@@ -5138,7 +5285,7 @@
       </c>
       <c r="I167" s="17"/>
       <c r="J167" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K167" s="18"/>
@@ -5158,7 +5305,7 @@
       </c>
       <c r="I168" s="17"/>
       <c r="J168" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K168" s="18"/>
@@ -5178,7 +5325,7 @@
       </c>
       <c r="I169" s="17"/>
       <c r="J169" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K169" s="18"/>
@@ -5198,7 +5345,7 @@
       </c>
       <c r="I170" s="17"/>
       <c r="J170" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K170" s="18"/>
@@ -5218,7 +5365,7 @@
       </c>
       <c r="I171" s="17"/>
       <c r="J171" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K171" s="18"/>
@@ -5238,7 +5385,7 @@
       </c>
       <c r="I172" s="17"/>
       <c r="J172" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K172" s="18"/>
@@ -5258,7 +5405,7 @@
       </c>
       <c r="I173" s="17"/>
       <c r="J173" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K173" s="18"/>
@@ -5278,7 +5425,7 @@
       </c>
       <c r="I174" s="17"/>
       <c r="J174" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K174" s="18"/>
@@ -5298,7 +5445,7 @@
       </c>
       <c r="I175" s="17"/>
       <c r="J175" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K175" s="18"/>
@@ -5318,7 +5465,7 @@
       </c>
       <c r="I176" s="17"/>
       <c r="J176" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K176" s="18"/>
@@ -5338,7 +5485,7 @@
       </c>
       <c r="I177" s="17"/>
       <c r="J177" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K177" s="18"/>
@@ -5358,7 +5505,7 @@
       </c>
       <c r="I178" s="17"/>
       <c r="J178" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K178" s="18"/>
@@ -5378,7 +5525,7 @@
       </c>
       <c r="I179" s="17"/>
       <c r="J179" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K179" s="18"/>
@@ -5398,7 +5545,7 @@
       </c>
       <c r="I180" s="17"/>
       <c r="J180" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K180" s="18"/>
@@ -5418,7 +5565,7 @@
       </c>
       <c r="I181" s="17"/>
       <c r="J181" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K181" s="18"/>
@@ -5438,7 +5585,7 @@
       </c>
       <c r="I182" s="17"/>
       <c r="J182" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K182" s="18"/>
@@ -5458,7 +5605,7 @@
       </c>
       <c r="I183" s="17"/>
       <c r="J183" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K183" s="18"/>
@@ -5478,7 +5625,7 @@
       </c>
       <c r="I184" s="17"/>
       <c r="J184" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K184" s="18"/>
@@ -5498,7 +5645,7 @@
       </c>
       <c r="I185" s="17"/>
       <c r="J185" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K185" s="18"/>
@@ -5518,7 +5665,7 @@
       </c>
       <c r="I186" s="17"/>
       <c r="J186" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K186" s="18"/>
@@ -5538,7 +5685,7 @@
       </c>
       <c r="I187" s="17"/>
       <c r="J187" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K187" s="18"/>
@@ -5558,7 +5705,7 @@
       </c>
       <c r="I188" s="17"/>
       <c r="J188" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K188" s="18"/>
@@ -5578,7 +5725,7 @@
       </c>
       <c r="I189" s="17"/>
       <c r="J189" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K189" s="18"/>
@@ -5598,7 +5745,7 @@
       </c>
       <c r="I190" s="17"/>
       <c r="J190" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K190" s="18"/>
@@ -5618,7 +5765,7 @@
       </c>
       <c r="I191" s="17"/>
       <c r="J191" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K191" s="18"/>
@@ -5638,7 +5785,7 @@
       </c>
       <c r="I192" s="17"/>
       <c r="J192" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K192" s="18"/>
@@ -5658,7 +5805,7 @@
       </c>
       <c r="I193" s="17"/>
       <c r="J193" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K193" s="18"/>
@@ -5678,7 +5825,7 @@
       </c>
       <c r="I194" s="17"/>
       <c r="J194" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K194" s="18"/>
@@ -5698,7 +5845,7 @@
       </c>
       <c r="I195" s="17"/>
       <c r="J195" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K195" s="18"/>
@@ -5718,7 +5865,7 @@
       </c>
       <c r="I196" s="17"/>
       <c r="J196" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K196" s="18"/>
@@ -5738,7 +5885,7 @@
       </c>
       <c r="I197" s="17"/>
       <c r="J197" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K197" s="18"/>
@@ -5758,7 +5905,7 @@
       </c>
       <c r="I198" s="17"/>
       <c r="J198" s="22">
-        <f t="shared" ref="J198:J200" si="3">SUM(I198*H198)</f>
+        <f t="shared" ref="J198:J200" si="4">SUM(I198*H198)</f>
         <v>0</v>
       </c>
       <c r="K198" s="18"/>
@@ -5778,7 +5925,7 @@
       </c>
       <c r="I199" s="17"/>
       <c r="J199" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K199" s="18"/>
@@ -5798,7 +5945,7 @@
       </c>
       <c r="I200" s="17"/>
       <c r="J200" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K200" s="18"/>
@@ -5811,31 +5958,32 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2:J2" r:id="rId1" display=" Projects and Stuff LLC - http://ww.projectsandstuff.com"/>
-    <hyperlink ref="B6" r:id="rId2"/>
-    <hyperlink ref="B7" r:id="rId3"/>
-    <hyperlink ref="B8" r:id="rId4"/>
-    <hyperlink ref="B9" r:id="rId5"/>
-    <hyperlink ref="B10" r:id="rId6"/>
-    <hyperlink ref="B12" r:id="rId7"/>
-    <hyperlink ref="B13" r:id="rId8"/>
-    <hyperlink ref="B15" r:id="rId9"/>
-    <hyperlink ref="B16" r:id="rId10"/>
-    <hyperlink ref="B17" r:id="rId11"/>
-    <hyperlink ref="B18" r:id="rId12"/>
-    <hyperlink ref="B19" r:id="rId13"/>
+    <hyperlink ref="B25" r:id="rId2"/>
+    <hyperlink ref="B21" r:id="rId3"/>
+    <hyperlink ref="B6" r:id="rId4"/>
+    <hyperlink ref="B7" r:id="rId5"/>
+    <hyperlink ref="B26" r:id="rId6"/>
+    <hyperlink ref="B22" r:id="rId7"/>
+    <hyperlink ref="B8" r:id="rId8"/>
+    <hyperlink ref="B11" r:id="rId9"/>
+    <hyperlink ref="B12" r:id="rId10"/>
+    <hyperlink ref="B10" r:id="rId11"/>
+    <hyperlink ref="B23" r:id="rId12"/>
+    <hyperlink ref="B18" r:id="rId13"/>
     <hyperlink ref="B20" r:id="rId14"/>
-    <hyperlink ref="B21" r:id="rId15"/>
-    <hyperlink ref="B22" r:id="rId16"/>
-    <hyperlink ref="B24" r:id="rId17"/>
-    <hyperlink ref="B25" r:id="rId18"/>
-    <hyperlink ref="B26" r:id="rId19"/>
-    <hyperlink ref="B23" r:id="rId20"/>
-    <hyperlink ref="B27" r:id="rId21"/>
+    <hyperlink ref="B9" r:id="rId15"/>
+    <hyperlink ref="B13" r:id="rId16"/>
+    <hyperlink ref="B15" r:id="rId17"/>
+    <hyperlink ref="B28" r:id="rId18"/>
+    <hyperlink ref="B24" r:id="rId19"/>
+    <hyperlink ref="B14" r:id="rId20"/>
+    <hyperlink ref="B16" r:id="rId21"/>
+    <hyperlink ref="B17" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId22"/>
+  <pageSetup scale="47" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId23"/>
   <tableParts count="1">
-    <tablePart r:id="rId23"/>
+    <tablePart r:id="rId24"/>
   </tableParts>
 </worksheet>
 </file>
@@ -5864,16 +6012,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
+      <c r="A1" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
       <c r="I1" s="8" t="s">
         <v>4</v>
       </c>
@@ -5882,16 +6030,16 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
     </row>
@@ -5958,13 +6106,13 @@
     </row>
     <row r="6" spans="1:10" ht="54" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="18" t="s">
         <v>88</v>
-      </c>
-      <c r="B6" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>90</v>
       </c>
       <c r="D6" s="16"/>
       <c r="E6" s="15">
@@ -5982,13 +6130,13 @@
         <v>240</v>
       </c>
       <c r="I6" s="18" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J6"/>
     </row>
     <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B7" s="26"/>
       <c r="C7" s="18"/>
@@ -6008,11 +6156,11 @@
     </row>
     <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B8" s="26"/>
       <c r="C8" s="18" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="15">

</xml_diff>

<commit_message>
Began updating BOM with new parts and updated data.
</commit_message>
<xml_diff>
--- a/Notes/Chameleon BOM.xlsx
+++ b/Notes/Chameleon BOM.xlsx
@@ -13,14 +13,14 @@
   <definedNames>
     <definedName name="Goal" localSheetId="1">Other!$J$1</definedName>
     <definedName name="Goal">Electronics!$L$1</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Electronics!$A$1:$L$28</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Electronics!$A$1:$L$31</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="113">
   <si>
     <t>Mfg Part #</t>
   </si>
@@ -70,27 +70,15 @@
     <t>IC Boost Regulator 5V 0.2A</t>
   </si>
   <si>
-    <t>6-TSOP (0.059", 1.50mm Width) 5 leads</t>
-  </si>
-  <si>
     <t>Digikey</t>
   </si>
   <si>
     <t>Also available at Newark, Farnell, Avnet, Verical, etc</t>
   </si>
   <si>
-    <t>BAT750TA</t>
-  </si>
-  <si>
     <t>SOT-23-3</t>
   </si>
   <si>
-    <t>Used with Boost Regulator. Typical Forward Voltage = 290mV @ 250mA</t>
-  </si>
-  <si>
-    <t>Diode Schottky 40V 750mA</t>
-  </si>
-  <si>
     <t>Output Capacitor used with Boost Regulator</t>
   </si>
   <si>
@@ -103,18 +91,9 @@
     <t>Capacitor Ceramic 10uF 10V Y5V</t>
   </si>
   <si>
-    <t>PCA9685PW,112</t>
-  </si>
-  <si>
-    <t>Future</t>
-  </si>
-  <si>
     <t>Also available at Digikey and Verical</t>
   </si>
   <si>
-    <t>TSSOP-28</t>
-  </si>
-  <si>
     <t>IC LED Driver RGBA</t>
   </si>
   <si>
@@ -130,15 +109,9 @@
     <t>50.5mm x 34.5 mm x 3.2mm</t>
   </si>
   <si>
-    <t>Crystal 20 MHZ 8pF</t>
-  </si>
-  <si>
     <t>DigiKey</t>
   </si>
   <si>
-    <t>AVR Timing</t>
-  </si>
-  <si>
     <t>CC0805DRNPO9BN8R0</t>
   </si>
   <si>
@@ -238,18 +211,6 @@
     <t>Connector Receptical USB Micro B</t>
   </si>
   <si>
-    <t>ZX62-B-5PA(11)</t>
-  </si>
-  <si>
-    <t>USB Connector for charging</t>
-  </si>
-  <si>
-    <t>5.0 mm x 3.2 mm</t>
-  </si>
-  <si>
-    <t>NX5032GA-20.000000MHZ-LN-CD-1</t>
-  </si>
-  <si>
     <t>JMK316BJ476ML-T</t>
   </si>
   <si>
@@ -265,12 +226,6 @@
     <t>Power/Status Indicator</t>
   </si>
   <si>
-    <t>14 SOIC</t>
-  </si>
-  <si>
-    <t>Microcontroller</t>
-  </si>
-  <si>
     <t>5.0mm x 5.0mm</t>
   </si>
   <si>
@@ -292,9 +247,6 @@
     <t>(Similar also available at http://www.packagingsupplies.com/White_Corrugated_Boxes__Mailers.html - they're cheaper, but may not be enough on hand)</t>
   </si>
   <si>
-    <t>ATTINY84A-SSUR</t>
-  </si>
-  <si>
     <t>Resistor 330Ω 1/4W 5%</t>
   </si>
   <si>
@@ -337,82 +289,76 @@
     <t>Series resistors for SCK and SDA lines</t>
   </si>
   <si>
-    <t>IC Microcontroller AVR 8KB 20MHZ</t>
-  </si>
-  <si>
-    <t>C1, C2, C3, C6, C7, C8, C10, C11, C13</t>
-  </si>
-  <si>
-    <t>R1, R2</t>
-  </si>
-  <si>
-    <t>R3, R22</t>
-  </si>
-  <si>
-    <t>R4, R5</t>
-  </si>
-  <si>
-    <t>C9, C14</t>
-  </si>
-  <si>
-    <t>RX0, RY0</t>
-  </si>
-  <si>
     <t>Resistor 1kΩ 1/4W 5%</t>
   </si>
   <si>
-    <t>R12, R13, R14, R15, R16, R17, R18, R19, R20, R21</t>
-  </si>
-  <si>
-    <t>R6, R7, R8, R9, R10, R11</t>
-  </si>
-  <si>
     <t>Battery (Li-Poly 3.7V 500mAh)</t>
   </si>
   <si>
-    <t>BT1</t>
-  </si>
-  <si>
-    <t>L1, L2</t>
-  </si>
-  <si>
-    <t>CS0</t>
-  </si>
-  <si>
-    <t>RYB0</t>
-  </si>
-  <si>
-    <t>C12</t>
-  </si>
-  <si>
-    <t>C4, C5</t>
-  </si>
-  <si>
-    <t>IC1</t>
-  </si>
-  <si>
-    <t>X1</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>D2</t>
-  </si>
-  <si>
-    <t>LED1, LED2, LED3, LED4, LED5</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>S1, S2</t>
+    <t>Microcontroller with USB</t>
+  </si>
+  <si>
+    <t>IC LDO 3.3V 0.15A</t>
+  </si>
+  <si>
+    <t>SOT-23-5</t>
+  </si>
+  <si>
+    <t>TLV71333PDBVR</t>
+  </si>
+  <si>
+    <t>5-TSOP</t>
+  </si>
+  <si>
+    <t>Diode Schottky 10V 0.57A</t>
+  </si>
+  <si>
+    <t>ZLLS410TA</t>
+  </si>
+  <si>
+    <t>Used with Boost Regulator</t>
+  </si>
+  <si>
+    <t>Per Board Cost:</t>
+  </si>
+  <si>
+    <t>AS1121-BQFT</t>
+  </si>
+  <si>
+    <t>32-TQFN (5x5)</t>
+  </si>
+  <si>
+    <t>ZX62WRD-B-5PC</t>
+  </si>
+  <si>
+    <t>Water resistant USB Connector for charging and data</t>
+  </si>
+  <si>
+    <t>TL1105JAF160Q</t>
+  </si>
+  <si>
+    <t>Switch Tactile SPST-NO 0.05A 12V</t>
+  </si>
+  <si>
+    <t>7.20mm x 7.00mm</t>
+  </si>
+  <si>
+    <t>Mode Select Switch</t>
+  </si>
+  <si>
+    <t>1RWHT</t>
+  </si>
+  <si>
+    <t>Switch Cap Round White</t>
+  </si>
+  <si>
+    <t>Cap for switch TL1105JAF160Q</t>
+  </si>
+  <si>
+    <t>IC Microcontroller ATXMEGA16A4U</t>
+  </si>
+  <si>
+    <t>GOOD</t>
   </si>
 </sst>
 </file>
@@ -423,7 +369,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00000"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -519,6 +465,38 @@
       <color theme="1"/>
       <name val="Lucida Sans Unicode"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Lucida Sans Unicode"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Lucida Sans Unicode"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Lucida Sans Unicode"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="9"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Lucida Sans Unicode"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -562,7 +540,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -642,9 +620,39 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1180,8 +1188,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A5:L200" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
-  <autoFilter ref="A5:L200"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A6:L203" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+  <autoFilter ref="A6:L203"/>
   <tableColumns count="12">
     <tableColumn id="1" name="Description" dataDxfId="23"/>
     <tableColumn id="2" name="Mfg Part #" dataDxfId="22"/>
@@ -1195,7 +1203,7 @@
     </tableColumn>
     <tableColumn id="11" name="Price per part at Qty" dataDxfId="15"/>
     <tableColumn id="7" name="Total Price" dataDxfId="14">
-      <calculatedColumnFormula>SUM(I6*H6)</calculatedColumnFormula>
+      <calculatedColumnFormula>SUM(I7*H7)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" name="Notes" dataDxfId="13"/>
     <tableColumn id="9" name="Part References" dataDxfId="12"/>
@@ -1517,17 +1525,17 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L200"/>
+  <dimension ref="A1:L203"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.28515625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" style="3" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" style="3" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" style="11" customWidth="1"/>
@@ -1541,38 +1549,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
+      <c r="A1" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
       <c r="K1" s="8" t="s">
         <v>4</v>
       </c>
       <c r="L1" s="9">
-        <v>1000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
     </row>
@@ -1590,16 +1598,21 @@
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="29">
-        <f>SUM(J6:J200)</f>
-        <v>5635.72</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
+      <c r="B4" s="37">
+        <f>SUM(J7:J203)</f>
+        <v>3027.59</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="37">
+        <f>B4/Goal</f>
+        <v>6.05518</v>
+      </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -1609,291 +1622,257 @@
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
     </row>
-    <row r="5" spans="1:12" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+    </row>
+    <row r="6" spans="1:12" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="B6" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="D6" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L6" s="2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="B6" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="16">
-        <v>186142</v>
-      </c>
-      <c r="G6" s="15">
-        <v>1</v>
-      </c>
-      <c r="H6" s="23">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>1000</v>
-      </c>
-      <c r="I6" s="17">
-        <v>0.28799999999999998</v>
-      </c>
-      <c r="J6" s="22">
-        <f t="shared" ref="J6:J25" si="0">SUM(I6*H6)</f>
-        <v>288</v>
-      </c>
-      <c r="K6" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="L6" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>26</v>
+        <v>64</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D7" s="21"/>
       <c r="E7" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F7" s="16">
-        <v>116496</v>
+        <v>186142</v>
       </c>
       <c r="G7" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H7" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="I7" s="17">
-        <v>3.8249999999999999E-2</v>
+        <v>0.28799999999999998</v>
       </c>
       <c r="J7" s="22">
-        <f t="shared" si="0"/>
-        <v>76.5</v>
+        <f t="shared" ref="J7:J27" si="0">SUM(I7*H7)</f>
+        <v>144</v>
       </c>
       <c r="K7" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="L7" t="s">
-        <v>110</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="L7"/>
     </row>
     <row r="8" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="C8" s="21" t="s">
         <v>40</v>
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="18" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="F8" s="16">
-        <v>7417</v>
+        <v>116496</v>
       </c>
       <c r="G8" s="15">
         <v>2</v>
       </c>
       <c r="H8" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="I8" s="17">
-        <v>1.6500000000000001E-2</v>
+        <v>3.8249999999999999E-2</v>
       </c>
       <c r="J8" s="22">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>38.25</v>
       </c>
       <c r="K8" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="L8" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="27" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="L8"/>
+    </row>
+    <row r="9" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="21">
-        <v>1206</v>
+        <v>30</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>31</v>
       </c>
       <c r="D9" s="21"/>
       <c r="E9" s="18" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F9" s="16">
-        <v>310439</v>
+        <v>7417</v>
       </c>
       <c r="G9" s="15">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H9" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>9000</v>
+        <v>1000</v>
       </c>
       <c r="I9" s="17">
-        <v>1.4069999999999999E-2</v>
+        <v>1.6500000000000001E-2</v>
       </c>
       <c r="J9" s="22">
         <f t="shared" si="0"/>
-        <v>126.63</v>
+        <v>16.5</v>
       </c>
       <c r="K9" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="L9" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="L9"/>
+    </row>
+    <row r="10" spans="1:12" ht="27" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C10" s="21">
         <v>1206</v>
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="18" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F10" s="16">
-        <v>55807</v>
+        <v>310439</v>
       </c>
       <c r="G10" s="15">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="H10" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>1000</v>
+        <v>4500</v>
       </c>
       <c r="I10" s="17">
-        <v>2.52E-2</v>
+        <v>1.4069999999999999E-2</v>
       </c>
       <c r="J10" s="22">
         <f t="shared" si="0"/>
-        <v>25.2</v>
+        <v>63.314999999999998</v>
       </c>
       <c r="K10" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="L10" t="s">
-        <v>118</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="L10"/>
     </row>
     <row r="11" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>112</v>
+        <v>42</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C11" s="21">
         <v>1206</v>
       </c>
       <c r="D11" s="21"/>
       <c r="E11" s="18" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F11" s="16">
-        <v>151361</v>
+        <v>55807</v>
       </c>
       <c r="G11" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H11" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="I11" s="17">
-        <v>4.47E-3</v>
+        <v>2.52E-2</v>
       </c>
       <c r="J11" s="22">
         <f t="shared" si="0"/>
-        <v>8.94</v>
+        <v>12.6</v>
       </c>
       <c r="K11" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="L11" t="s">
-        <v>111</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="L11"/>
     </row>
     <row r="12" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>47</v>
+        <v>89</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>49</v>
+        <v>36</v>
+      </c>
+      <c r="C12" s="21">
+        <v>1206</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="18" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F12" s="16">
-        <v>38808</v>
+        <v>151361</v>
       </c>
       <c r="G12" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H12" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
@@ -1907,397 +1886,377 @@
         <v>4.47</v>
       </c>
       <c r="K12" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="L12" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="40.5" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="L12"/>
+    </row>
+    <row r="13" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="C13" s="21">
-        <v>1206</v>
+        <v>39</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>40</v>
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="18" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="F13" s="16">
-        <v>100000</v>
+        <v>38808</v>
       </c>
       <c r="G13" s="15">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H13" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>10000</v>
+        <v>500</v>
       </c>
       <c r="I13" s="17">
-        <v>2.8300000000000001E-3</v>
+        <v>4.47E-3</v>
       </c>
       <c r="J13" s="22">
         <f t="shared" si="0"/>
-        <v>28.3</v>
+        <v>2.2349999999999999</v>
       </c>
       <c r="K13" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="L13" t="s">
-        <v>113</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="L13"/>
     </row>
     <row r="14" spans="1:12" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>91</v>
+        <v>57</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14" s="25"/>
+        <v>56</v>
+      </c>
+      <c r="C14" s="21">
+        <v>1206</v>
+      </c>
+      <c r="D14" s="21"/>
       <c r="E14" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F14" s="16">
-        <v>625000</v>
+        <v>100000</v>
       </c>
       <c r="G14" s="15">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H14" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>6000</v>
+        <v>5000</v>
       </c>
       <c r="I14" s="17">
         <v>2.8300000000000001E-3</v>
       </c>
       <c r="J14" s="22">
         <f t="shared" si="0"/>
-        <v>16.98</v>
+        <v>14.15</v>
       </c>
       <c r="K14" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="L14" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="L14"/>
+    </row>
+    <row r="15" spans="1:12" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="21"/>
+        <v>76</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="25"/>
       <c r="E15" s="18" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="F15" s="16">
-        <v>1480000</v>
+        <v>625000</v>
       </c>
       <c r="G15" s="15">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H15" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="I15" s="17">
         <v>2.8300000000000001E-3</v>
       </c>
       <c r="J15" s="22">
         <f t="shared" si="0"/>
-        <v>5.66</v>
+        <v>8.49</v>
       </c>
       <c r="K15" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="L15" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="27" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="L15"/>
+    </row>
+    <row r="16" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
-        <v>100</v>
+        <v>58</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>101</v>
-      </c>
-      <c r="C16" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="D16" s="25"/>
+        <v>59</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="21"/>
       <c r="E16" s="18" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="F16" s="16">
-        <v>141711</v>
+        <v>1480000</v>
       </c>
       <c r="G16" s="15">
         <v>2</v>
       </c>
       <c r="H16" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="I16" s="17">
-        <v>4.47E-3</v>
+        <v>2.8300000000000001E-3</v>
       </c>
       <c r="J16" s="22">
         <f t="shared" si="0"/>
-        <v>8.94</v>
+        <v>2.83</v>
       </c>
       <c r="K16" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="L16" s="18" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="L16"/>
+    </row>
+    <row r="17" spans="1:12" ht="27" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D17" s="25"/>
       <c r="E17" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F17" s="16">
-        <v>362104</v>
+        <v>141711</v>
       </c>
       <c r="G17" s="15">
         <v>2</v>
       </c>
       <c r="H17" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="I17" s="17">
         <v>4.47E-3</v>
       </c>
       <c r="J17" s="22">
         <f t="shared" si="0"/>
-        <v>8.94</v>
+        <v>4.47</v>
       </c>
       <c r="K17" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="L17" s="18" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="27" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="L17" s="18"/>
+    </row>
+    <row r="18" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
-        <v>57</v>
+        <v>86</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" s="21"/>
+        <v>87</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="25"/>
       <c r="E18" s="18" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="F18" s="16">
-        <v>2440</v>
+        <v>362104</v>
       </c>
       <c r="G18" s="15">
         <v>2</v>
       </c>
       <c r="H18" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="I18" s="17">
-        <v>6.9750000000000006E-2</v>
+        <v>4.47E-3</v>
       </c>
       <c r="J18" s="22">
         <f t="shared" si="0"/>
-        <v>139.5</v>
+        <v>4.47</v>
       </c>
       <c r="K18" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="L18" s="18" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="L18" s="18"/>
+    </row>
+    <row r="19" spans="1:12" ht="27" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="26"/>
+        <v>48</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>49</v>
+      </c>
       <c r="C19" s="21" t="s">
-        <v>83</v>
+        <v>50</v>
       </c>
       <c r="D19" s="21"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="16"/>
+      <c r="E19" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="16">
+        <v>2440</v>
+      </c>
       <c r="G19" s="15">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H19" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>5000</v>
-      </c>
-      <c r="I19" s="17"/>
+        <v>1000</v>
+      </c>
+      <c r="I19" s="17">
+        <v>6.9750000000000006E-2</v>
+      </c>
       <c r="J19" s="22">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>69.75</v>
       </c>
       <c r="K19" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="L19" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="L19" s="18"/>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="B20" s="26" t="s">
-        <v>61</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="B20" s="26"/>
       <c r="C20" s="21" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D20" s="21"/>
-      <c r="E20" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="F20" s="16">
-        <v>586403</v>
-      </c>
+      <c r="E20" s="18"/>
+      <c r="F20" s="16"/>
       <c r="G20" s="15">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H20" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>1000</v>
-      </c>
-      <c r="I20" s="17">
-        <v>5.9799999999999999E-2</v>
-      </c>
+        <v>2500</v>
+      </c>
+      <c r="I20" s="17"/>
       <c r="J20" s="22">
         <f t="shared" si="0"/>
-        <v>59.8</v>
+        <v>0</v>
       </c>
       <c r="K20" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="L20" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="27" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="L20"/>
+    </row>
+    <row r="21" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" s="25"/>
+        <v>52</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="21"/>
       <c r="E21" s="18" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="F21" s="16">
-        <v>22159</v>
+        <v>586403</v>
       </c>
       <c r="G21" s="15">
         <v>1</v>
       </c>
       <c r="H21" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I21" s="17">
-        <v>9.4759999999999997E-2</v>
+        <v>5.9799999999999999E-2</v>
       </c>
       <c r="J21" s="22">
         <f t="shared" si="0"/>
-        <v>94.759999999999991</v>
+        <v>29.9</v>
       </c>
       <c r="K21" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="L21" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="27" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="L21"/>
+    </row>
+    <row r="22" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
-        <v>36</v>
+        <v>96</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="C22" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="D22" s="21"/>
+        <v>97</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>112</v>
+      </c>
       <c r="E22" s="18" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="F22" s="16">
-        <v>4000</v>
+        <v>34988</v>
       </c>
       <c r="G22" s="15">
         <v>1</v>
       </c>
       <c r="H22" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I22" s="17">
-        <v>0.3024</v>
+        <v>0.12328</v>
       </c>
       <c r="J22" s="22">
         <f t="shared" si="0"/>
-        <v>302.39999999999998</v>
+        <v>61.64</v>
       </c>
       <c r="K22" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="L22" t="s">
-        <v>123</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="L22"/>
     </row>
     <row r="23" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D23" s="21"/>
       <c r="E23" s="18" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F23" s="16">
         <v>112229</v>
@@ -2307,269 +2266,303 @@
       </c>
       <c r="H23" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="I23" s="17">
         <v>0.12870000000000001</v>
       </c>
       <c r="J23" s="22">
         <f t="shared" si="0"/>
-        <v>257.40000000000003</v>
+        <v>128.70000000000002</v>
       </c>
       <c r="K23" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="L23" t="s">
-        <v>130</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="L23"/>
     </row>
     <row r="24" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="B24" s="26" t="s">
-        <v>90</v>
+      <c r="B24" s="39" t="s">
+        <v>104</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="D24" s="25"/>
       <c r="E24" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F24" s="16">
-        <v>1439</v>
+        <v>17721</v>
       </c>
       <c r="G24" s="15">
         <v>1</v>
       </c>
-      <c r="H24" s="23">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>1000</v>
+      <c r="H24" s="40">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>500</v>
       </c>
       <c r="I24" s="17">
-        <v>0.8246</v>
+        <v>0.31540000000000001</v>
       </c>
       <c r="J24" s="22">
-        <f t="shared" si="0"/>
-        <v>824.6</v>
+        <f>SUM(I24*H24)</f>
+        <v>157.70000000000002</v>
       </c>
       <c r="K24" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="L24" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="L24" s="18"/>
+    </row>
+    <row r="25" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="B25" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="24"/>
-      <c r="E25" s="18" t="s">
-        <v>17</v>
-      </c>
       <c r="F25" s="16">
-        <v>1335</v>
+        <v>11252</v>
       </c>
       <c r="G25" s="15">
         <v>1</v>
       </c>
-      <c r="H25" s="23">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>1000</v>
+      <c r="H25" s="40">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>500</v>
       </c>
       <c r="I25" s="17">
-        <v>0.33</v>
+        <v>0.1449</v>
       </c>
       <c r="J25" s="22">
-        <f t="shared" si="0"/>
-        <v>330</v>
+        <f>SUM(I25*H25)</f>
+        <v>72.45</v>
       </c>
       <c r="K25" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="L25" t="s">
-        <v>127</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="L25" s="18"/>
     </row>
     <row r="26" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D26" s="25"/>
+        <v>111</v>
+      </c>
+      <c r="B26" s="26"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25" t="s">
+        <v>112</v>
+      </c>
       <c r="E26" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="F26" s="16">
-        <v>1375</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="F26" s="16"/>
       <c r="G26" s="15">
         <v>1</v>
       </c>
       <c r="H26" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>1000</v>
-      </c>
-      <c r="I26" s="17">
-        <v>0.95</v>
-      </c>
+        <v>500</v>
+      </c>
+      <c r="I26" s="17"/>
       <c r="J26" s="22">
-        <f t="shared" ref="J26:J69" si="1">SUM(I26*H26)</f>
-        <v>950</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="K26" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="L26" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="54" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="L26"/>
+    </row>
+    <row r="27" spans="1:12" ht="27" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
-        <v>115</v>
+        <v>15</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="D27" s="25"/>
+        <v>14</v>
+      </c>
+      <c r="C27" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>112</v>
+      </c>
       <c r="E27" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F27" s="16"/>
+        <v>16</v>
+      </c>
+      <c r="F27" s="16">
+        <v>25844</v>
+      </c>
       <c r="G27" s="15">
         <v>1</v>
       </c>
       <c r="H27" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I27" s="17">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="J27" s="22">
+        <f t="shared" si="0"/>
+        <v>206</v>
+      </c>
+      <c r="K27" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="L27"/>
+    </row>
+    <row r="28" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="B28" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="E28" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" s="32">
+        <v>3261</v>
+      </c>
+      <c r="G28" s="33">
+        <v>1</v>
+      </c>
+      <c r="H28" s="34">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>500</v>
+      </c>
+      <c r="I28" s="35">
+        <v>0.1326</v>
+      </c>
+      <c r="J28" s="36">
+        <f>SUM(I28*H28)</f>
+        <v>66.3</v>
+      </c>
+      <c r="K28" s="31"/>
+      <c r="L28" s="31"/>
+    </row>
+    <row r="29" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="C29" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="D29" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" s="16">
+        <v>990</v>
+      </c>
+      <c r="G29" s="15">
+        <v>1</v>
+      </c>
+      <c r="H29" s="23">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>500</v>
+      </c>
+      <c r="I29" s="17">
+        <v>1.34714</v>
+      </c>
+      <c r="J29" s="22">
+        <f t="shared" ref="J29:J72" si="1">SUM(I29*H29)</f>
+        <v>673.57</v>
+      </c>
+      <c r="K29" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="L29"/>
+    </row>
+    <row r="30" spans="1:12" ht="54" x14ac:dyDescent="0.25">
+      <c r="A30" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D30" s="25"/>
+      <c r="E30" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F30" s="16"/>
+      <c r="G30" s="15">
+        <v>1</v>
+      </c>
+      <c r="H30" s="23">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>500</v>
+      </c>
+      <c r="I30" s="17">
         <v>1.66</v>
       </c>
-      <c r="J27" s="22">
-        <f t="shared" si="1"/>
-        <v>1660</v>
-      </c>
-      <c r="K27" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="L27" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="B28" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="C28" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="D28" s="25"/>
-      <c r="E28" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="F28" s="16">
-        <v>19970</v>
-      </c>
-      <c r="G28" s="15">
+      <c r="J30" s="22">
+        <f t="shared" si="1"/>
+        <v>830</v>
+      </c>
+      <c r="K30" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="L30"/>
+    </row>
+    <row r="31" spans="1:12" ht="27" x14ac:dyDescent="0.25">
+      <c r="A31" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C31" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F31" s="16">
+        <v>4925</v>
+      </c>
+      <c r="G31" s="15">
         <v>1</v>
       </c>
-      <c r="H28" s="23">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>1000</v>
-      </c>
-      <c r="I28" s="17">
-        <v>0.38569999999999999</v>
-      </c>
-      <c r="J28" s="22">
-        <f t="shared" si="1"/>
-        <v>385.7</v>
-      </c>
-      <c r="K28" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="L28" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="20"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="23">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="I29" s="17"/>
-      <c r="J29" s="22">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K29" s="18"/>
-      <c r="L29" s="18"/>
-    </row>
-    <row r="30" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="20"/>
-      <c r="B30" s="19"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="23">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="I30" s="17"/>
-      <c r="J30" s="22">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K30" s="18"/>
-      <c r="L30" s="18"/>
-    </row>
-    <row r="31" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="20"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="15"/>
       <c r="H31" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="I31" s="17"/>
+        <v>500</v>
+      </c>
+      <c r="I31" s="17">
+        <v>0.83160000000000001</v>
+      </c>
       <c r="J31" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K31" s="18"/>
-      <c r="L31" s="18"/>
+        <v>415.8</v>
+      </c>
+      <c r="K31" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="L31"/>
     </row>
     <row r="32" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="20"/>
@@ -3345,7 +3338,7 @@
       </c>
       <c r="I70" s="17"/>
       <c r="J70" s="22">
-        <f t="shared" ref="J70:J133" si="2">SUM(I70*H70)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K70" s="18"/>
@@ -3365,7 +3358,7 @@
       </c>
       <c r="I71" s="17"/>
       <c r="J71" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K71" s="18"/>
@@ -3385,7 +3378,7 @@
       </c>
       <c r="I72" s="17"/>
       <c r="J72" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K72" s="18"/>
@@ -3405,7 +3398,7 @@
       </c>
       <c r="I73" s="17"/>
       <c r="J73" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="J73:J136" si="2">SUM(I73*H73)</f>
         <v>0</v>
       </c>
       <c r="K73" s="18"/>
@@ -4625,7 +4618,7 @@
       </c>
       <c r="I134" s="17"/>
       <c r="J134" s="22">
-        <f t="shared" ref="J134:J197" si="3">SUM(I134*H134)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K134" s="18"/>
@@ -4645,7 +4638,7 @@
       </c>
       <c r="I135" s="17"/>
       <c r="J135" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K135" s="18"/>
@@ -4665,7 +4658,7 @@
       </c>
       <c r="I136" s="17"/>
       <c r="J136" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K136" s="18"/>
@@ -4685,7 +4678,7 @@
       </c>
       <c r="I137" s="17"/>
       <c r="J137" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="J137:J200" si="3">SUM(I137*H137)</f>
         <v>0</v>
       </c>
       <c r="K137" s="18"/>
@@ -5905,7 +5898,7 @@
       </c>
       <c r="I198" s="17"/>
       <c r="J198" s="22">
-        <f t="shared" ref="J198:J200" si="4">SUM(I198*H198)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K198" s="18"/>
@@ -5925,7 +5918,7 @@
       </c>
       <c r="I199" s="17"/>
       <c r="J199" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K199" s="18"/>
@@ -5945,11 +5938,71 @@
       </c>
       <c r="I200" s="17"/>
       <c r="J200" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K200" s="18"/>
       <c r="L200" s="18"/>
+    </row>
+    <row r="201" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A201" s="20"/>
+      <c r="B201" s="19"/>
+      <c r="C201" s="25"/>
+      <c r="D201" s="25"/>
+      <c r="E201" s="18"/>
+      <c r="F201" s="16"/>
+      <c r="G201" s="15"/>
+      <c r="H201" s="23">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="I201" s="17"/>
+      <c r="J201" s="22">
+        <f t="shared" ref="J201:J203" si="4">SUM(I201*H201)</f>
+        <v>0</v>
+      </c>
+      <c r="K201" s="18"/>
+      <c r="L201" s="18"/>
+    </row>
+    <row r="202" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A202" s="20"/>
+      <c r="B202" s="19"/>
+      <c r="C202" s="25"/>
+      <c r="D202" s="25"/>
+      <c r="E202" s="18"/>
+      <c r="F202" s="16"/>
+      <c r="G202" s="15"/>
+      <c r="H202" s="23">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="I202" s="17"/>
+      <c r="J202" s="22">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K202" s="18"/>
+      <c r="L202" s="18"/>
+    </row>
+    <row r="203" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A203" s="20"/>
+      <c r="B203" s="19"/>
+      <c r="C203" s="25"/>
+      <c r="D203" s="25"/>
+      <c r="E203" s="18"/>
+      <c r="F203" s="16"/>
+      <c r="G203" s="15"/>
+      <c r="H203" s="23">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="I203" s="17"/>
+      <c r="J203" s="22">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K203" s="18"/>
+      <c r="L203" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5958,32 +6011,29 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2:J2" r:id="rId1" display=" Projects and Stuff LLC - http://ww.projectsandstuff.com"/>
-    <hyperlink ref="B25" r:id="rId2"/>
-    <hyperlink ref="B21" r:id="rId3"/>
-    <hyperlink ref="B6" r:id="rId4"/>
-    <hyperlink ref="B7" r:id="rId5"/>
-    <hyperlink ref="B26" r:id="rId6"/>
-    <hyperlink ref="B22" r:id="rId7"/>
-    <hyperlink ref="B8" r:id="rId8"/>
-    <hyperlink ref="B11" r:id="rId9"/>
-    <hyperlink ref="B12" r:id="rId10"/>
-    <hyperlink ref="B10" r:id="rId11"/>
-    <hyperlink ref="B23" r:id="rId12"/>
-    <hyperlink ref="B18" r:id="rId13"/>
-    <hyperlink ref="B20" r:id="rId14"/>
-    <hyperlink ref="B9" r:id="rId15"/>
-    <hyperlink ref="B13" r:id="rId16"/>
-    <hyperlink ref="B15" r:id="rId17"/>
-    <hyperlink ref="B28" r:id="rId18"/>
-    <hyperlink ref="B24" r:id="rId19"/>
-    <hyperlink ref="B14" r:id="rId20"/>
-    <hyperlink ref="B16" r:id="rId21"/>
-    <hyperlink ref="B17" r:id="rId22"/>
+    <hyperlink ref="B22" r:id="rId2"/>
+    <hyperlink ref="B7" r:id="rId3"/>
+    <hyperlink ref="B8" r:id="rId4"/>
+    <hyperlink ref="B9" r:id="rId5"/>
+    <hyperlink ref="B12" r:id="rId6"/>
+    <hyperlink ref="B13" r:id="rId7"/>
+    <hyperlink ref="B11" r:id="rId8"/>
+    <hyperlink ref="B23" r:id="rId9"/>
+    <hyperlink ref="B19" r:id="rId10"/>
+    <hyperlink ref="B21" r:id="rId11"/>
+    <hyperlink ref="B10" r:id="rId12"/>
+    <hyperlink ref="B14" r:id="rId13"/>
+    <hyperlink ref="B16" r:id="rId14"/>
+    <hyperlink ref="B31" r:id="rId15" display="ZX62-B-5PA(11)"/>
+    <hyperlink ref="B15" r:id="rId16"/>
+    <hyperlink ref="B17" r:id="rId17"/>
+    <hyperlink ref="B18" r:id="rId18"/>
+    <hyperlink ref="B27" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="47" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId23"/>
+  <pageSetup scale="47" orientation="landscape" r:id="rId20"/>
   <tableParts count="1">
-    <tablePart r:id="rId24"/>
+    <tablePart r:id="rId21"/>
   </tableParts>
 </worksheet>
 </file>
@@ -6012,16 +6062,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
+      <c r="A1" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
       <c r="I1" s="8" t="s">
         <v>4</v>
       </c>
@@ -6030,16 +6080,16 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
     </row>
@@ -6106,13 +6156,13 @@
     </row>
     <row r="6" spans="1:10" ht="54" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="D6" s="16"/>
       <c r="E6" s="15">
@@ -6130,13 +6180,13 @@
         <v>240</v>
       </c>
       <c r="I6" s="18" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="J6"/>
     </row>
     <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="B7" s="26"/>
       <c r="C7" s="18"/>
@@ -6156,11 +6206,11 @@
     </row>
     <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="B8" s="26"/>
       <c r="C8" s="18" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="15">

</xml_diff>

<commit_message>
Updated BOM with current prices and mostly 0603 packages for discrete components.
</commit_message>
<xml_diff>
--- a/Notes/Chameleon BOM.xlsx
+++ b/Notes/Chameleon BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24240" windowHeight="12075"/>
+    <workbookView xWindow="120" yWindow="210" windowWidth="24240" windowHeight="12015"/>
   </bookViews>
   <sheets>
     <sheet name="Electronics" sheetId="1" r:id="rId1"/>
@@ -13,14 +13,14 @@
   <definedNames>
     <definedName name="Goal" localSheetId="1">Other!$J$1</definedName>
     <definedName name="Goal">Electronics!$L$1</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Electronics!$A$1:$L$31</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Electronics!$A$1:$L$34</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="123">
   <si>
     <t>Mfg Part #</t>
   </si>
@@ -73,9 +73,6 @@
     <t>Digikey</t>
   </si>
   <si>
-    <t>Also available at Newark, Farnell, Avnet, Verical, etc</t>
-  </si>
-  <si>
     <t>SOT-23-3</t>
   </si>
   <si>
@@ -85,15 +82,6 @@
     <t>Input Capacitor used with Boost Regulator</t>
   </si>
   <si>
-    <t>C3216Y5V1A106Z/0.85</t>
-  </si>
-  <si>
-    <t>Capacitor Ceramic 10uF 10V Y5V</t>
-  </si>
-  <si>
-    <t>Also available at Digikey and Verical</t>
-  </si>
-  <si>
     <t>IC LED Driver RGBA</t>
   </si>
   <si>
@@ -112,36 +100,15 @@
     <t>DigiKey</t>
   </si>
   <si>
-    <t>CC0805DRNPO9BN8R0</t>
-  </si>
-  <si>
-    <t>0805</t>
-  </si>
-  <si>
-    <t>Capacitor Ceramic 8pF 50V</t>
-  </si>
-  <si>
-    <t>Used for Crystal loading</t>
-  </si>
-  <si>
     <t>PLCC-6 RGB LED</t>
   </si>
   <si>
     <t>LED Lighting</t>
   </si>
   <si>
-    <t>RC1206JR-071KL</t>
-  </si>
-  <si>
     <t>Used for QMatrix X&amp;Y line resistors</t>
   </si>
   <si>
-    <t>Resistor 470K OHM 1/4W 5%</t>
-  </si>
-  <si>
-    <t>RC1206JR-07470KL</t>
-  </si>
-  <si>
     <t>1206</t>
   </si>
   <si>
@@ -151,12 +118,6 @@
     <t>Capacitor Ceramic 4.7nF 50V 10%</t>
   </si>
   <si>
-    <t>CC1206KRX7R9BB472</t>
-  </si>
-  <si>
-    <t>Used for QMatrix RY line capacitors</t>
-  </si>
-  <si>
     <t>Switch Tactile SPST-NO 0.05A 15V</t>
   </si>
   <si>
@@ -178,48 +139,18 @@
     <t>LED Red Diffused</t>
   </si>
   <si>
-    <t>LH N974-KN-1</t>
-  </si>
-  <si>
-    <t>Capacitor Ceramic 0.1uF 50V 10%</t>
-  </si>
-  <si>
-    <t>GRM319R71H104KA01D</t>
-  </si>
-  <si>
     <t>Used for Power Input/Output filtering and Decoupling</t>
   </si>
   <si>
-    <t>RC1206JR-07220RL</t>
-  </si>
-  <si>
-    <t>Resistor 220Ω 1/4W 5%</t>
-  </si>
-  <si>
-    <t>Resistor 10kΩ 1/4W 5%</t>
-  </si>
-  <si>
-    <t>RC1206JR-0710KL</t>
-  </si>
-  <si>
-    <t>Pull-up resistors</t>
-  </si>
-  <si>
     <t>USB - Micro B</t>
   </si>
   <si>
     <t>Connector Receptical USB Micro B</t>
   </si>
   <si>
-    <t>JMK316BJ476ML-T</t>
-  </si>
-  <si>
     <t>Capacitor Ceramic 47uF 6.3V 20%</t>
   </si>
   <si>
-    <t>Used with AVR Analog Reference Filtering and Boost Regulator</t>
-  </si>
-  <si>
     <t>AVR Reset and Mode Switch</t>
   </si>
   <si>
@@ -247,18 +178,6 @@
     <t>(Similar also available at http://www.packagingsupplies.com/White_Corrugated_Boxes__Mailers.html - they're cheaper, but may not be enough on hand)</t>
   </si>
   <si>
-    <t>Resistor 330Ω 1/4W 5%</t>
-  </si>
-  <si>
-    <t>RC1206JR-07330RL</t>
-  </si>
-  <si>
-    <t>Current Limiting for Blue &amp; Green LEDs (Any resistor around 220 Ohms and with the same package will do)</t>
-  </si>
-  <si>
-    <t>Current Limiting for Red LEDs (Any resistor around 330 Ohms and with the same package will do)</t>
-  </si>
-  <si>
     <t>Plastic Case</t>
   </si>
   <si>
@@ -271,27 +190,6 @@
     <t>KiCad Footprint</t>
   </si>
   <si>
-    <t>Pull-up and series resistors for I2C SCK and SDA lines</t>
-  </si>
-  <si>
-    <t>Resistor 1.8kΩ 1/4W 5%</t>
-  </si>
-  <si>
-    <t>RC1206JR-071K8L</t>
-  </si>
-  <si>
-    <t>Resistor 100Ω 1/4W 5%</t>
-  </si>
-  <si>
-    <t>RC1206JR-07100RL</t>
-  </si>
-  <si>
-    <t>Series resistors for SCK and SDA lines</t>
-  </si>
-  <si>
-    <t>Resistor 1kΩ 1/4W 5%</t>
-  </si>
-  <si>
     <t>Battery (Li-Poly 3.7V 500mAh)</t>
   </si>
   <si>
@@ -359,6 +257,138 @@
   </si>
   <si>
     <t>GOOD</t>
+  </si>
+  <si>
+    <t>LED White</t>
+  </si>
+  <si>
+    <t>0603</t>
+  </si>
+  <si>
+    <t>AliExpress</t>
+  </si>
+  <si>
+    <t>White LED Lighting</t>
+  </si>
+  <si>
+    <t>Fuse PTC 500mA</t>
+  </si>
+  <si>
+    <t>MF-FSMF050X-2</t>
+  </si>
+  <si>
+    <t>Ferrite Bead</t>
+  </si>
+  <si>
+    <t>BK0603HS330-T</t>
+  </si>
+  <si>
+    <t>Analog Input filtering for uC</t>
+  </si>
+  <si>
+    <t>Protects USB from drawing too much current</t>
+  </si>
+  <si>
+    <t>Also available at Newark, Farnell, Avnet, Verical, etc. Used for powering LEDs</t>
+  </si>
+  <si>
+    <t>Provides power for digital components and White LEDs</t>
+  </si>
+  <si>
+    <t>GRM31CR60J476ME19L</t>
+  </si>
+  <si>
+    <t>Capacitor Ceramic 10uF 6.3V X5R</t>
+  </si>
+  <si>
+    <t>CL10A106MQ8NNNC</t>
+  </si>
+  <si>
+    <t>RC1608J121CS</t>
+  </si>
+  <si>
+    <t>Current limiting resistors for White LEDs</t>
+  </si>
+  <si>
+    <t>RC1608J103CS</t>
+  </si>
+  <si>
+    <t>Resistor 10kΩ 1/10W 5%</t>
+  </si>
+  <si>
+    <t>Pull-up/down resistors</t>
+  </si>
+  <si>
+    <t>Capacitor Ceramic 1nF</t>
+  </si>
+  <si>
+    <t>Resistor 120Ω 1/10W 5%</t>
+  </si>
+  <si>
+    <t>Resistor 4kΩ</t>
+  </si>
+  <si>
+    <t>Provides Current Bias for the As1121</t>
+  </si>
+  <si>
+    <t>Used for QMatrix RY line capacitors and USB Shield Termination</t>
+  </si>
+  <si>
+    <t>Part of USB Shield Termination</t>
+  </si>
+  <si>
+    <t>Input Filtering for uC Power</t>
+  </si>
+  <si>
+    <t>Filtering for LEDs</t>
+  </si>
+  <si>
+    <t>CL10B102KB8SFNC</t>
+  </si>
+  <si>
+    <t>CL10B472KB8SFNC</t>
+  </si>
+  <si>
+    <t>CL10B104KO8NNNC</t>
+  </si>
+  <si>
+    <t>Capacitor Ceramic 0.1uF 16V 10%</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>RC0603JR-071KL</t>
+  </si>
+  <si>
+    <t>Resistor 1kΩ 1/10W 5%</t>
+  </si>
+  <si>
+    <t>RC1608J474CS</t>
+  </si>
+  <si>
+    <t>RC1608J392CS</t>
+  </si>
+  <si>
+    <t>Resistor 470KΩ 1/10W 5%</t>
+  </si>
+  <si>
+    <t>RC1608F1054CS</t>
+  </si>
+  <si>
+    <t>Resistor 1.05MΩ 1/10W 1%</t>
+  </si>
+  <si>
+    <t>LB3218T100K</t>
+  </si>
+  <si>
+    <t>Inductor 10uH 340mA 10%</t>
+  </si>
+  <si>
+    <t>Used with Boost Regulator Input</t>
+  </si>
+  <si>
+    <t>LS L29K-G1J2-1-Z</t>
   </si>
 </sst>
 </file>
@@ -464,6 +494,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Lucida Sans Unicode"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -484,11 +515,13 @@
       <sz val="9"/>
       <color theme="1"/>
       <name val="Lucida Sans Unicode"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Lucida Sans Unicode"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -496,6 +529,7 @@
       <sz val="9"/>
       <color theme="0" tint="-0.499984740745262"/>
       <name val="Lucida Sans Unicode"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1188,8 +1222,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A6:L203" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
-  <autoFilter ref="A6:L203"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A6:L206" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+  <autoFilter ref="A6:L206"/>
   <tableColumns count="12">
     <tableColumn id="1" name="Description" dataDxfId="23"/>
     <tableColumn id="2" name="Mfg Part #" dataDxfId="22"/>
@@ -1525,10 +1559,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L203"/>
+  <dimension ref="A1:L206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1550,7 +1584,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="41" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="B1" s="41"/>
       <c r="C1" s="41"/>
@@ -1603,15 +1637,15 @@
         <v>11</v>
       </c>
       <c r="B4" s="37">
-        <f>SUM(J7:J203)</f>
-        <v>3027.59</v>
+        <f>SUM(J7:J206)</f>
+        <v>3148.8249999999998</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>99</v>
+        <v>65</v>
       </c>
       <c r="D4" s="37">
         <f>B4/Goal</f>
-        <v>6.05518</v>
+        <v>6.29765</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
@@ -1647,7 +1681,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>12</v>
@@ -1674,58 +1708,62 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>63</v>
+        <v>107</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="21"/>
+        <v>80</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>78</v>
+      </c>
       <c r="E7" s="18" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F7" s="16">
-        <v>186142</v>
+        <v>80889</v>
       </c>
       <c r="G7" s="15">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H7" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>500</v>
+        <v>5500</v>
       </c>
       <c r="I7" s="17">
-        <v>0.28799999999999998</v>
+        <v>3.3899999999999998E-3</v>
       </c>
       <c r="J7" s="22">
-        <f t="shared" ref="J7:J27" si="0">SUM(I7*H7)</f>
-        <v>144</v>
+        <f>SUM(I7*H7)</f>
+        <v>18.645</v>
       </c>
       <c r="K7" s="18" t="s">
-        <v>19</v>
+        <v>106</v>
       </c>
       <c r="L7"/>
     </row>
-    <row r="8" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="27" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="26" t="s">
-        <v>21</v>
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>108</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="21"/>
+        <v>80</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>78</v>
+      </c>
       <c r="E8" s="18" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F8" s="16">
-        <v>116496</v>
+        <v>8836</v>
       </c>
       <c r="G8" s="15">
         <v>2</v>
@@ -1735,86 +1773,90 @@
         <v>1000</v>
       </c>
       <c r="I8" s="17">
-        <v>3.8249999999999999E-2</v>
+        <v>6.1799999999999997E-3</v>
       </c>
       <c r="J8" s="22">
-        <f t="shared" si="0"/>
-        <v>38.25</v>
+        <f>SUM(I8*H8)</f>
+        <v>6.18</v>
       </c>
       <c r="K8" s="18" t="s">
-        <v>20</v>
+        <v>103</v>
       </c>
       <c r="L8"/>
     </row>
-    <row r="9" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="27" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="26" t="s">
-        <v>30</v>
+        <v>110</v>
+      </c>
+      <c r="B9" t="s">
+        <v>109</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="21"/>
+        <v>80</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>78</v>
+      </c>
       <c r="E9" s="18" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F9" s="16">
-        <v>7417</v>
+        <v>3312000</v>
       </c>
       <c r="G9" s="15">
+        <v>8</v>
+      </c>
+      <c r="H9" s="23">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>4000</v>
+      </c>
+      <c r="I9" s="17">
+        <v>3.5899999999999999E-3</v>
+      </c>
+      <c r="J9" s="22">
+        <f>SUM(I9*H9)</f>
+        <v>14.36</v>
+      </c>
+      <c r="K9" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="L9"/>
+    </row>
+    <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="16">
+        <v>167415</v>
+      </c>
+      <c r="G10" s="15">
         <v>2</v>
       </c>
-      <c r="H9" s="23">
+      <c r="H10" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
         <v>1000</v>
       </c>
-      <c r="I9" s="17">
-        <v>1.6500000000000001E-2</v>
-      </c>
-      <c r="J9" s="22">
-        <f t="shared" si="0"/>
-        <v>16.5</v>
-      </c>
-      <c r="K9" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="L9"/>
-    </row>
-    <row r="10" spans="1:12" ht="27" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="B10" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" s="21">
-        <v>1206</v>
-      </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="16">
-        <v>310439</v>
-      </c>
-      <c r="G10" s="15">
-        <v>9</v>
-      </c>
-      <c r="H10" s="23">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>4500</v>
-      </c>
       <c r="I10" s="17">
-        <v>1.4069999999999999E-2</v>
+        <v>4.65E-2</v>
       </c>
       <c r="J10" s="22">
-        <f t="shared" si="0"/>
-        <v>63.314999999999998</v>
+        <f>SUM(I10*H10)</f>
+        <v>46.5</v>
       </c>
       <c r="K10" s="18" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="L10"/>
     </row>
@@ -1822,18 +1864,20 @@
       <c r="A11" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="21">
-        <v>1206</v>
-      </c>
-      <c r="D11" s="21"/>
+      <c r="B11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>78</v>
+      </c>
       <c r="E11" s="18" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="F11" s="16">
-        <v>55807</v>
+        <v>151601</v>
       </c>
       <c r="G11" s="15">
         <v>1</v>
@@ -1843,141 +1887,149 @@
         <v>500</v>
       </c>
       <c r="I11" s="17">
-        <v>2.52E-2</v>
+        <v>0.19846</v>
       </c>
       <c r="J11" s="22">
-        <f t="shared" si="0"/>
-        <v>12.6</v>
+        <f t="shared" ref="J11:J29" si="0">SUM(I11*H11)</f>
+        <v>99.23</v>
       </c>
       <c r="K11" s="18" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="L11"/>
     </row>
     <row r="12" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="B12" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="21">
-        <v>1206</v>
-      </c>
-      <c r="D12" s="21"/>
+        <v>100</v>
+      </c>
+      <c r="B12" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>78</v>
+      </c>
       <c r="E12" s="18" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="F12" s="16">
-        <v>151361</v>
+        <v>9886</v>
       </c>
       <c r="G12" s="15">
-        <v>2</v>
-      </c>
-      <c r="H12" s="23">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>1000</v>
+        <v>5</v>
+      </c>
+      <c r="H12" s="40">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>2500</v>
       </c>
       <c r="I12" s="17">
-        <v>4.47E-3</v>
+        <v>1.74E-3</v>
       </c>
       <c r="J12" s="22">
-        <f t="shared" si="0"/>
-        <v>4.47</v>
+        <f>SUM(I12*H12)</f>
+        <v>4.3499999999999996</v>
       </c>
       <c r="K12" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="L12"/>
+        <v>95</v>
+      </c>
+      <c r="L12" s="18"/>
     </row>
     <row r="13" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="26" t="s">
-        <v>39</v>
+        <v>113</v>
+      </c>
+      <c r="B13" t="s">
+        <v>112</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="21"/>
+        <v>80</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>78</v>
+      </c>
       <c r="E13" s="18" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F13" s="16">
-        <v>38808</v>
+        <v>38481</v>
       </c>
       <c r="G13" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H13" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="I13" s="17">
-        <v>4.47E-3</v>
+        <v>2.0699999999999998E-3</v>
       </c>
       <c r="J13" s="22">
         <f t="shared" si="0"/>
-        <v>2.2349999999999999</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="K13" s="18" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="L13"/>
     </row>
-    <row r="14" spans="1:12" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B14" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="21">
-        <v>1206</v>
-      </c>
-      <c r="D14" s="21"/>
+        <v>101</v>
+      </c>
+      <c r="B14" s="39" t="s">
+        <v>115</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>78</v>
+      </c>
       <c r="E14" s="18" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F14" s="16">
-        <v>100000</v>
+        <v>9400</v>
       </c>
       <c r="G14" s="15">
-        <v>10</v>
-      </c>
-      <c r="H14" s="23">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>5000</v>
+        <v>1</v>
+      </c>
+      <c r="H14" s="40">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>500</v>
       </c>
       <c r="I14" s="17">
-        <v>2.8300000000000001E-3</v>
+        <v>2.7399999999999998E-3</v>
       </c>
       <c r="J14" s="22">
-        <f t="shared" si="0"/>
-        <v>14.15</v>
+        <f>SUM(I14*H14)</f>
+        <v>1.3699999999999999</v>
       </c>
       <c r="K14" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="L14"/>
-    </row>
-    <row r="15" spans="1:12" ht="40.5" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="L14" s="18"/>
+    </row>
+    <row r="15" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="B15" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="C15" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="25"/>
+        <v>97</v>
+      </c>
+      <c r="B15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>78</v>
+      </c>
       <c r="E15" s="18" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F15" s="16">
-        <v>625000</v>
+        <v>3129</v>
       </c>
       <c r="G15" s="15">
         <v>6</v>
@@ -1987,563 +2039,577 @@
         <v>3000</v>
       </c>
       <c r="I15" s="17">
-        <v>2.8300000000000001E-3</v>
+        <v>2.0100000000000001E-3</v>
       </c>
       <c r="J15" s="22">
         <f t="shared" si="0"/>
-        <v>8.49</v>
+        <v>6.03</v>
       </c>
       <c r="K15" s="18" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="L15"/>
     </row>
     <row r="16" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="B16" s="26" t="s">
-        <v>59</v>
+        <v>116</v>
+      </c>
+      <c r="B16" t="s">
+        <v>114</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="21"/>
+        <v>80</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>78</v>
+      </c>
       <c r="E16" s="18" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F16" s="16">
-        <v>1480000</v>
+        <v>10000</v>
       </c>
       <c r="G16" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H16" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I16" s="17">
-        <v>2.8300000000000001E-3</v>
+        <v>2.7399999999999998E-3</v>
       </c>
       <c r="J16" s="22">
-        <f t="shared" si="0"/>
-        <v>2.83</v>
+        <f>SUM(I16*H16)</f>
+        <v>1.3699999999999999</v>
       </c>
       <c r="K16" s="18" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="L16"/>
     </row>
-    <row r="17" spans="1:12" ht="27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="B17" s="26" t="s">
-        <v>85</v>
+        <v>118</v>
+      </c>
+      <c r="B17" s="39" t="s">
+        <v>117</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="25"/>
+        <v>80</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>78</v>
+      </c>
       <c r="E17" s="18" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F17" s="16">
-        <v>141711</v>
+        <v>9475</v>
       </c>
       <c r="G17" s="15">
-        <v>2</v>
-      </c>
-      <c r="H17" s="23">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>1000</v>
+        <v>1</v>
+      </c>
+      <c r="H17" s="40">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>500</v>
       </c>
       <c r="I17" s="17">
-        <v>4.47E-3</v>
+        <v>2.0600000000000002E-3</v>
       </c>
       <c r="J17" s="22">
-        <f t="shared" si="0"/>
-        <v>4.47</v>
+        <f>SUM(I17*H17)</f>
+        <v>1.03</v>
       </c>
       <c r="K17" s="18" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="L17" s="18"/>
     </row>
     <row r="18" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="B18" s="26" t="s">
-        <v>87</v>
+        <v>120</v>
+      </c>
+      <c r="B18" s="39" t="s">
+        <v>119</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="25"/>
+        <v>37</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>78</v>
+      </c>
       <c r="E18" s="18" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F18" s="16">
-        <v>362104</v>
+        <v>19931</v>
       </c>
       <c r="G18" s="15">
-        <v>2</v>
-      </c>
-      <c r="H18" s="23">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>1000</v>
+        <v>1</v>
+      </c>
+      <c r="H18" s="40">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>500</v>
       </c>
       <c r="I18" s="17">
-        <v>4.47E-3</v>
+        <v>8.5260000000000002E-2</v>
       </c>
       <c r="J18" s="22">
-        <f t="shared" si="0"/>
-        <v>4.47</v>
+        <f>SUM(I18*H18)</f>
+        <v>42.63</v>
       </c>
       <c r="K18" s="18" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="L18" s="18"/>
     </row>
-    <row r="19" spans="1:12" ht="27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" s="26" t="s">
-        <v>49</v>
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="21"/>
+        <v>37</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>78</v>
+      </c>
       <c r="E19" s="18" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F19" s="16">
-        <v>2440</v>
+        <v>3051</v>
       </c>
       <c r="G19" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H19" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I19" s="17">
-        <v>6.9750000000000006E-2</v>
+        <v>8.5260000000000002E-2</v>
       </c>
       <c r="J19" s="22">
         <f t="shared" si="0"/>
-        <v>69.75</v>
+        <v>42.63</v>
       </c>
       <c r="K19" s="18" t="s">
-        <v>65</v>
+        <v>121</v>
       </c>
       <c r="L19" s="18"/>
     </row>
-    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="26"/>
-      <c r="C20" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="D20" s="21"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="16"/>
+        <v>85</v>
+      </c>
+      <c r="B20" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="16">
+        <v>22721</v>
+      </c>
       <c r="G20" s="15">
+        <v>1</v>
+      </c>
+      <c r="H20" s="40">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>500</v>
+      </c>
+      <c r="I20" s="17">
+        <v>4.5539999999999997E-2</v>
+      </c>
+      <c r="J20" s="22">
+        <f>SUM(I20*H20)</f>
+        <v>22.77</v>
+      </c>
+      <c r="K20" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="L20" s="18"/>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="26"/>
+      <c r="C21" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="E21" s="18"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="15">
         <v>5</v>
       </c>
-      <c r="H20" s="23">
+      <c r="H21" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
         <v>2500</v>
       </c>
-      <c r="I20" s="17"/>
-      <c r="J20" s="22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K20" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="L20"/>
-    </row>
-    <row r="21" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="B21" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" s="21"/>
-      <c r="E21" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="F21" s="16">
-        <v>586403</v>
-      </c>
-      <c r="G21" s="15">
-        <v>1</v>
-      </c>
-      <c r="H21" s="23">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>500</v>
-      </c>
-      <c r="I21" s="17">
-        <v>5.9799999999999999E-2</v>
-      </c>
+      <c r="I21" s="17"/>
       <c r="J21" s="22">
         <f t="shared" si="0"/>
-        <v>29.9</v>
+        <v>0</v>
       </c>
       <c r="K21" s="18" t="s">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="L21"/>
     </row>
-    <row r="22" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="B22" s="26" t="s">
-        <v>97</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="B22" s="39"/>
       <c r="C22" s="25" t="s">
-        <v>18</v>
+        <v>80</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E22" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22" s="16"/>
+      <c r="G22" s="15">
+        <v>5</v>
+      </c>
+      <c r="H22" s="40">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>2500</v>
+      </c>
+      <c r="I22" s="17">
+        <v>0.03</v>
+      </c>
+      <c r="J22" s="22">
+        <f>SUM(I22*H22)</f>
+        <v>75</v>
+      </c>
+      <c r="K22" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="L22" s="18"/>
+    </row>
+    <row r="23" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" t="s">
+        <v>122</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="16">
+        <v>63971</v>
+      </c>
+      <c r="G23" s="15">
+        <v>1</v>
+      </c>
+      <c r="H23" s="23">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>500</v>
+      </c>
+      <c r="I23" s="17">
+        <v>9.1399999999999995E-2</v>
+      </c>
+      <c r="J23" s="22">
+        <f t="shared" si="0"/>
+        <v>45.699999999999996</v>
+      </c>
+      <c r="K23" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="L23"/>
+    </row>
+    <row r="24" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="E24" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="16">
+      <c r="F24" s="16">
         <v>34988</v>
       </c>
-      <c r="G22" s="15">
+      <c r="G24" s="15">
         <v>1</v>
       </c>
-      <c r="H22" s="23">
+      <c r="H24" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
         <v>500</v>
       </c>
-      <c r="I22" s="17">
+      <c r="I24" s="17">
         <v>0.12328</v>
       </c>
-      <c r="J22" s="22">
+      <c r="J24" s="22">
         <f t="shared" si="0"/>
         <v>61.64</v>
       </c>
-      <c r="K22" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="L22"/>
-    </row>
-    <row r="23" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="D23" s="21"/>
-      <c r="E23" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="F23" s="16">
+      <c r="K24" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="L24"/>
+    </row>
+    <row r="25" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="21"/>
+      <c r="E25" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="16">
         <v>112229</v>
       </c>
-      <c r="G23" s="15">
+      <c r="G25" s="15">
         <v>2</v>
       </c>
-      <c r="H23" s="23">
+      <c r="H25" s="23">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
         <v>1000</v>
       </c>
-      <c r="I23" s="17">
+      <c r="I25" s="17">
         <v>0.12870000000000001</v>
       </c>
-      <c r="J23" s="22">
+      <c r="J25" s="22">
         <f t="shared" si="0"/>
         <v>128.70000000000002</v>
       </c>
-      <c r="K23" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="L23"/>
-    </row>
-    <row r="24" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="B24" s="39" t="s">
-        <v>104</v>
-      </c>
-      <c r="C24" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="D24" s="25"/>
-      <c r="E24" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F24" s="16">
-        <v>17721</v>
-      </c>
-      <c r="G24" s="15">
-        <v>1</v>
-      </c>
-      <c r="H24" s="40">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>500</v>
-      </c>
-      <c r="I24" s="17">
-        <v>0.31540000000000001</v>
-      </c>
-      <c r="J24" s="22">
-        <f>SUM(I24*H24)</f>
-        <v>157.70000000000002</v>
-      </c>
-      <c r="K24" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="L24" s="18"/>
-    </row>
-    <row r="25" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="B25" s="39" t="s">
-        <v>108</v>
-      </c>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25" s="16">
-        <v>11252</v>
-      </c>
-      <c r="G25" s="15">
-        <v>1</v>
-      </c>
-      <c r="H25" s="40">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>500</v>
-      </c>
-      <c r="I25" s="17">
-        <v>0.1449</v>
-      </c>
-      <c r="J25" s="22">
-        <f>SUM(I25*H25)</f>
-        <v>72.45</v>
-      </c>
       <c r="K25" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="L25" s="18"/>
+        <v>43</v>
+      </c>
+      <c r="L25"/>
     </row>
     <row r="26" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="B26" s="26"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25" t="s">
-        <v>112</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="B26" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" s="25"/>
       <c r="E26" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="F26" s="16"/>
+      <c r="F26" s="16">
+        <v>17721</v>
+      </c>
       <c r="G26" s="15">
         <v>1</v>
       </c>
-      <c r="H26" s="23">
+      <c r="H26" s="40">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
         <v>500</v>
       </c>
-      <c r="I26" s="17"/>
+      <c r="I26" s="17">
+        <v>0.31540000000000001</v>
+      </c>
       <c r="J26" s="22">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>SUM(I26*H26)</f>
+        <v>157.70000000000002</v>
       </c>
       <c r="K26" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="L26"/>
-    </row>
-    <row r="27" spans="1:12" ht="27" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="L26" s="18"/>
+    </row>
+    <row r="27" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="B27" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="D27" s="25" t="s">
-        <v>112</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="B27" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
       <c r="E27" s="18" t="s">
         <v>16</v>
       </c>
       <c r="F27" s="16">
-        <v>25844</v>
+        <v>11252</v>
       </c>
       <c r="G27" s="15">
         <v>1</v>
       </c>
-      <c r="H27" s="23">
+      <c r="H27" s="40">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
         <v>500</v>
       </c>
       <c r="I27" s="17">
+        <v>0.1449</v>
+      </c>
+      <c r="J27" s="22">
+        <f>SUM(I27*H27)</f>
+        <v>72.45</v>
+      </c>
+      <c r="K27" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="L27" s="18"/>
+    </row>
+    <row r="28" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" s="26"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" s="16"/>
+      <c r="G28" s="15">
+        <v>1</v>
+      </c>
+      <c r="H28" s="23">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>500</v>
+      </c>
+      <c r="I28" s="17"/>
+      <c r="J28" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K28" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="L28"/>
+    </row>
+    <row r="29" spans="1:12" ht="27" x14ac:dyDescent="0.25">
+      <c r="A29" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" s="16">
+        <v>25844</v>
+      </c>
+      <c r="G29" s="15">
+        <v>1</v>
+      </c>
+      <c r="H29" s="23">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>500</v>
+      </c>
+      <c r="I29" s="17">
         <v>0.41199999999999998</v>
       </c>
-      <c r="J27" s="22">
+      <c r="J29" s="22">
         <f t="shared" si="0"/>
         <v>206</v>
       </c>
-      <c r="K27" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="L27"/>
-    </row>
-    <row r="28" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="B28" s="39" t="s">
-        <v>94</v>
-      </c>
-      <c r="C28" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="D28" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="E28" s="31" t="s">
+      <c r="K29" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="L29"/>
+    </row>
+    <row r="30" spans="1:12" ht="27" x14ac:dyDescent="0.25">
+      <c r="A30" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="E30" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F28" s="32">
+      <c r="F30" s="32">
         <v>3261</v>
       </c>
-      <c r="G28" s="33">
+      <c r="G30" s="33">
         <v>1</v>
       </c>
-      <c r="H28" s="34">
+      <c r="H30" s="34">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
         <v>500</v>
       </c>
-      <c r="I28" s="35">
+      <c r="I30" s="35">
         <v>0.1326</v>
       </c>
-      <c r="J28" s="36">
-        <f>SUM(I28*H28)</f>
+      <c r="J30" s="36">
+        <f>SUM(I30*H30)</f>
         <v>66.3</v>
       </c>
-      <c r="K28" s="31"/>
-      <c r="L28" s="31"/>
-    </row>
-    <row r="29" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" s="26" t="s">
-        <v>100</v>
-      </c>
-      <c r="C29" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="D29" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="E29" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F29" s="16">
-        <v>990</v>
-      </c>
-      <c r="G29" s="15">
-        <v>1</v>
-      </c>
-      <c r="H29" s="23">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>500</v>
-      </c>
-      <c r="I29" s="17">
-        <v>1.34714</v>
-      </c>
-      <c r="J29" s="22">
-        <f t="shared" ref="J29:J72" si="1">SUM(I29*H29)</f>
-        <v>673.57</v>
-      </c>
-      <c r="K29" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="L29"/>
-    </row>
-    <row r="30" spans="1:12" ht="54" x14ac:dyDescent="0.25">
-      <c r="A30" s="20" t="s">
+      <c r="K30" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="B30" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="C30" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="D30" s="25"/>
-      <c r="E30" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="F30" s="16"/>
-      <c r="G30" s="15">
-        <v>1</v>
-      </c>
-      <c r="H30" s="23">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>500</v>
-      </c>
-      <c r="I30" s="17">
-        <v>1.66</v>
-      </c>
-      <c r="J30" s="22">
-        <f t="shared" si="1"/>
-        <v>830</v>
-      </c>
-      <c r="K30" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="L30"/>
-    </row>
-    <row r="31" spans="1:12" ht="27" x14ac:dyDescent="0.25">
+      <c r="L30" s="31"/>
+    </row>
+    <row r="31" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>102</v>
+        <v>66</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D31" s="25" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="E31" s="18" t="s">
         <v>16</v>
       </c>
       <c r="F31" s="16">
-        <v>4925</v>
+        <v>990</v>
       </c>
       <c r="G31" s="15">
         <v>1</v>
@@ -2553,76 +2619,124 @@
         <v>500</v>
       </c>
       <c r="I31" s="17">
+        <v>1.34714</v>
+      </c>
+      <c r="J31" s="22">
+        <f t="shared" ref="J31:J75" si="1">SUM(I31*H31)</f>
+        <v>673.57</v>
+      </c>
+      <c r="K31" s="18"/>
+      <c r="L31"/>
+    </row>
+    <row r="32" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="B32" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="D32" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32" s="16">
+        <v>13969</v>
+      </c>
+      <c r="G32" s="15">
+        <v>1</v>
+      </c>
+      <c r="H32" s="40">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>500</v>
+      </c>
+      <c r="I32" s="17">
+        <v>0.21360000000000001</v>
+      </c>
+      <c r="J32" s="22">
+        <f>SUM(I32*H32)</f>
+        <v>106.80000000000001</v>
+      </c>
+      <c r="K32" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="L32" s="18"/>
+    </row>
+    <row r="33" spans="1:12" ht="54" x14ac:dyDescent="0.25">
+      <c r="A33" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" s="25"/>
+      <c r="E33" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="F33" s="16"/>
+      <c r="G33" s="15">
+        <v>1</v>
+      </c>
+      <c r="H33" s="23">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>500</v>
+      </c>
+      <c r="I33" s="17">
+        <v>1.66</v>
+      </c>
+      <c r="J33" s="22">
+        <f t="shared" si="1"/>
+        <v>830</v>
+      </c>
+      <c r="K33" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="L33"/>
+    </row>
+    <row r="34" spans="1:12" ht="27" x14ac:dyDescent="0.25">
+      <c r="A34" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D34" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F34" s="16">
+        <v>4925</v>
+      </c>
+      <c r="G34" s="15">
+        <v>1</v>
+      </c>
+      <c r="H34" s="23">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>500</v>
+      </c>
+      <c r="I34" s="17">
         <v>0.83160000000000001</v>
       </c>
-      <c r="J31" s="22">
+      <c r="J34" s="22">
         <f t="shared" si="1"/>
         <v>415.8</v>
       </c>
-      <c r="K31" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="L31"/>
-    </row>
-    <row r="32" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="20"/>
-      <c r="B32" s="19"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="23">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="I32" s="17"/>
-      <c r="J32" s="22">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K32" s="18"/>
-      <c r="L32" s="18"/>
-    </row>
-    <row r="33" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="20"/>
-      <c r="B33" s="19"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="23">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="I33" s="17"/>
-      <c r="J33" s="22">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K33" s="18"/>
-      <c r="L33" s="18"/>
-    </row>
-    <row r="34" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="20"/>
-      <c r="B34" s="19"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="23">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="I34" s="17"/>
-      <c r="J34" s="22">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K34" s="18"/>
-      <c r="L34" s="18"/>
+      <c r="K34" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="L34"/>
     </row>
     <row r="35" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="20"/>
@@ -3398,7 +3512,7 @@
       </c>
       <c r="I73" s="17"/>
       <c r="J73" s="22">
-        <f t="shared" ref="J73:J136" si="2">SUM(I73*H73)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K73" s="18"/>
@@ -3418,7 +3532,7 @@
       </c>
       <c r="I74" s="17"/>
       <c r="J74" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K74" s="18"/>
@@ -3438,7 +3552,7 @@
       </c>
       <c r="I75" s="17"/>
       <c r="J75" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K75" s="18"/>
@@ -3458,7 +3572,7 @@
       </c>
       <c r="I76" s="17"/>
       <c r="J76" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="J76:J139" si="2">SUM(I76*H76)</f>
         <v>0</v>
       </c>
       <c r="K76" s="18"/>
@@ -4678,7 +4792,7 @@
       </c>
       <c r="I137" s="17"/>
       <c r="J137" s="22">
-        <f t="shared" ref="J137:J200" si="3">SUM(I137*H137)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K137" s="18"/>
@@ -4698,7 +4812,7 @@
       </c>
       <c r="I138" s="17"/>
       <c r="J138" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K138" s="18"/>
@@ -4718,7 +4832,7 @@
       </c>
       <c r="I139" s="17"/>
       <c r="J139" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K139" s="18"/>
@@ -4738,7 +4852,7 @@
       </c>
       <c r="I140" s="17"/>
       <c r="J140" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="J140:J203" si="3">SUM(I140*H140)</f>
         <v>0</v>
       </c>
       <c r="K140" s="18"/>
@@ -5958,7 +6072,7 @@
       </c>
       <c r="I201" s="17"/>
       <c r="J201" s="22">
-        <f t="shared" ref="J201:J203" si="4">SUM(I201*H201)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K201" s="18"/>
@@ -5978,7 +6092,7 @@
       </c>
       <c r="I202" s="17"/>
       <c r="J202" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K202" s="18"/>
@@ -5998,11 +6112,71 @@
       </c>
       <c r="I203" s="17"/>
       <c r="J203" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K203" s="18"/>
       <c r="L203" s="18"/>
+    </row>
+    <row r="204" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A204" s="20"/>
+      <c r="B204" s="19"/>
+      <c r="C204" s="25"/>
+      <c r="D204" s="25"/>
+      <c r="E204" s="18"/>
+      <c r="F204" s="16"/>
+      <c r="G204" s="15"/>
+      <c r="H204" s="23">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="I204" s="17"/>
+      <c r="J204" s="22">
+        <f t="shared" ref="J204:J206" si="4">SUM(I204*H204)</f>
+        <v>0</v>
+      </c>
+      <c r="K204" s="18"/>
+      <c r="L204" s="18"/>
+    </row>
+    <row r="205" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A205" s="20"/>
+      <c r="B205" s="19"/>
+      <c r="C205" s="25"/>
+      <c r="D205" s="25"/>
+      <c r="E205" s="18"/>
+      <c r="F205" s="16"/>
+      <c r="G205" s="15"/>
+      <c r="H205" s="23">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="I205" s="17"/>
+      <c r="J205" s="22">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K205" s="18"/>
+      <c r="L205" s="18"/>
+    </row>
+    <row r="206" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A206" s="20"/>
+      <c r="B206" s="19"/>
+      <c r="C206" s="25"/>
+      <c r="D206" s="25"/>
+      <c r="E206" s="18"/>
+      <c r="F206" s="16"/>
+      <c r="G206" s="15"/>
+      <c r="H206" s="23">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="I206" s="17"/>
+      <c r="J206" s="22">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K206" s="18"/>
+      <c r="L206" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -6011,29 +6185,11 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2:J2" r:id="rId1" display=" Projects and Stuff LLC - http://ww.projectsandstuff.com"/>
-    <hyperlink ref="B22" r:id="rId2"/>
-    <hyperlink ref="B7" r:id="rId3"/>
-    <hyperlink ref="B8" r:id="rId4"/>
-    <hyperlink ref="B9" r:id="rId5"/>
-    <hyperlink ref="B12" r:id="rId6"/>
-    <hyperlink ref="B13" r:id="rId7"/>
-    <hyperlink ref="B11" r:id="rId8"/>
-    <hyperlink ref="B23" r:id="rId9"/>
-    <hyperlink ref="B19" r:id="rId10"/>
-    <hyperlink ref="B21" r:id="rId11"/>
-    <hyperlink ref="B10" r:id="rId12"/>
-    <hyperlink ref="B14" r:id="rId13"/>
-    <hyperlink ref="B16" r:id="rId14"/>
-    <hyperlink ref="B31" r:id="rId15" display="ZX62-B-5PA(11)"/>
-    <hyperlink ref="B15" r:id="rId16"/>
-    <hyperlink ref="B17" r:id="rId17"/>
-    <hyperlink ref="B18" r:id="rId18"/>
-    <hyperlink ref="B27" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="47" orientation="landscape" r:id="rId20"/>
+  <pageSetup scale="47" orientation="landscape" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId21"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -6063,7 +6219,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="41" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="B1" s="41"/>
       <c r="C1" s="41"/>
@@ -6156,13 +6312,13 @@
     </row>
     <row r="6" spans="1:10" ht="54" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="D6" s="16"/>
       <c r="E6" s="15">
@@ -6180,13 +6336,13 @@
         <v>240</v>
       </c>
       <c r="I6" s="18" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="J6"/>
     </row>
     <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="B7" s="26"/>
       <c r="C7" s="18"/>
@@ -6206,11 +6362,11 @@
     </row>
     <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
       <c r="B8" s="26"/>
       <c r="C8" s="18" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="15">

</xml_diff>

<commit_message>
Began placing components onto board
</commit_message>
<xml_diff>
--- a/Notes/Chameleon BOM.xlsx
+++ b/Notes/Chameleon BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="124">
   <si>
     <t>Mfg Part #</t>
   </si>
@@ -253,9 +253,6 @@
     <t>Cap for switch TL1105JAF160Q</t>
   </si>
   <si>
-    <t>IC Microcontroller ATXMEGA16A4U</t>
-  </si>
-  <si>
     <t>GOOD</t>
   </si>
   <si>
@@ -389,6 +386,12 @@
   </si>
   <si>
     <t>LS L29K-G1J2-1-Z</t>
+  </si>
+  <si>
+    <t>IC Microcontroller</t>
+  </si>
+  <si>
+    <t>ATXMEGA16A4U</t>
   </si>
 </sst>
 </file>
@@ -1562,7 +1565,7 @@
   <dimension ref="A1:L206"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1710,16 +1713,16 @@
     </row>
     <row r="7" spans="1:12" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>25</v>
@@ -1742,7 +1745,7 @@
         <v>18.645</v>
       </c>
       <c r="K7" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L7"/>
     </row>
@@ -1751,13 +1754,13 @@
         <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E8" s="18" t="s">
         <v>25</v>
@@ -1780,22 +1783,22 @@
         <v>6.18</v>
       </c>
       <c r="K8" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L8"/>
     </row>
     <row r="9" spans="1:12" ht="27" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E9" s="18" t="s">
         <v>25</v>
@@ -1824,16 +1827,16 @@
     </row>
     <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" t="s">
         <v>92</v>
       </c>
-      <c r="B10" t="s">
-        <v>93</v>
-      </c>
       <c r="C10" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E10" s="18" t="s">
         <v>16</v>
@@ -1865,13 +1868,13 @@
         <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C11" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E11" s="18" t="s">
         <v>16</v>
@@ -1900,16 +1903,16 @@
     </row>
     <row r="12" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B12" s="39" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E12" s="18" t="s">
         <v>16</v>
@@ -1932,22 +1935,22 @@
         <v>4.3499999999999996</v>
       </c>
       <c r="K12" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L12" s="18"/>
     </row>
     <row r="13" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E13" s="18" t="s">
         <v>25</v>
@@ -1976,16 +1979,16 @@
     </row>
     <row r="14" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B14" s="39" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E14" s="18" t="s">
         <v>25</v>
@@ -2008,22 +2011,22 @@
         <v>1.3699999999999999</v>
       </c>
       <c r="K14" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L14" s="18"/>
     </row>
     <row r="15" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E15" s="18" t="s">
         <v>25</v>
@@ -2046,22 +2049,22 @@
         <v>6.03</v>
       </c>
       <c r="K15" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L15"/>
     </row>
     <row r="16" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E16" s="18" t="s">
         <v>25</v>
@@ -2090,16 +2093,16 @@
     </row>
     <row r="17" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B17" s="39" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E17" s="18" t="s">
         <v>25</v>
@@ -2122,22 +2125,22 @@
         <v>1.03</v>
       </c>
       <c r="K17" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L17" s="18"/>
     </row>
     <row r="18" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B18" s="39" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C18" s="25" t="s">
         <v>37</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E18" s="18" t="s">
         <v>25</v>
@@ -2160,7 +2163,7 @@
         <v>42.63</v>
       </c>
       <c r="K18" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L18" s="18"/>
     </row>
@@ -2175,7 +2178,7 @@
         <v>37</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E19" s="18" t="s">
         <v>25</v>
@@ -2198,22 +2201,22 @@
         <v>42.63</v>
       </c>
       <c r="K19" s="18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L19" s="18"/>
     </row>
     <row r="20" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="B20" s="39" t="s">
-        <v>86</v>
-      </c>
       <c r="C20" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E20" s="18" t="s">
         <v>16</v>
@@ -2236,7 +2239,7 @@
         <v>22.77</v>
       </c>
       <c r="K20" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L20" s="18"/>
     </row>
@@ -2249,7 +2252,7 @@
         <v>45</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E21" s="18"/>
       <c r="F21" s="16"/>
@@ -2272,17 +2275,17 @@
     </row>
     <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B22" s="39"/>
       <c r="C22" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="E22" s="18" t="s">
         <v>80</v>
-      </c>
-      <c r="D22" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="E22" s="18" t="s">
-        <v>81</v>
       </c>
       <c r="F22" s="16"/>
       <c r="G22" s="15">
@@ -2300,7 +2303,7 @@
         <v>75</v>
       </c>
       <c r="K22" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L22" s="18"/>
     </row>
@@ -2309,13 +2312,13 @@
         <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E23" s="18" t="s">
         <v>25</v>
@@ -2353,7 +2356,7 @@
         <v>17</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E24" s="18" t="s">
         <v>16</v>
@@ -2488,12 +2491,14 @@
     </row>
     <row r="28" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="B28" s="26"/>
+        <v>122</v>
+      </c>
+      <c r="B28" s="26" t="s">
+        <v>123</v>
+      </c>
       <c r="C28" s="25"/>
       <c r="D28" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E28" s="18" t="s">
         <v>16</v>
@@ -2527,7 +2532,7 @@
         <v>61</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E29" s="18" t="s">
         <v>16</v>
@@ -2550,7 +2555,7 @@
         <v>206</v>
       </c>
       <c r="K29" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L29"/>
     </row>
@@ -2565,7 +2570,7 @@
         <v>59</v>
       </c>
       <c r="D30" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E30" s="31" t="s">
         <v>16</v>
@@ -2588,7 +2593,7 @@
         <v>66.3</v>
       </c>
       <c r="K30" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L30" s="31"/>
     </row>
@@ -2603,7 +2608,7 @@
         <v>67</v>
       </c>
       <c r="D31" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E31" s="18" t="s">
         <v>16</v>
@@ -2630,16 +2635,16 @@
     </row>
     <row r="32" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B32" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="B32" s="39" t="s">
-        <v>84</v>
-      </c>
       <c r="C32" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D32" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E32" s="18" t="s">
         <v>16</v>
@@ -2662,7 +2667,7 @@
         <v>106.80000000000001</v>
       </c>
       <c r="K32" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L32" s="18"/>
     </row>
@@ -2711,7 +2716,7 @@
         <v>40</v>
       </c>
       <c r="D34" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E34" s="18" t="s">
         <v>16</v>

</xml_diff>